<commit_message>
Updated CORDEX_register; deleted coordination issues
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -23,7 +23,7 @@
     <definedName name="ANT44tier1">#REF!</definedName>
     <definedName name="ARC_44">#REF!</definedName>
     <definedName name="ARC44tier1">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$AW$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$57</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
     <definedName name="EUR_11" localSheetId="0">ReadMe!#REF!</definedName>
     <definedName name="EUR_11">AllEntries!#REF!</definedName>
@@ -524,9 +524,6 @@
     <t>name and/or e-mail of a contact for the ESGF publication; this need not be the contact included in the archive files as NetCDF attribute</t>
   </si>
   <si>
-    <t xml:space="preserve">UNSW </t>
-  </si>
-  <si>
     <t xml:space="preserve">unrestricted </t>
   </si>
   <si>
@@ -609,6 +606,9 @@
   </si>
   <si>
     <t>non-commercial</t>
+  </si>
+  <si>
+    <t>UNSW</t>
   </si>
 </sst>
 </file>
@@ -1125,6 +1125,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1134,38 +1161,11 @@
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1175,7 +1175,17 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1722,20 +1732,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1743,7 +1753,7 @@
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <f>AllEntries!A1</f>
-        <v>42099</v>
+        <v>42101</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1761,20 +1771,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1797,127 +1807,127 @@
       <c r="A5" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="67"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="65" t="s">
         <v>147</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="66"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="66"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="66"/>
     </row>
     <row r="10" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="66"/>
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="72"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="69"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="68" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
+      <c r="A13" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="59"/>
@@ -1932,32 +1942,32 @@
       <c r="J14" s="59"/>
     </row>
     <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="69" t="s">
-        <v>162</v>
-      </c>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
+      <c r="A15" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1966,10 +1976,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:CI58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="50" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2018,7 +2031,7 @@
   <sheetData>
     <row r="1" spans="1:87" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4">
-        <v>42099</v>
+        <v>42101</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2127,13 +2140,13 @@
         <v>41</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY3" s="23"/>
       <c r="BZ3" s="23"/>
@@ -2168,7 +2181,7 @@
         <v>140</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY4" s="23"/>
       <c r="BZ4" s="23"/>
@@ -2238,7 +2251,7 @@
         <v>142</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY6" s="23"/>
       <c r="BZ6" s="23"/>
@@ -2344,7 +2357,7 @@
         <v>145</v>
       </c>
       <c r="G9" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY9" s="23"/>
       <c r="BZ9" s="23"/>
@@ -2379,7 +2392,7 @@
         <v>136</v>
       </c>
       <c r="G10" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY10" s="23"/>
       <c r="BZ10" s="23"/>
@@ -2414,7 +2427,7 @@
         <v>145</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY11" s="23"/>
       <c r="BZ11" s="23"/>
@@ -2449,7 +2462,7 @@
         <v>145</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY12" s="23"/>
       <c r="BZ12" s="23"/>
@@ -2484,7 +2497,7 @@
         <v>145</v>
       </c>
       <c r="G13" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY13" s="23"/>
       <c r="BZ13" s="23"/>
@@ -2519,7 +2532,7 @@
         <v>145</v>
       </c>
       <c r="G14" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY14" s="23"/>
       <c r="BZ14" s="23"/>
@@ -2554,7 +2567,7 @@
         <v>145</v>
       </c>
       <c r="G15" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY15" s="23"/>
       <c r="BZ15" s="23"/>
@@ -2624,7 +2637,7 @@
         <v>145</v>
       </c>
       <c r="G17" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY17" s="23"/>
       <c r="BZ17" s="23"/>
@@ -2723,7 +2736,7 @@
         <v>32</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>135</v>
@@ -2799,7 +2812,7 @@
         <v>145</v>
       </c>
       <c r="G22" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY22" s="23"/>
       <c r="BZ22" s="23"/>
@@ -3079,7 +3092,7 @@
         <v>145</v>
       </c>
       <c r="G30" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY30" s="23"/>
       <c r="BZ30" s="23"/>
@@ -3105,16 +3118,16 @@
         <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G31" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY31" s="23"/>
       <c r="BZ31" s="23"/>
@@ -3149,7 +3162,7 @@
         <v>145</v>
       </c>
       <c r="G32" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY32" s="23"/>
       <c r="BZ32" s="23"/>
@@ -3219,7 +3232,7 @@
         <v>145</v>
       </c>
       <c r="G34" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY34" s="23"/>
       <c r="BZ34" s="23"/>
@@ -3359,7 +3372,7 @@
         <v>145</v>
       </c>
       <c r="G38" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY38" s="23"/>
       <c r="BZ38" s="23"/>
@@ -3375,26 +3388,26 @@
     </row>
     <row r="39" spans="1:87" s="22" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C39" s="18" t="str">
         <f>CONCATENATE(B39,"-",A39)</f>
         <v>MGO-RRCM</v>
       </c>
-      <c r="D39" s="73" t="s">
-        <v>171</v>
-      </c>
-      <c r="E39" s="74" t="s">
-        <v>173</v>
+      <c r="D39" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="E39" s="62" t="s">
+        <v>172</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G39" s="44" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
       <c r="BY39" s="23"/>
       <c r="BZ39" s="23"/>
@@ -3420,16 +3433,16 @@
         <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F40" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G40" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY40" s="23"/>
       <c r="BZ40" s="23"/>
@@ -3455,16 +3468,16 @@
         <v>UM-WRF331</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G41" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY41" s="23"/>
       <c r="BZ41" s="23"/>
@@ -3490,13 +3503,13 @@
         <v>BCCR-WRF331</v>
       </c>
       <c r="D42" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="21" t="s">
         <v>156</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="F42" s="21" t="s">
-        <v>157</v>
       </c>
       <c r="G42" s="44" t="s">
         <v>88</v>
@@ -3525,16 +3538,16 @@
         <v>MIUB-WRF331A</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G43" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY43" s="23"/>
       <c r="BZ43" s="23"/>
@@ -3560,10 +3573,10 @@
         <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F44" s="21" t="s">
         <v>145</v>
@@ -3595,16 +3608,16 @@
         <v>AUTH-Met-WRF331A</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F45" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G45" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY45" s="23"/>
       <c r="BZ45" s="23"/>
@@ -3630,13 +3643,13 @@
         <v>BCCR-WRF331C</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G46" s="44" t="s">
         <v>88</v>
@@ -3665,16 +3678,16 @@
         <v>IDL-WRF331D</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F47" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G47" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY47" s="23"/>
       <c r="BZ47" s="23"/>
@@ -3703,13 +3716,13 @@
         <v>105</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F48" s="20" t="s">
         <v>137</v>
       </c>
       <c r="G48" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY48" s="23"/>
       <c r="BZ48" s="23"/>
@@ -3735,16 +3748,16 @@
         <v>UCAN-WRF331G</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F49" s="20" t="s">
         <v>140</v>
       </c>
       <c r="G49" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY49" s="23"/>
       <c r="BZ49" s="23"/>
@@ -3779,7 +3792,7 @@
         <v>145</v>
       </c>
       <c r="G50" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY50" s="23"/>
       <c r="BZ50" s="23"/>
@@ -3805,16 +3818,16 @@
         <v>UCAN-WRF350I</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F51" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G51" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BY51" s="23"/>
       <c r="BZ51" s="23"/>
@@ -3830,26 +3843,26 @@
     </row>
     <row r="52" spans="1:87" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="C52" s="18" t="str">
         <f t="shared" ref="C52" si="2">CONCATENATE(B52,"-",A52)</f>
-        <v>UNSW -WRF360J</v>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D52" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E52" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="E52" s="58" t="s">
+      <c r="F52" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="F52" s="21" t="s">
-        <v>154</v>
-      </c>
       <c r="G52" s="44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BY52" s="23"/>
       <c r="BZ52" s="23"/>
@@ -3865,26 +3878,26 @@
     </row>
     <row r="53" spans="1:87" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="C53" s="18" t="str">
         <f>CONCATENATE(B53,"-",A53)</f>
-        <v>UNSW -WRF360K</v>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D53" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E53" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="E53" s="58" t="s">
+      <c r="F53" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="F53" s="21" t="s">
-        <v>154</v>
-      </c>
       <c r="G53" s="44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BY53" s="23"/>
       <c r="BZ53" s="23"/>
@@ -3900,26 +3913,26 @@
     </row>
     <row r="54" spans="1:87" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="C54" s="18" t="str">
         <f t="shared" ref="C54" si="3">CONCATENATE(B54,"-",A54)</f>
-        <v>UNSW -WRF360L</v>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D54" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="E54" s="58" t="s">
+      <c r="F54" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="F54" s="21" t="s">
-        <v>154</v>
-      </c>
       <c r="G54" s="44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BY54" s="23"/>
       <c r="BZ54" s="23"/>
@@ -3935,26 +3948,26 @@
     </row>
     <row r="55" spans="1:87" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C55" s="18" t="str">
         <f>CONCATENATE(B55,"-",A55)</f>
         <v>MU-WRF360M</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F55" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G55" s="44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BY55" s="23"/>
       <c r="BZ55" s="23"/>
@@ -3970,7 +3983,7 @@
     </row>
     <row r="56" spans="1:87" s="22" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B56" s="31" t="s">
         <v>19</v>
@@ -3980,13 +3993,13 @@
         <v>BCCR-WRF361</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G56" s="44" t="s">
         <v>88</v>
@@ -4024,7 +4037,7 @@
         <v>145</v>
       </c>
       <c r="G57" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="BY57" s="23"/>
       <c r="BZ57" s="23"/>
@@ -4060,124 +4073,129 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G33:G37 E32:E38 A22:A38 A43:C51 F44:G44 A57:C58 B55:C55 E57:G58 E55:G55 B3:C39 A40:C41 F40:F41 F43 E46:G46 F45 E50:G50 F47:F48 F51 F49:G49">
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A20 F38:F39 G31 E3:G30">
-    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:F37">
-    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:G54 B54:C54">
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53:G53 B53:C53">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:G52 A52:C52">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:C42 E42:G42">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:C56 E56:G56">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E39)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G38:G41">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="G38 G40:G41">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:G48">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40:E41">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43:E45">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:E49">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E51)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" display="mailto:John.Scinocca@ec.gc.ca"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="83" fitToWidth="7" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added information lost in the conversion process
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="825" windowWidth="16605" windowHeight="8610" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="885" windowWidth="16605" windowHeight="8550" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AU$1</definedName>
     <definedName name="Print_Area" localSheetId="0">ReadMe!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$59</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="201">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -58,18 +58,12 @@
     <t>ALADIN52</t>
   </si>
   <si>
-    <t>RM3</t>
-  </si>
-  <si>
     <t>CanRCM4</t>
   </si>
   <si>
     <t>CCAM</t>
   </si>
   <si>
-    <t>GFDL</t>
-  </si>
-  <si>
     <t>UQAM</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t>CRP-GL</t>
   </si>
   <si>
-    <t>GISS</t>
-  </si>
-  <si>
     <t>ICTP</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
   </si>
   <si>
     <t>MOHC</t>
-  </si>
-  <si>
-    <t>KAUST</t>
   </si>
   <si>
     <t>NUIM</t>
@@ -326,19 +314,7 @@
     <t>Jack.Katzfey@csiro.au</t>
   </si>
   <si>
-    <t>King Abdullah University, Thuwal, Saudi Arabien</t>
-  </si>
-  <si>
     <t>ALADIN53</t>
-  </si>
-  <si>
-    <t>NASA Goddard Institute for Space Studies (GISS)</t>
-  </si>
-  <si>
-    <t>Ruben Worrell                     Howard Spergel                   Crae Sosa               Kush Dave</t>
-  </si>
-  <si>
-    <t>georgiy.stenchikov@ kaust.edu.sa</t>
   </si>
   <si>
     <t>Kirsten.Warrach-Sagi@uni-hohenheim.de</t>
@@ -468,9 +444,6 @@
     <t>When changing the file, do not forget to change the date (in AllEntries!).</t>
   </si>
   <si>
-    <t>not confirmed</t>
-  </si>
-  <si>
     <t>WRF360K</t>
   </si>
   <si>
@@ -529,9 +502,6 @@
   </si>
   <si>
     <t>samuel.somot@meteo.fr</t>
-  </si>
-  <si>
-    <t>S. Legutkelegutke@dkrz.de</t>
   </si>
   <si>
     <t>sven.kotlarski@env.ethz.ch</t>
@@ -642,6 +612,51 @@
   </si>
   <si>
     <t>Royal Meteorological Institute of Belgium and Ghent University</t>
+  </si>
+  <si>
+    <t>University of Cantabria</t>
+  </si>
+  <si>
+    <t>Institut Pierre-Simon Laplace</t>
+  </si>
+  <si>
+    <t>Czech Hydro-Meteorological Institute</t>
+  </si>
+  <si>
+    <t>Jesus Fernandez jesus.fernandez@unican.es</t>
+  </si>
+  <si>
+    <t>S. Legutke legutke@dkrz.de</t>
+  </si>
+  <si>
+    <t>k.goergen@fz-juelich.de</t>
+  </si>
+  <si>
+    <t>Meteorological Institute, Bonn University</t>
+  </si>
+  <si>
+    <t>Public Research Centre - Gabriel Lippmann, Luxembourg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aristotle University of Thessaloniki, Department of Meteorology &amp; Climatology </t>
+  </si>
+  <si>
+    <t>Eleni Katragkou katragou@auth.gr</t>
+  </si>
+  <si>
+    <t>Aristotle University of Thessaloniki, Laboratory of Heat Transfer and Environmental Engeneering</t>
+  </si>
+  <si>
+    <t>Liana Kalognomou liana@aix.meng.auth.gr</t>
+  </si>
+  <si>
+    <t>Universidad de Murcia</t>
+  </si>
+  <si>
+    <t>Pedro Jimenez pedro.jimenezguerrero@um.es</t>
+  </si>
+  <si>
+    <t>Tomas Halenka tomas.halenka@mff.cuni.cz</t>
   </si>
 </sst>
 </file>
@@ -979,14 +994,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1126,9 +1142,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1179,74 +1192,15 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Hyperlink 2" xfId="4"/>
     <cellStyle name="Hyperlänk 2" xfId="3"/>
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1893,20 +1847,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
+      <c r="A1" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1932,25 +1886,25 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
+      <c r="A3" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1966,129 +1920,129 @@
     </row>
     <row r="5" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="65"/>
+        <v>114</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="64"/>
     </row>
     <row r="6" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="63"/>
+        <v>28</v>
+      </c>
+      <c r="B6" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="62"/>
     </row>
     <row r="7" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="63"/>
+        <v>27</v>
+      </c>
+      <c r="B7" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="62"/>
     </row>
     <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="62" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="63"/>
+        <v>94</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="63"/>
+        <v>72</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="68" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="63"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="62"/>
     </row>
     <row r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="69" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="70"/>
+        <v>96</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="69"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="66" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
+      <c r="A13" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
     </row>
     <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="51"/>
@@ -2103,18 +2057,18 @@
       <c r="J14" s="51"/>
     </row>
     <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
+      <c r="A15" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2140,15 +2094,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI62"/>
+  <dimension ref="A1:CI60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="58" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="57" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="5" width="22.7109375" customWidth="1"/>
@@ -2191,7 +2145,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:87" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54">
+      <c r="A1" s="53">
         <v>42159</v>
       </c>
       <c r="B1" s="5"/>
@@ -2254,25 +2208,25 @@
     </row>
     <row r="2" spans="1:87" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>102</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>110</v>
       </c>
       <c r="BY2" s="44"/>
       <c r="BZ2" s="44"/>
@@ -2291,23 +2245,23 @@
         <v>4</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f t="shared" ref="C3:C61" si="0">CONCATENATE(B3,"-",A3)</f>
+        <f t="shared" ref="C3:C59" si="0">CONCATENATE(B3,"-",A3)</f>
         <v>CHMI-ALADIN52</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="BY3" s="22"/>
       <c r="BZ3" s="22"/>
@@ -2326,23 +2280,23 @@
         <v>4</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" s="18" t="str">
         <f t="shared" si="0"/>
         <v>HMS-ALADIN52</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY4" s="22"/>
       <c r="BZ4" s="22"/>
@@ -2361,23 +2315,23 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CNRM-ALADIN52</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY5" s="22"/>
       <c r="BZ5" s="22"/>
@@ -2392,27 +2346,27 @@
       <c r="CI5" s="22"/>
     </row>
     <row r="6" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
-        <v>93</v>
+      <c r="A6" s="54" t="s">
+        <v>88</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CNRM-ALADIN53</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY6" s="22"/>
       <c r="BZ6" s="22"/>
@@ -2428,26 +2382,26 @@
     </row>
     <row r="7" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CNRM-ARPEGE52</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M7" s="26"/>
       <c r="BY7" s="22"/>
@@ -2464,26 +2418,26 @@
     </row>
     <row r="8" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CCCma-CanRCM4</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY8" s="22"/>
       <c r="BZ8" s="22"/>
@@ -2499,26 +2453,26 @@
     </row>
     <row r="9" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C9" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CSIRO-CCAM</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="BY9" s="22"/>
       <c r="BZ9" s="22"/>
@@ -2534,26 +2488,26 @@
     </row>
     <row r="10" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY10" s="22"/>
       <c r="BZ10" s="22"/>
@@ -2569,26 +2523,26 @@
     </row>
     <row r="11" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY11" s="22"/>
       <c r="BZ11" s="22"/>
@@ -2604,26 +2558,26 @@
     </row>
     <row r="12" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY12" s="22"/>
       <c r="BZ12" s="22"/>
@@ -2639,26 +2593,26 @@
     </row>
     <row r="13" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY13" s="22"/>
       <c r="BZ13" s="22"/>
@@ -2674,26 +2628,26 @@
     </row>
     <row r="14" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY14" s="22"/>
       <c r="BZ14" s="22"/>
@@ -2709,26 +2663,26 @@
     </row>
     <row r="15" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY15" s="22"/>
       <c r="BZ15" s="22"/>
@@ -2744,26 +2698,26 @@
     </row>
     <row r="16" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C16" s="18" t="str">
         <f t="shared" ref="C16" si="1">CONCATENATE(B16,"-",A16)</f>
         <v>OURANOS-CRCM5</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY16" s="22"/>
       <c r="BZ16" s="22"/>
@@ -2779,26 +2733,26 @@
     </row>
     <row r="17" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C17" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UQAM-CRCM5</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY17" s="22"/>
       <c r="BZ17" s="22"/>
@@ -2814,26 +2768,26 @@
     </row>
     <row r="18" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UNIBELGRADE-EBU1</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY18" s="22"/>
       <c r="BZ18" s="22"/>
@@ -2849,26 +2803,26 @@
     </row>
     <row r="19" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UNIBELGRADE-EBUPOM2c1</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY19" s="22"/>
       <c r="BZ19" s="22"/>
@@ -2883,27 +2837,27 @@
       <c r="CI19" s="22"/>
     </row>
     <row r="20" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>8</v>
+      <c r="A20" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C20" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KAUST-GFDL</v>
+        <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>150</v>
+        <v>69</v>
       </c>
       <c r="BY20" s="22"/>
       <c r="BZ20" s="22"/>
@@ -2919,26 +2873,26 @@
     </row>
     <row r="21" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MOHC-HadGEM3-RA</v>
+        <v>MOHC-HadRM3P</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>121</v>
+        <v>74</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY21" s="22"/>
       <c r="BZ21" s="22"/>
@@ -2954,26 +2908,26 @@
     </row>
     <row r="22" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>1</v>
       </c>
       <c r="C22" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MOHC-HadRM3P</v>
+        <v>DMI-HIRHAM5</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>38</v>
+        <v>175</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>120</v>
+        <v>145</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>181</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY22" s="22"/>
       <c r="BZ22" s="22"/>
@@ -2987,28 +2941,28 @@
       <c r="CH22" s="22"/>
       <c r="CI22" s="22"/>
     </row>
-    <row r="23" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C23" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DMI-HIRHAM5</v>
+        <v>AWI-HIRHAM5</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>154</v>
+        <v>77</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>191</v>
+        <v>113</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY23" s="22"/>
       <c r="BZ23" s="22"/>
@@ -3022,28 +2976,28 @@
       <c r="CH23" s="22"/>
       <c r="CI23" s="22"/>
     </row>
-    <row r="24" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>40</v>
+    <row r="24" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C24" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AWI-HIRHAM5</v>
+        <v>UCLM-PROMES</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="BY24" s="22"/>
       <c r="BZ24" s="22"/>
@@ -3057,28 +3011,28 @@
       <c r="CH24" s="22"/>
       <c r="CI24" s="22"/>
     </row>
-    <row r="25" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>12</v>
+    <row r="25" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="C25" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCLM-PROMES</v>
+        <v>KNMI-RACMO21P</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="E25" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" s="37" t="s">
         <v>69</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25" s="37" t="s">
-        <v>150</v>
       </c>
       <c r="BY25" s="22"/>
       <c r="BZ25" s="22"/>
@@ -3094,26 +3048,26 @@
     </row>
     <row r="26" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>KNMI-RACMO22E</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>KNMI-RACMO21P</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>46</v>
-      </c>
       <c r="E26" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G26" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY26" s="22"/>
       <c r="BZ26" s="22"/>
@@ -3129,26 +3083,26 @@
     </row>
     <row r="27" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C27" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO22E</v>
+        <v>KNMI-RACMO22T</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY27" s="22"/>
       <c r="BZ27" s="22"/>
@@ -3163,27 +3117,27 @@
       <c r="CI27" s="22"/>
     </row>
     <row r="28" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>25</v>
+      <c r="A28" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C28" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO22T</v>
+        <v>SMHI-RCA4</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>67</v>
+        <v>26</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G28" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY28" s="22"/>
       <c r="BZ28" s="22"/>
@@ -3199,26 +3153,26 @@
     </row>
     <row r="29" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C29" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCA4</v>
+        <v>SMHI-RCA4-SN</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>30</v>
+        <v>166</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>115</v>
+        <v>64</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>106</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY29" s="22"/>
       <c r="BZ29" s="22"/>
@@ -3234,26 +3188,26 @@
     </row>
     <row r="30" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C30" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCA4-SN</v>
+        <v>SMHI-RCAO</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>114</v>
+        <v>64</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY30" s="22"/>
       <c r="BZ30" s="22"/>
@@ -3269,26 +3223,26 @@
     </row>
     <row r="31" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C31" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO</v>
+        <v>SMHI-RCAO-SN</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY31" s="22"/>
       <c r="BZ31" s="22"/>
@@ -3302,28 +3256,28 @@
       <c r="CH31" s="22"/>
       <c r="CI31" s="22"/>
     </row>
-    <row r="32" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="C32" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO-SN</v>
+        <v>IITM-RegCM4-1</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="BY32" s="22"/>
       <c r="BZ32" s="22"/>
@@ -3339,26 +3293,26 @@
     </row>
     <row r="33" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="C33" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>IITM-RegCM4-1</v>
+        <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G33" s="37" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="BY33" s="22"/>
       <c r="BZ33" s="22"/>
@@ -3372,28 +3326,28 @@
       <c r="CH33" s="22"/>
       <c r="CI33" s="22"/>
     </row>
-    <row r="34" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C34" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CUNI-RegCM4-2</v>
+        <v>DHMZ-RegCM4-2</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="BY34" s="22"/>
       <c r="BZ34" s="22"/>
@@ -3409,26 +3363,26 @@
     </row>
     <row r="35" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C35" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DHMZ-RegCM4-2</v>
+        <v>ICTP-RegCM4-3</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>174</v>
+        <v>79</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="BY35" s="22"/>
       <c r="BZ35" s="22"/>
@@ -3442,28 +3396,28 @@
       <c r="CH35" s="22"/>
       <c r="CI35" s="22"/>
     </row>
-    <row r="36" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="C36" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ICTP-RegCM4-3</v>
+        <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="BY36" s="22"/>
       <c r="BZ36" s="22"/>
@@ -3479,26 +3433,26 @@
     </row>
     <row r="37" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="C37" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ENEA-RegCM4-3</v>
+        <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="BY37" s="22"/>
       <c r="BZ37" s="22"/>
@@ -3514,26 +3468,26 @@
     </row>
     <row r="38" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C38" s="18" t="str">
         <f t="shared" si="0"/>
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>121</v>
+        <v>66</v>
+      </c>
+      <c r="F38" s="28" t="s">
+        <v>105</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY38" s="22"/>
       <c r="BZ38" s="22"/>
@@ -3549,26 +3503,26 @@
     </row>
     <row r="39" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C39" s="18" t="str">
         <f t="shared" si="0"/>
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F39" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="20" t="s">
         <v>113</v>
       </c>
       <c r="G39" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY39" s="22"/>
       <c r="BZ39" s="22"/>
@@ -3582,28 +3536,28 @@
       <c r="CH39" s="22"/>
       <c r="CI39" s="22"/>
     </row>
-    <row r="40" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>49</v>
+        <v>183</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>48</v>
+        <v>184</v>
       </c>
       <c r="C40" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MPI-CSC-REMO2009</v>
+        <v>Alaro0-RMIB-Ugent</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>70</v>
+        <v>185</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G40" s="37" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="BY40" s="22"/>
       <c r="BZ40" s="22"/>
@@ -3617,28 +3571,28 @@
       <c r="CH40" s="22"/>
       <c r="CI40" s="22"/>
     </row>
-    <row r="41" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>14</v>
+    <row r="41" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>140</v>
       </c>
       <c r="C41" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>GISS-RM3</v>
+        <f>CONCATENATE(B41,"-",A41)</f>
+        <v>MGO-RRCM</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G41" s="37" t="s">
-        <v>150</v>
+        <v>69</v>
       </c>
       <c r="BY41" s="22"/>
       <c r="BZ41" s="22"/>
@@ -3652,28 +3606,28 @@
       <c r="CH41" s="22"/>
       <c r="CI41" s="22"/>
     </row>
-    <row r="42" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>193</v>
+        <v>58</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>194</v>
+        <v>57</v>
       </c>
       <c r="C42" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>Alaro0-RMIB-Ugent</v>
+        <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>195</v>
+        <v>197</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>196</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="BY42" s="22"/>
       <c r="BZ42" s="22"/>
@@ -3688,27 +3642,27 @@
       <c r="CI42" s="22"/>
     </row>
     <row r="43" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="B43" s="27" t="s">
-        <v>149</v>
+      <c r="A43" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="C43" s="18" t="str">
-        <f>CONCATENATE(B43,"-",A43)</f>
-        <v>MGO-RRCM</v>
+        <f t="shared" si="0"/>
+        <v>UM-WRF331</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E43" s="53" t="s">
-        <v>148</v>
+        <v>199</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>198</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G43" s="37" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="BY43" s="22"/>
       <c r="BZ43" s="22"/>
@@ -3722,28 +3676,28 @@
       <c r="CH43" s="22"/>
       <c r="CI43" s="22"/>
     </row>
-    <row r="44" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>61</v>
+    <row r="44" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C44" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>AUTH-LHTEE-WRF321B</v>
+        <f t="shared" ref="C44" si="2">CONCATENATE(B44,"-",A44)</f>
+        <v>BCCR-WRF331</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>150</v>
+        <v>123</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G44" s="37" t="s">
-        <v>150</v>
+        <v>69</v>
       </c>
       <c r="BY44" s="22"/>
       <c r="BZ44" s="22"/>
@@ -3757,28 +3711,28 @@
       <c r="CH44" s="22"/>
       <c r="CI44" s="22"/>
     </row>
-    <row r="45" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>10</v>
+    <row r="45" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>55</v>
       </c>
       <c r="C45" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UM-WRF331</v>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>150</v>
+        <v>191</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>192</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G45" s="37" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="BY45" s="22"/>
       <c r="BZ45" s="22"/>
@@ -3793,27 +3747,27 @@
       <c r="CI45" s="22"/>
     </row>
     <row r="46" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>19</v>
+      <c r="A46" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="C46" s="18" t="str">
-        <f t="shared" ref="C46" si="2">CONCATENATE(B46,"-",A46)</f>
-        <v>BCCR-WRF331</v>
+        <f t="shared" si="0"/>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>131</v>
+        <v>191</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="G46" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY46" s="22"/>
       <c r="BZ46" s="22"/>
@@ -3827,28 +3781,28 @@
       <c r="CH46" s="22"/>
       <c r="CI46" s="22"/>
     </row>
-    <row r="47" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>59</v>
+    <row r="47" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="C47" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MIUB-WRF331A</v>
+        <v>AUTH-Met-WRF331A</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>150</v>
+        <v>195</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>194</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G47" s="37" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="BY47" s="22"/>
       <c r="BZ47" s="22"/>
@@ -3862,28 +3816,28 @@
       <c r="CH47" s="22"/>
       <c r="CI47" s="22"/>
     </row>
-    <row r="48" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>13</v>
+    <row r="48" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C48" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CRP-GL-WRF331A</v>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>150</v>
+        <v>123</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="G48" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="BY48" s="22"/>
       <c r="BZ48" s="22"/>
@@ -3898,27 +3852,27 @@
       <c r="CI48" s="22"/>
     </row>
     <row r="49" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>60</v>
+      <c r="A49" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="C49" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AUTH-Met-WRF331A</v>
+        <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="F49" s="20" t="s">
-        <v>121</v>
+        <v>187</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="G49" s="37" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="BY49" s="22"/>
       <c r="BZ49" s="22"/>
@@ -3933,27 +3887,27 @@
       <c r="CI49" s="22"/>
     </row>
     <row r="50" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="29" t="s">
-        <v>19</v>
+      <c r="B50" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="C50" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>BCCR-WRF331C</v>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="F50" s="20" t="s">
-        <v>135</v>
+        <v>189</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="G50" s="37" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="BY50" s="22"/>
       <c r="BZ50" s="22"/>
@@ -3967,28 +3921,28 @@
       <c r="CH50" s="22"/>
       <c r="CI50" s="22"/>
     </row>
-    <row r="51" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>65</v>
+    <row r="51" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C51" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>IPSL-INERIS-WRF331F</v>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="F51" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F51" s="20" t="s">
         <v>113</v>
       </c>
       <c r="G51" s="37" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="BY51" s="22"/>
       <c r="BZ51" s="22"/>
@@ -4002,28 +3956,28 @@
       <c r="CH51" s="22"/>
       <c r="CI51" s="22"/>
     </row>
-    <row r="52" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>57</v>
+        <v>178</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C52" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF331G</v>
+        <f>CONCATENATE(B52,"-",A52)</f>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>116</v>
+        <v>180</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="G52" s="37" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="BY52" s="22"/>
       <c r="BZ52" s="22"/>
@@ -4039,26 +3993,26 @@
     </row>
     <row r="53" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C53" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>NUIM-WRF341E</v>
+        <v>UCAN-WRF350I</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G53" s="37" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="BZ53" s="22"/>
@@ -4072,28 +4026,28 @@
       <c r="CH53" s="22"/>
       <c r="CI53" s="22"/>
     </row>
-    <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>20</v>
+    <row r="54" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="C54" s="18" t="str">
-        <f>CONCATENATE(B54,"-",A54)</f>
-        <v>IDL-WRF350D</v>
+        <f t="shared" ref="C54" si="3">CONCATENATE(B54,"-",A54)</f>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>190</v>
+        <v>119</v>
+      </c>
+      <c r="E54" s="50" t="s">
+        <v>120</v>
       </c>
       <c r="F54" s="20" t="s">
         <v>121</v>
       </c>
       <c r="G54" s="37" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="BY54" s="22"/>
       <c r="BZ54" s="22"/>
@@ -4107,28 +4061,28 @@
       <c r="CH54" s="22"/>
       <c r="CI54" s="22"/>
     </row>
-    <row r="55" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="31" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="C55" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF350I</v>
+        <f>CONCATENATE(B55,"-",A55)</f>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>150</v>
+        <v>119</v>
+      </c>
+      <c r="E55" s="50" t="s">
+        <v>120</v>
       </c>
       <c r="F55" s="20" t="s">
         <v>121</v>
       </c>
       <c r="G55" s="37" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="BY55" s="22"/>
       <c r="BZ55" s="22"/>
@@ -4144,26 +4098,26 @@
     </row>
     <row r="56" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C56" s="18" t="str">
-        <f t="shared" ref="C56" si="3">CONCATENATE(B56,"-",A56)</f>
-        <v>UNSW-WRF360J</v>
+        <f t="shared" ref="C56" si="4">CONCATENATE(B56,"-",A56)</f>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E56" s="50" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G56" s="37" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="BY56" s="22"/>
       <c r="BZ56" s="22"/>
@@ -4177,28 +4131,28 @@
       <c r="CH56" s="22"/>
       <c r="CI56" s="22"/>
     </row>
-    <row r="57" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="C57" s="18" t="str">
         <f>CONCATENATE(B57,"-",A57)</f>
-        <v>UNSW-WRF360K</v>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="E57" s="50" t="s">
-        <v>128</v>
+        <v>135</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="G57" s="37" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="BY57" s="22"/>
       <c r="BZ57" s="22"/>
@@ -4212,28 +4166,28 @@
       <c r="CH57" s="22"/>
       <c r="CI57" s="22"/>
     </row>
-    <row r="58" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>153</v>
+    <row r="58" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C58" s="18" t="str">
-        <f t="shared" ref="C58" si="4">CONCATENATE(B58,"-",A58)</f>
-        <v>UNSW-WRF360L</v>
+        <f t="shared" ref="C58" si="5">CONCATENATE(B58,"-",A58)</f>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="E58" s="50" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G58" s="37" t="s">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="BY58" s="22"/>
       <c r="BZ58" s="22"/>
@@ -4247,28 +4201,28 @@
       <c r="CH58" s="22"/>
       <c r="CI58" s="22"/>
     </row>
-    <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
+    <row r="59" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>UHOH-WRF361H</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E59" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="F59" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G59" s="38" t="s">
         <v>142</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C59" s="18" t="str">
-        <f>CONCATENATE(B59,"-",A59)</f>
-        <v>MU-WRF360M</v>
-      </c>
-      <c r="D59" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G59" s="37" t="s">
-        <v>152</v>
       </c>
       <c r="BY59" s="22"/>
       <c r="BZ59" s="22"/>
@@ -4282,29 +4236,14 @@
       <c r="CH59" s="22"/>
       <c r="CI59" s="22"/>
     </row>
-    <row r="60" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="B60" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C60" s="18" t="str">
-        <f t="shared" ref="C60" si="5">CONCATENATE(B60,"-",A60)</f>
-        <v>BCCR-WRF361</v>
-      </c>
-      <c r="D60" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="G60" s="37" t="s">
-        <v>73</v>
-      </c>
+    <row r="60" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="56"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="46"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="48"/>
       <c r="BY60" s="22"/>
       <c r="BZ60" s="22"/>
       <c r="CA60" s="22"/>
@@ -4317,105 +4256,60 @@
       <c r="CH60" s="22"/>
       <c r="CI60" s="22"/>
     </row>
-    <row r="61" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C61" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>UHOH-WRF361H</v>
-      </c>
-      <c r="D61" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="E61" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="F61" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="G61" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="BY61" s="22"/>
-      <c r="BZ61" s="22"/>
-      <c r="CA61" s="22"/>
-      <c r="CB61" s="22"/>
-      <c r="CC61" s="22"/>
-      <c r="CD61" s="22"/>
-      <c r="CE61" s="22"/>
-      <c r="CF61" s="22"/>
-      <c r="CG61" s="22"/>
-      <c r="CH61" s="22"/>
-      <c r="CI61" s="22"/>
-    </row>
-    <row r="62" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="48"/>
-      <c r="BY62" s="22"/>
-      <c r="BZ62" s="22"/>
-      <c r="CA62" s="22"/>
-      <c r="CB62" s="22"/>
-      <c r="CC62" s="22"/>
-      <c r="CD62" s="22"/>
-      <c r="CE62" s="22"/>
-      <c r="CF62" s="22"/>
-      <c r="CG62" s="22"/>
-      <c r="CH62" s="22"/>
-      <c r="CI62" s="22"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="G36:G40 E35:E41 A25:A42 F48:G48 A61:C62 B59:C59 E61:G62 E59:G59 B3:C15 A44:C45 F44:F45 F47 F49 F55 B21:C43 C17 C20 A47:C55 E50:G53 F54:G54 E52:E55">
-    <cfRule type="containsText" dxfId="30" priority="29" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E34:E39 F46:G46 A59:C60 B57:C57 E59:G60 E57:G57 B3:C15 A42:C43 F45 F47 F53 C17 A45:C53 E48:G51 F52:G52 E50:E53 A17:A22 F17:G22 E19:E22 A24:A40 B20:C41 F40:F43 G35:G40">
+    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A15 F41:F43 G34 E3:G14 E24:G33 A17:A23 F17:G23 F15:G15">
-    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A3:A15 G33 E3:G14 E23:G32 F15:G15">
+    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="28" priority="31" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G35)))</formula>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G34)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:F40">
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",F34)))</formula>
+  <conditionalFormatting sqref="F33:F39">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",F33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58:G58 B58:C58">
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B58)))</formula>
+  <conditionalFormatting sqref="F56:G56 B56:C56">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F57:G57 B57:C57">
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B57)))</formula>
+  <conditionalFormatting sqref="F55:G55 B55:C55">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56:G56 A56:C56">
-    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A56)))</formula>
+  <conditionalFormatting sqref="F54:G54 A54:C54">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A46:C46 E46:G46">
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A46)))</formula>
+  <conditionalFormatting sqref="A44:C44 E44:G44">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A44)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A60:C60 E60:G60">
+  <conditionalFormatting sqref="A58:C58 E58:G58">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
     <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
@@ -4423,104 +4317,89 @@
       <formula>NOT(ISERROR(SEARCH("unrestricted",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
+  <conditionalFormatting sqref="E41">
     <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
+  <conditionalFormatting sqref="G42:G43">
     <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
+  <conditionalFormatting sqref="G45">
     <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G41:G42 G44:G45">
+  <conditionalFormatting sqref="G47">
     <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G53">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G55">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44:E45">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:E49">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B20">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="B17:B19">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E23">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Changes for CNRM and CHMI
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -33,7 +33,7 @@
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AU$1</definedName>
     <definedName name="Print_Area" localSheetId="0">ReadMe!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$61</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="204">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -272,9 +272,6 @@
     <t>Met Office Hadley Centre</t>
   </si>
   <si>
-    <t>Centre National de Recherches Meteorologiques</t>
-  </si>
-  <si>
     <t>Hungarian Meteorological Service</t>
   </si>
   <si>
@@ -376,9 +373,6 @@
   </si>
   <si>
     <t>"EUR-44 EUR-11"</t>
-  </si>
-  <si>
-    <t>"EUR-??"</t>
   </si>
   <si>
     <t>"ANT-44"</t>
@@ -617,9 +611,6 @@
     <t>Institut Pierre-Simon Laplace</t>
   </si>
   <si>
-    <t>Czech Hydro-Meteorological Institute</t>
-  </si>
-  <si>
     <t>Jesus Fernandez jesus.fernandez@unican.es</t>
   </si>
   <si>
@@ -660,6 +651,21 @@
   </si>
   <si>
     <t>WRF311NEMO</t>
+  </si>
+  <si>
+    <t>Czech Hydrometeorological Institute</t>
+  </si>
+  <si>
+    <t>RCSM4</t>
+  </si>
+  <si>
+    <t>Météo-France / Centre National de Recherches Météorologiques</t>
+  </si>
+  <si>
+    <t>"AFR-44" "MED-44"</t>
+  </si>
+  <si>
+    <t>"EUR-44" "EUR-11"</t>
   </si>
 </sst>
 </file>
@@ -1158,6 +1164,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1165,33 +1192,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1850,20 +1856,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
+      <c r="A1" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1889,25 +1895,25 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="67" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
+      <c r="A3" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1923,129 +1929,129 @@
     </row>
     <row r="5" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="68" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="64"/>
     </row>
     <row r="6" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
+      <c r="B6" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="62"/>
     </row>
     <row r="7" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="61"/>
+      <c r="B7" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="62"/>
     </row>
     <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
+        <v>92</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="61"/>
+      <c r="B9" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="61"/>
+        <v>93</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="62"/>
     </row>
     <row r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="64"/>
+        <v>94</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="69"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
+      <c r="A13" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
     </row>
     <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="51"/>
@@ -2060,32 +2066,32 @@
       <c r="J14" s="51"/>
     </row>
     <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
+      <c r="A15" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2097,10 +2103,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI61"/>
+  <dimension ref="A1:CI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,7 +2217,7 @@
     </row>
     <row r="2" spans="1:87" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="40" t="s">
         <v>28</v>
@@ -2220,16 +2226,16 @@
         <v>27</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="40" t="s">
         <v>71</v>
       </c>
       <c r="F2" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>100</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>101</v>
       </c>
       <c r="BY2" s="44"/>
       <c r="BZ2" s="44"/>
@@ -2245,23 +2251,23 @@
     </row>
     <row r="3" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f t="shared" ref="C3:C60" si="0">CONCATENATE(B3,"-",A3)</f>
-        <v>CHMI-ALADIN52</v>
+        <f t="shared" ref="C3:C61" si="0">CONCATENATE(B3,"-",A3)</f>
+        <v>CHMI-ALADIN53</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>140</v>
@@ -2293,13 +2299,13 @@
         <v>48</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY4" s="22"/>
       <c r="BZ4" s="22"/>
@@ -2313,7 +2319,7 @@
       <c r="CH4" s="22"/>
       <c r="CI4" s="22"/>
     </row>
-    <row r="5" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>4</v>
       </c>
@@ -2325,16 +2331,16 @@
         <v>CNRM-ALADIN52</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>74</v>
+        <v>201</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>112</v>
+        <v>202</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY5" s="22"/>
       <c r="BZ5" s="22"/>
@@ -2348,9 +2354,9 @@
       <c r="CH5" s="22"/>
       <c r="CI5" s="22"/>
     </row>
-    <row r="6" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>13</v>
@@ -2360,16 +2366,16 @@
         <v>CNRM-ALADIN53</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>74</v>
+        <v>145</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>201</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY6" s="22"/>
       <c r="BZ6" s="22"/>
@@ -2383,7 +2389,7 @@
       <c r="CH6" s="22"/>
       <c r="CI6" s="22"/>
     </row>
-    <row r="7" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>47</v>
       </c>
@@ -2395,13 +2401,13 @@
         <v>CNRM-ARPEGE52</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>74</v>
+        <v>144</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>201</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G7" s="37" t="s">
         <v>68</v>
@@ -2431,13 +2437,13 @@
         <v>CCCma-CanRCM4</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>69</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G8" s="37" t="s">
         <v>68</v>
@@ -2459,23 +2465,23 @@
         <v>6</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>CSIRO-CCAM</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>CSIRO-CCAM</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>85</v>
-      </c>
       <c r="F9" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BY9" s="22"/>
       <c r="BZ9" s="22"/>
@@ -2501,16 +2507,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY10" s="22"/>
       <c r="BZ10" s="22"/>
@@ -2536,16 +2542,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY11" s="22"/>
       <c r="BZ11" s="22"/>
@@ -2571,16 +2577,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY12" s="22"/>
       <c r="BZ12" s="22"/>
@@ -2606,16 +2612,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY13" s="22"/>
       <c r="BZ13" s="22"/>
@@ -2641,16 +2647,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY14" s="22"/>
       <c r="BZ14" s="22"/>
@@ -2676,16 +2682,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY15" s="22"/>
       <c r="BZ15" s="22"/>
@@ -2704,20 +2710,20 @@
         <v>30</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C16" s="18" t="str">
         <f t="shared" ref="C16" si="1">CONCATENATE(B16,"-",A16)</f>
         <v>OURANOS-CRCM5</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G16" s="37" t="s">
         <v>68</v>
@@ -2746,13 +2752,13 @@
         <v>UQAM-CRCM5</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>70</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G17" s="37" t="s">
         <v>68</v>
@@ -2771,26 +2777,26 @@
     </row>
     <row r="18" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UNIBELGRADE-EBU1</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UNIBELGRADE-EBU1</v>
-      </c>
-      <c r="D18" s="23" t="s">
+      <c r="F18" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="E18" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>172</v>
-      </c>
       <c r="G18" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY18" s="22"/>
       <c r="BZ18" s="22"/>
@@ -2806,26 +2812,26 @@
     </row>
     <row r="19" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B19" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>UNIBELGRADE-EBUPOM2c1</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="C19" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UNIBELGRADE-EBUPOM2c1</v>
-      </c>
-      <c r="D19" s="23" t="s">
+      <c r="E19" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>172</v>
-      </c>
       <c r="G19" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY19" s="22"/>
       <c r="BZ19" s="22"/>
@@ -2851,13 +2857,13 @@
         <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G20" s="37" t="s">
         <v>68</v>
@@ -2892,7 +2898,7 @@
         <v>73</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G21" s="37" t="s">
         <v>68</v>
@@ -2921,13 +2927,13 @@
         <v>DMI-HIRHAM5</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G22" s="37" t="s">
         <v>68</v>
@@ -2959,10 +2965,10 @@
         <v>35</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G23" s="37" t="s">
         <v>68</v>
@@ -2991,16 +2997,16 @@
         <v>UCLM-PROMES</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>64</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BY24" s="22"/>
       <c r="BZ24" s="22"/>
@@ -3032,7 +3038,7 @@
         <v>62</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G25" s="37" t="s">
         <v>68</v>
@@ -3067,7 +3073,7 @@
         <v>62</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G26" s="37" t="s">
         <v>68</v>
@@ -3102,7 +3108,7 @@
         <v>62</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G27" s="37" t="s">
         <v>68</v>
@@ -3137,7 +3143,7 @@
         <v>63</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G28" s="37" t="s">
         <v>68</v>
@@ -3166,13 +3172,13 @@
         <v>SMHI-RCA4-SN</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>63</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G29" s="37" t="s">
         <v>68</v>
@@ -3201,13 +3207,13 @@
         <v>SMHI-RCAO</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>63</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G30" s="37" t="s">
         <v>68</v>
@@ -3226,26 +3232,26 @@
     </row>
     <row r="31" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO-SN</v>
+        <v>CNRM-RCSM4</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>112</v>
+        <v>170</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY31" s="22"/>
       <c r="BZ31" s="22"/>
@@ -3259,28 +3265,28 @@
       <c r="CH31" s="22"/>
       <c r="CI31" s="22"/>
     </row>
-    <row r="32" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="C32" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>IITM-RegCM4-1</v>
+        <v>SMHI-RCAO-SN</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="BY32" s="22"/>
       <c r="BZ32" s="22"/>
@@ -3296,23 +3302,23 @@
     </row>
     <row r="33" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="C33" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CUNI-RegCM4-2</v>
+        <v>IITM-RegCM4-1</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>158</v>
+        <v>80</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G33" s="37" t="s">
         <v>140</v>
@@ -3334,23 +3340,23 @@
         <v>49</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C34" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DHMZ-RegCM4-2</v>
+        <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>72</v>
+        <v>156</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="BY34" s="22"/>
       <c r="BZ34" s="22"/>
@@ -3366,26 +3372,26 @@
     </row>
     <row r="35" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C35" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ICTP-RegCM4-3</v>
+        <v>DHMZ-RegCM4-2</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY35" s="22"/>
       <c r="BZ35" s="22"/>
@@ -3399,28 +3405,28 @@
       <c r="CH35" s="22"/>
       <c r="CI35" s="22"/>
     </row>
-    <row r="36" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="C36" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ENEA-RegCM4-3</v>
+        <v>ICTP-RegCM4-3</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>157</v>
+        <v>77</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="BY36" s="22"/>
       <c r="BZ36" s="22"/>
@@ -3436,26 +3442,26 @@
     </row>
     <row r="37" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C37" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MPI-CSC-REMO2009</v>
+        <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY37" s="22"/>
       <c r="BZ37" s="22"/>
@@ -3481,13 +3487,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F38" s="28" t="s">
-        <v>104</v>
+      <c r="F38" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="G38" s="37" t="s">
         <v>68</v>
@@ -3516,13 +3522,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="20" t="s">
-        <v>112</v>
+      <c r="F39" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="G39" s="37" t="s">
         <v>68</v>
@@ -3539,28 +3545,28 @@
       <c r="CH39" s="22"/>
       <c r="CI39" s="22"/>
     </row>
-    <row r="40" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
       <c r="C40" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>Alaro0-RMIB-Ugent</v>
+        <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>184</v>
+        <v>65</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G40" s="37" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="BY40" s="22"/>
       <c r="BZ40" s="22"/>
@@ -3574,28 +3580,28 @@
       <c r="CH40" s="22"/>
       <c r="CI40" s="22"/>
     </row>
-    <row r="41" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>139</v>
+    <row r="41" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>181</v>
       </c>
       <c r="C41" s="18" t="str">
-        <f>CONCATENATE(B41,"-",A41)</f>
-        <v>MGO-RRCM</v>
+        <f t="shared" si="0"/>
+        <v>Alaro0-RMIB-Ugent</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G41" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY41" s="22"/>
       <c r="BZ41" s="22"/>
@@ -3609,28 +3615,28 @@
       <c r="CH41" s="22"/>
       <c r="CI41" s="22"/>
     </row>
-    <row r="42" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>56</v>
+    <row r="42" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="C42" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>AUTH-LHTEE-WRF321B</v>
+        <f>CONCATENATE(B42,"-",A42)</f>
+        <v>MGO-RRCM</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>195</v>
+        <v>134</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY42" s="22"/>
       <c r="BZ42" s="22"/>
@@ -3644,28 +3650,28 @@
       <c r="CH42" s="22"/>
       <c r="CI42" s="22"/>
     </row>
-    <row r="43" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>60</v>
+    <row r="43" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="C43" s="18" t="str">
-        <f t="shared" ref="C43:C44" si="2">CONCATENATE(B43,"-",A43)</f>
-        <v>IPSL-INERIS-WRF311</v>
+        <f t="shared" si="0"/>
+        <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>172</v>
+        <v>193</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="G43" s="37" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="BY43" s="22"/>
       <c r="BZ43" s="22"/>
@@ -3681,26 +3687,26 @@
     </row>
     <row r="44" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B44" s="25" t="s">
         <v>60</v>
       </c>
       <c r="C44" s="18" t="str">
-        <f t="shared" si="2"/>
-        <v>IPSL-INERIS-WRF311NEMO</v>
+        <f t="shared" ref="C44:C45" si="2">CONCATENATE(B44,"-",A44)</f>
+        <v>IPSL-INERIS-WRF311</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G44" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY44" s="22"/>
       <c r="BZ44" s="22"/>
@@ -3714,25 +3720,25 @@
       <c r="CH44" s="22"/>
       <c r="CI44" s="22"/>
     </row>
-    <row r="45" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>8</v>
+    <row r="45" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>60</v>
       </c>
       <c r="C45" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UM-WRF331</v>
+        <f t="shared" si="2"/>
+        <v>IPSL-INERIS-WRF311NEMO</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>112</v>
+        <v>160</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="G45" s="37" t="s">
         <v>140</v>
@@ -3750,27 +3756,27 @@
       <c r="CI45" s="22"/>
     </row>
     <row r="46" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="29" t="s">
-        <v>16</v>
+      <c r="B46" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="C46" s="18" t="str">
-        <f t="shared" ref="C46" si="3">CONCATENATE(B46,"-",A46)</f>
-        <v>BCCR-WRF331</v>
+        <f t="shared" si="0"/>
+        <v>UM-WRF331</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>121</v>
+        <v>195</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>194</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G46" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY46" s="22"/>
       <c r="BZ46" s="22"/>
@@ -3786,26 +3792,26 @@
     </row>
     <row r="47" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C47" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>MIUB-WRF331A</v>
+        <f t="shared" ref="C47" si="3">CONCATENATE(B47,"-",A47)</f>
+        <v>BCCR-WRF331</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G47" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY47" s="22"/>
       <c r="BZ47" s="22"/>
@@ -3820,27 +3826,27 @@
       <c r="CI47" s="22"/>
     </row>
     <row r="48" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="25" t="s">
-        <v>11</v>
+      <c r="B48" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="C48" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CRP-GL-WRF331A</v>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G48" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY48" s="22"/>
       <c r="BZ48" s="22"/>
@@ -3854,28 +3860,28 @@
       <c r="CH48" s="22"/>
       <c r="CI48" s="22"/>
     </row>
-    <row r="49" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
+    <row r="49" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>55</v>
+      <c r="B49" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="C49" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AUTH-Met-WRF331A</v>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="E49" s="23" t="s">
-        <v>193</v>
+        <v>187</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>189</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G49" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY49" s="22"/>
       <c r="BZ49" s="22"/>
@@ -3889,28 +3895,28 @@
       <c r="CH49" s="22"/>
       <c r="CI49" s="22"/>
     </row>
-    <row r="50" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>16</v>
+    <row r="50" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C50" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>BCCR-WRF331C</v>
+        <v>AUTH-Met-WRF331A</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>121</v>
+        <v>191</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="G50" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY50" s="22"/>
       <c r="BZ50" s="22"/>
@@ -3925,27 +3931,27 @@
       <c r="CI50" s="22"/>
     </row>
     <row r="51" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>52</v>
+      <c r="A51" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C51" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCAN-WRF331G</v>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>107</v>
+        <v>120</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="G51" s="37" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="BY51" s="22"/>
       <c r="BZ51" s="22"/>
@@ -3960,27 +3966,27 @@
       <c r="CI51" s="22"/>
     </row>
     <row r="52" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="31" t="s">
-        <v>67</v>
+      <c r="A52" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C52" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>NUIM-WRF341E</v>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F52" s="20" t="s">
-        <v>112</v>
+        <v>183</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="G52" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY52" s="22"/>
       <c r="BZ52" s="22"/>
@@ -3995,27 +4001,27 @@
       <c r="CI52" s="22"/>
     </row>
     <row r="53" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>17</v>
+      <c r="A53" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C53" s="18" t="str">
-        <f>CONCATENATE(B53,"-",A53)</f>
-        <v>IDL-WRF350D</v>
+        <f t="shared" si="0"/>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>179</v>
+        <v>79</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G53" s="37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="BZ53" s="22"/>
@@ -4030,24 +4036,24 @@
       <c r="CI53" s="22"/>
     </row>
     <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>52</v>
+      <c r="A54" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C54" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF350I</v>
+        <f>CONCATENATE(B54,"-",A54)</f>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G54" s="37" t="s">
         <v>140</v>
@@ -4064,28 +4070,28 @@
       <c r="CH54" s="22"/>
       <c r="CI54" s="22"/>
     </row>
-    <row r="55" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>143</v>
+        <v>52</v>
       </c>
       <c r="C55" s="18" t="str">
-        <f t="shared" ref="C55" si="4">CONCATENATE(B55,"-",A55)</f>
-        <v>UNSW-WRF360J</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF350I</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="E55" s="50" t="s">
-        <v>119</v>
+        <v>185</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>183</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G55" s="37" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="BY55" s="22"/>
       <c r="BZ55" s="22"/>
@@ -4101,26 +4107,26 @@
     </row>
     <row r="56" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C56" s="18" t="str">
-        <f>CONCATENATE(B56,"-",A56)</f>
-        <v>UNSW-WRF360K</v>
+        <f t="shared" ref="C56" si="4">CONCATENATE(B56,"-",A56)</f>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D56" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E56" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="F56" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>120</v>
-      </c>
       <c r="G56" s="37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="BY56" s="22"/>
       <c r="BZ56" s="22"/>
@@ -4136,26 +4142,26 @@
     </row>
     <row r="57" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="31" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C57" s="18" t="str">
-        <f t="shared" ref="C57" si="5">CONCATENATE(B57,"-",A57)</f>
-        <v>UNSW-WRF360L</v>
+        <f>CONCATENATE(B57,"-",A57)</f>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D57" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="F57" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E57" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>120</v>
-      </c>
       <c r="G57" s="37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="BY57" s="22"/>
       <c r="BZ57" s="22"/>
@@ -4169,28 +4175,28 @@
       <c r="CH57" s="22"/>
       <c r="CI57" s="22"/>
     </row>
-    <row r="58" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C58" s="18" t="str">
-        <f>CONCATENATE(B58,"-",A58)</f>
-        <v>MU-WRF360M</v>
+        <f t="shared" ref="C58" si="5">CONCATENATE(B58,"-",A58)</f>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>133</v>
+        <v>116</v>
+      </c>
+      <c r="E58" s="50" t="s">
+        <v>117</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G58" s="37" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="BY58" s="22"/>
       <c r="BZ58" s="22"/>
@@ -4204,28 +4210,28 @@
       <c r="CH58" s="22"/>
       <c r="CI58" s="22"/>
     </row>
-    <row r="59" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" s="29" t="s">
-        <v>16</v>
+    <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="C59" s="18" t="str">
-        <f t="shared" ref="C59" si="6">CONCATENATE(B59,"-",A59)</f>
-        <v>BCCR-WRF361</v>
+        <f>CONCATENATE(B59,"-",A59)</f>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>121</v>
+        <v>132</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="G59" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY59" s="22"/>
       <c r="BZ59" s="22"/>
@@ -4239,28 +4245,28 @@
       <c r="CH59" s="22"/>
       <c r="CI59" s="22"/>
     </row>
-    <row r="60" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="B60" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>UHOH-WRF361H</v>
+    <row r="60" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="18" t="str">
+        <f t="shared" ref="C60" si="6">CONCATENATE(B60,"-",A60)</f>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="F60" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="G60" s="38" t="s">
-        <v>141</v>
+        <v>120</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G60" s="37" t="s">
+        <v>68</v>
       </c>
       <c r="BY60" s="22"/>
       <c r="BZ60" s="22"/>
@@ -4274,14 +4280,29 @@
       <c r="CH60" s="22"/>
       <c r="CI60" s="22"/>
     </row>
-    <row r="61" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="56"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="46"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="48"/>
+    <row r="61" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>UHOH-WRF361H</v>
+      </c>
+      <c r="D61" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E61" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F61" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G61" s="38" t="s">
+        <v>139</v>
+      </c>
       <c r="BY61" s="22"/>
       <c r="BZ61" s="22"/>
       <c r="CA61" s="22"/>
@@ -4294,160 +4315,180 @@
       <c r="CH61" s="22"/>
       <c r="CI61" s="22"/>
     </row>
+    <row r="62" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="56"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="48"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="48"/>
+      <c r="BY62" s="22"/>
+      <c r="BZ62" s="22"/>
+      <c r="CA62" s="22"/>
+      <c r="CB62" s="22"/>
+      <c r="CC62" s="22"/>
+      <c r="CD62" s="22"/>
+      <c r="CE62" s="22"/>
+      <c r="CF62" s="22"/>
+      <c r="CG62" s="22"/>
+      <c r="CH62" s="22"/>
+      <c r="CI62" s="22"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E34:E39 F48:G48 A60:C61 B58:C58 E60:G61 E58:G58 B3:C15 A42:C42 F47 F49 F54 C17 F53:G53 E51:E54 A17:A22 F17:G22 E19:E22 A24:A40 B20:C41 F40:F42 G35:G40 F45 A45:C45 A47:C54 E50:G52">
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E35:E40 F49:G49 A61:C62 B59:C59 E61:G62 E59:G59 B3:C15 A43:C43 F48 F50 F55 C17 F54:G54 E52:E55 A17:A22 F17:G22 E19:E22 A24:A41 B20:C42 F41:F43 G36:G41 F46 A46:C46 A48:C55 E51:G53">
+    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A15 G33 E3:G14 E23:G32 F15:G15">
-    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A3:A15 G34 F15:G15 E23:G33 E3:G14">
+    <cfRule type="containsText" dxfId="31" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G34)))</formula>
+  <conditionalFormatting sqref="G35">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F33:F39">
-    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",F33)))</formula>
+  <conditionalFormatting sqref="F34:F40">
+    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",F34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58:G58 B58:C58">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:G57 B57:C57">
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56:G56 B56:C56">
-    <cfRule type="containsText" dxfId="25" priority="31" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F55:G55 A55:C55">
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:C46 E46:G46">
-    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:C59 E59:G59">
-    <cfRule type="containsText" dxfId="22" priority="28" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="F56:G56 A56:C56">
+    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A56)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A47:C47 E47:G47">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:C60 E60:G60">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42 G45">
-    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43 G46">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G48">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50">
+    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G55">
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
-    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G54">
-    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E54">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E47)))</formula>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:C43 E43:G43">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A43)))</formula>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:C44 E44:G44">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:C45 E45:G45">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Try to correct confusion about IPSL and IPSL-INERIS
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -33,7 +33,7 @@
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AU$1</definedName>
     <definedName name="Print_Area" localSheetId="0">ReadMe!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="207">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -666,6 +666,15 @@
   </si>
   <si>
     <t>"EUR-44" "EUR-11"</t>
+  </si>
+  <si>
+    <t>WRF311F</t>
+  </si>
+  <si>
+    <t>Sophie.Bastin@latmos.ipsl.fr</t>
+  </si>
+  <si>
+    <t>IPSL</t>
   </si>
 </sst>
 </file>
@@ -1164,6 +1173,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1173,31 +1203,10 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1856,20 +1865,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1895,20 +1904,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1931,127 +1940,127 @@
       <c r="A5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="64"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="62"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
     </row>
     <row r="7" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="62"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="61"/>
     </row>
     <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="61"/>
     </row>
     <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="61"/>
     </row>
     <row r="10" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="62"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="61"/>
     </row>
     <row r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="69"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="64"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
     </row>
     <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="51"/>
@@ -2066,32 +2075,32 @@
       <c r="J14" s="51"/>
     </row>
     <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2103,10 +2112,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI62"/>
+  <dimension ref="A1:CI63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,7 +2266,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f t="shared" ref="C3:C61" si="0">CONCATENATE(B3,"-",A3)</f>
+        <f t="shared" ref="C3:C62" si="0">CONCATENATE(B3,"-",A3)</f>
         <v>CHMI-ALADIN53</v>
       </c>
       <c r="D3" s="23" t="s">
@@ -3690,14 +3699,14 @@
         <v>197</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>60</v>
+        <v>206</v>
       </c>
       <c r="C44" s="18" t="str">
-        <f t="shared" ref="C44:C45" si="2">CONCATENATE(B44,"-",A44)</f>
-        <v>IPSL-INERIS-WRF311</v>
+        <f>CONCATENATE(B44,"-",A44)</f>
+        <v>IPSL-WRF311</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>184</v>
@@ -3722,14 +3731,14 @@
     </row>
     <row r="45" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B45" s="25" t="s">
         <v>60</v>
       </c>
       <c r="C45" s="18" t="str">
-        <f t="shared" si="2"/>
-        <v>IPSL-INERIS-WRF311NEMO</v>
+        <f>CONCATENATE(B45,"-",A45)</f>
+        <v>IPSL-INERIS-WRF311F</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>160</v>
@@ -3738,10 +3747,10 @@
         <v>184</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>170</v>
+        <v>107</v>
       </c>
       <c r="G45" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY45" s="22"/>
       <c r="BZ45" s="22"/>
@@ -3755,28 +3764,28 @@
       <c r="CH45" s="22"/>
       <c r="CI45" s="22"/>
     </row>
-    <row r="46" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>8</v>
+    <row r="46" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>206</v>
       </c>
       <c r="C46" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UM-WRF331</v>
+        <f t="shared" ref="C46" si="2">CONCATENATE(B46,"-",A46)</f>
+        <v>IPSL-WRF311NEMO</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>110</v>
+        <v>160</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="G46" s="37" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="BY46" s="22"/>
       <c r="BZ46" s="22"/>
@@ -3791,27 +3800,27 @@
       <c r="CI46" s="22"/>
     </row>
     <row r="47" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="29" t="s">
-        <v>16</v>
+      <c r="B47" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="C47" s="18" t="str">
-        <f t="shared" ref="C47" si="3">CONCATENATE(B47,"-",A47)</f>
-        <v>BCCR-WRF331</v>
+        <f t="shared" si="0"/>
+        <v>UM-WRF331</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>119</v>
+        <v>195</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>194</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G47" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY47" s="22"/>
       <c r="BZ47" s="22"/>
@@ -3827,26 +3836,26 @@
     </row>
     <row r="48" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C48" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>MIUB-WRF331A</v>
+        <f t="shared" ref="C48" si="3">CONCATENATE(B48,"-",A48)</f>
+        <v>BCCR-WRF331</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G48" s="37" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="BY48" s="22"/>
       <c r="BZ48" s="22"/>
@@ -3861,27 +3870,27 @@
       <c r="CI48" s="22"/>
     </row>
     <row r="49" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="25" t="s">
-        <v>11</v>
+      <c r="B49" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="C49" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CRP-GL-WRF331A</v>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="D49" s="23" t="s">
         <v>187</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F49" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G49" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY49" s="22"/>
       <c r="BZ49" s="22"/>
@@ -3895,28 +3904,28 @@
       <c r="CH49" s="22"/>
       <c r="CI49" s="22"/>
     </row>
-    <row r="50" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
+    <row r="50" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="17" t="s">
-        <v>55</v>
+      <c r="B50" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="C50" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AUTH-Met-WRF331A</v>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>189</v>
       </c>
       <c r="F50" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G50" s="37" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="BY50" s="22"/>
       <c r="BZ50" s="22"/>
@@ -3930,28 +3939,28 @@
       <c r="CH50" s="22"/>
       <c r="CI50" s="22"/>
     </row>
-    <row r="51" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>16</v>
+    <row r="51" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C51" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>BCCR-WRF331C</v>
+        <v>AUTH-Met-WRF331A</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E51" s="24" t="s">
-        <v>119</v>
+        <v>191</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="G51" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY51" s="22"/>
       <c r="BZ51" s="22"/>
@@ -3966,27 +3975,27 @@
       <c r="CI51" s="22"/>
     </row>
     <row r="52" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>52</v>
+      <c r="A52" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C52" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCAN-WRF331G</v>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>106</v>
+        <v>120</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="G52" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY52" s="22"/>
       <c r="BZ52" s="22"/>
@@ -4001,24 +4010,24 @@
       <c r="CI52" s="22"/>
     </row>
     <row r="53" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
-        <v>67</v>
+      <c r="A53" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C53" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>NUIM-WRF341E</v>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F53" s="20" t="s">
-        <v>110</v>
+        <v>183</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="G53" s="37" t="s">
         <v>140</v>
@@ -4036,21 +4045,21 @@
       <c r="CI53" s="22"/>
     </row>
     <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>17</v>
+      <c r="A54" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C54" s="18" t="str">
-        <f>CONCATENATE(B54,"-",A54)</f>
-        <v>IDL-WRF350D</v>
+        <f t="shared" si="0"/>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>177</v>
+        <v>79</v>
       </c>
       <c r="F54" s="20" t="s">
         <v>110</v>
@@ -4071,27 +4080,27 @@
       <c r="CI54" s="22"/>
     </row>
     <row r="55" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>52</v>
+      <c r="A55" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C55" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF350I</v>
+        <f>CONCATENATE(B55,"-",A55)</f>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F55" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G55" s="37" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="BY55" s="22"/>
       <c r="BZ55" s="22"/>
@@ -4105,28 +4114,28 @@
       <c r="CH55" s="22"/>
       <c r="CI55" s="22"/>
     </row>
-    <row r="56" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="C56" s="18" t="str">
-        <f t="shared" ref="C56" si="4">CONCATENATE(B56,"-",A56)</f>
-        <v>UNSW-WRF360J</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF350I</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="E56" s="50" t="s">
-        <v>117</v>
+        <v>185</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>183</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G56" s="37" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="BY56" s="22"/>
       <c r="BZ56" s="22"/>
@@ -4142,14 +4151,14 @@
     </row>
     <row r="57" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>141</v>
       </c>
       <c r="C57" s="18" t="str">
-        <f>CONCATENATE(B57,"-",A57)</f>
-        <v>UNSW-WRF360K</v>
+        <f t="shared" ref="C57" si="4">CONCATENATE(B57,"-",A57)</f>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D57" s="23" t="s">
         <v>116</v>
@@ -4177,14 +4186,14 @@
     </row>
     <row r="58" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>141</v>
       </c>
       <c r="C58" s="18" t="str">
-        <f t="shared" ref="C58" si="5">CONCATENATE(B58,"-",A58)</f>
-        <v>UNSW-WRF360L</v>
+        <f>CONCATENATE(B58,"-",A58)</f>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D58" s="23" t="s">
         <v>116</v>
@@ -4210,28 +4219,28 @@
       <c r="CH58" s="22"/>
       <c r="CI58" s="22"/>
     </row>
-    <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C59" s="18" t="str">
-        <f>CONCATENATE(B59,"-",A59)</f>
-        <v>MU-WRF360M</v>
+        <f t="shared" ref="C59" si="5">CONCATENATE(B59,"-",A59)</f>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>131</v>
+        <v>116</v>
+      </c>
+      <c r="E59" s="50" t="s">
+        <v>117</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G59" s="37" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="BY59" s="22"/>
       <c r="BZ59" s="22"/>
@@ -4245,28 +4254,28 @@
       <c r="CH59" s="22"/>
       <c r="CI59" s="22"/>
     </row>
-    <row r="60" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B60" s="29" t="s">
-        <v>16</v>
+    <row r="60" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="C60" s="18" t="str">
-        <f t="shared" ref="C60" si="6">CONCATENATE(B60,"-",A60)</f>
-        <v>BCCR-WRF361</v>
+        <f>CONCATENATE(B60,"-",A60)</f>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>119</v>
+        <v>132</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G60" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY60" s="22"/>
       <c r="BZ60" s="22"/>
@@ -4280,28 +4289,28 @@
       <c r="CH60" s="22"/>
       <c r="CI60" s="22"/>
     </row>
-    <row r="61" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B61" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>UHOH-WRF361H</v>
+    <row r="61" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="18" t="str">
+        <f t="shared" ref="C61" si="6">CONCATENATE(B61,"-",A61)</f>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E61" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="F61" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G61" s="38" t="s">
-        <v>139</v>
+        <v>120</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G61" s="37" t="s">
+        <v>68</v>
       </c>
       <c r="BY61" s="22"/>
       <c r="BZ61" s="22"/>
@@ -4315,14 +4324,29 @@
       <c r="CH61" s="22"/>
       <c r="CI61" s="22"/>
     </row>
-    <row r="62" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="56"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="48"/>
+    <row r="62" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>UHOH-WRF361H</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F62" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G62" s="38" t="s">
+        <v>139</v>
+      </c>
       <c r="BY62" s="22"/>
       <c r="BZ62" s="22"/>
       <c r="CA62" s="22"/>
@@ -4335,163 +4359,191 @@
       <c r="CH62" s="22"/>
       <c r="CI62" s="22"/>
     </row>
+    <row r="63" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="56"/>
+      <c r="B63" s="45"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="48"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="48"/>
+      <c r="BY63" s="22"/>
+      <c r="BZ63" s="22"/>
+      <c r="CA63" s="22"/>
+      <c r="CB63" s="22"/>
+      <c r="CC63" s="22"/>
+      <c r="CD63" s="22"/>
+      <c r="CE63" s="22"/>
+      <c r="CF63" s="22"/>
+      <c r="CG63" s="22"/>
+      <c r="CH63" s="22"/>
+      <c r="CI63" s="22"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E35:E40 F49:G49 A61:C62 B59:C59 E61:G62 E59:G59 B3:C15 A43:C43 F48 F50 F55 C17 F54:G54 E52:E55 A17:A22 F17:G22 E19:E22 A24:A41 B20:C42 F41:F43 G36:G41 F46 A46:C46 A48:C55 E51:G53">
-    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E35:E40 F50:G50 A62:C63 B60:C60 E62:G63 E60:G60 B3:C15 A43:C43 F49 F51 F56 C17 F55:G55 E53:E56 A17:A22 F17:G22 E19:E22 A24:A41 B20:C42 F41:F43 G36:G41 F47 A47:C47 A49:C56 E52:G54">
+    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A15 G34 F15:G15 E23:G33 E3:G14">
-    <cfRule type="containsText" dxfId="31" priority="36" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:F40">
-    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F34)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F59:G59 B59:C59">
+    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F58:G58 B58:C58">
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B58)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F57:G57 B57:C57">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F56:G56 A56:C56">
-    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47:C47 E47:G47">
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:C60 E60:G60">
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="F57:G57 A57:C57">
+    <cfRule type="containsText" dxfId="25" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A48:C48 E48:G48">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:C61 E61:G61">
+    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="28" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43 G46">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="G43 G47">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G48)))</formula>
+  <conditionalFormatting sqref="G49">
+    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
+  <conditionalFormatting sqref="G51">
+    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G55">
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G55)))</formula>
+  <conditionalFormatting sqref="G56">
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E55)))</formula>
+  <conditionalFormatting sqref="E56">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A44:C44 E44:G44">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A44)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A46:C46 E46:G46">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A45:C45 E45:G45">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A45)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D44" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Further IPSL correction by Sophie Bastin
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="885" windowWidth="16605" windowHeight="8550" activeTab="1"/>
+    <workbookView xWindow="10755" yWindow="4065" windowWidth="22320" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="7" r:id="rId1"/>
@@ -36,12 +36,17 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="210">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -675,6 +680,15 @@
   </si>
   <si>
     <t>IPSL</t>
+  </si>
+  <si>
+    <t>sophie.bastin@latmos.ipsl.fr</t>
+  </si>
+  <si>
+    <t>"MED-18"</t>
+  </si>
+  <si>
+    <t>"MED-44 MED-18"</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1232,17 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1854,7 +1878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1864,7 +1888,7 @@
     <col min="2" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>90</v>
       </c>
@@ -1883,10 +1907,10 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <f>AllEntries!A1</f>
-        <v>42159</v>
+        <v>42284</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1903,7 +1927,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="67" t="s">
         <v>91</v>
       </c>
@@ -1920,7 +1944,7 @@
       <c r="L3" s="67"/>
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:15" s="6" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>97</v>
       </c>
@@ -1936,7 +1960,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>111</v>
       </c>
@@ -1952,7 +1976,7 @@
       <c r="I5" s="68"/>
       <c r="J5" s="69"/>
     </row>
-    <row r="6" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
@@ -1968,7 +1992,7 @@
       <c r="I6" s="60"/>
       <c r="J6" s="61"/>
     </row>
-    <row r="7" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
@@ -1984,7 +2008,7 @@
       <c r="I7" s="60"/>
       <c r="J7" s="61"/>
     </row>
-    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>92</v>
       </c>
@@ -2000,7 +2024,7 @@
       <c r="I8" s="60"/>
       <c r="J8" s="61"/>
     </row>
-    <row r="9" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
@@ -2016,7 +2040,7 @@
       <c r="I9" s="60"/>
       <c r="J9" s="61"/>
     </row>
-    <row r="10" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>93</v>
       </c>
@@ -2032,7 +2056,7 @@
       <c r="I10" s="60"/>
       <c r="J10" s="61"/>
     </row>
-    <row r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
@@ -2048,7 +2072,7 @@
       <c r="I11" s="63"/>
       <c r="J11" s="64"/>
     </row>
-    <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="58" t="s">
         <v>125</v>
       </c>
@@ -2062,7 +2086,7 @@
       <c r="I13" s="58"/>
       <c r="J13" s="58"/>
     </row>
-    <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="51"/>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
@@ -2074,7 +2098,7 @@
       <c r="I14" s="51"/>
       <c r="J14" s="51"/>
     </row>
-    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="59" t="s">
         <v>126</v>
       </c>
@@ -2103,26 +2127,31 @@
     <mergeCell ref="B11:J11"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:CI63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="57" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
@@ -2136,7 +2165,7 @@
     <col min="20" max="20" width="14.42578125" customWidth="1"/>
     <col min="21" max="21" width="16" customWidth="1"/>
     <col min="22" max="22" width="17.28515625" customWidth="1"/>
-    <col min="23" max="24" width="17.5703125" customWidth="1"/>
+    <col min="23" max="24" width="17.42578125" customWidth="1"/>
     <col min="25" max="25" width="12" customWidth="1"/>
     <col min="26" max="26" width="15.28515625" customWidth="1"/>
     <col min="27" max="27" width="12.42578125" customWidth="1"/>
@@ -2148,23 +2177,23 @@
     <col min="33" max="33" width="16.85546875" customWidth="1"/>
     <col min="34" max="36" width="20.42578125" customWidth="1"/>
     <col min="37" max="37" width="10.7109375" customWidth="1"/>
-    <col min="38" max="38" width="23.5703125" customWidth="1"/>
+    <col min="38" max="38" width="23.42578125" customWidth="1"/>
     <col min="39" max="39" width="12.28515625" customWidth="1"/>
-    <col min="40" max="40" width="15.5703125" customWidth="1"/>
+    <col min="40" max="40" width="15.42578125" customWidth="1"/>
     <col min="41" max="41" width="18.28515625" customWidth="1"/>
     <col min="42" max="42" width="20.140625" customWidth="1"/>
     <col min="43" max="43" width="16" customWidth="1"/>
     <col min="44" max="44" width="13.7109375" customWidth="1"/>
     <col min="45" max="45" width="22.42578125" customWidth="1"/>
     <col min="46" max="46" width="16.140625" customWidth="1"/>
-    <col min="47" max="48" width="15.5703125" customWidth="1"/>
+    <col min="47" max="48" width="15.42578125" customWidth="1"/>
     <col min="49" max="49" width="16.140625" customWidth="1"/>
     <col min="77" max="87" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:87" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="53">
-        <v>42159</v>
+        <v>42284</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3712,7 +3741,7 @@
         <v>184</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="G44" s="37" t="s">
         <v>140</v>
@@ -3775,14 +3804,14 @@
         <f t="shared" ref="C46" si="2">CONCATENATE(B46,"-",A46)</f>
         <v>IPSL-WRF311NEMO</v>
       </c>
-      <c r="D46" s="23" t="s">
-        <v>160</v>
+      <c r="D46" s="24" t="s">
+        <v>207</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>184</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="G46" s="37" t="s">
         <v>140</v>
@@ -4381,169 +4410,180 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E35:E40 F50:G50 A62:C63 B60:C60 E62:G63 E60:G60 B3:C15 A43:C43 F49 F51 F56 C17 F55:G55 E53:E56 A17:A22 F17:G22 E19:E22 A24:A41 B20:C42 F41:F43 G36:G41 F47 A47:C47 A49:C56 E52:G54">
-    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A15 G34 F15:G15 E23:G33 E3:G14">
-    <cfRule type="containsText" dxfId="30" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:F40">
-    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:G59 B59:C59">
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58:G58 B58:C58">
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:G57 A57:C57">
-    <cfRule type="containsText" dxfId="25" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:C61 E61:G61">
-    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="containsText" dxfId="22" priority="28" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43 G47">
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:C44 E44:G44">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:C46 E46:G46">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:C45 E45:G45">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A45)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",D46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D44" r:id="rId1"/>
+    <hyperlink ref="D46" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added University of Michigan
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -33,7 +33,7 @@
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AU$1</definedName>
     <definedName name="Print_Area" localSheetId="0">ReadMe!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$63</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="213">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -689,6 +689,15 @@
   </si>
   <si>
     <t>"MED-44 MED-18"</t>
+  </si>
+  <si>
+    <t>Alexander Bryan (ambrya@umich.edu)</t>
+  </si>
+  <si>
+    <t>University of Michigan</t>
+  </si>
+  <si>
+    <t>"NAM-44"</t>
   </si>
 </sst>
 </file>
@@ -698,7 +707,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-407]d/\ mmm\ yy;@"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -867,6 +876,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1136,9 +1152,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1187,6 +1200,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1194,12 +1228,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1208,20 +1236,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1232,7 +1248,27 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1889,20 +1925,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1928,20 +1964,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1964,17 +2000,17 @@
       <c r="A5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="63"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -2044,7 +2080,7 @@
       <c r="A10" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="66" t="s">
         <v>101</v>
       </c>
       <c r="C10" s="60"/>
@@ -2060,71 +2096,71 @@
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="64"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="68"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2141,15 +2177,15 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI63"/>
+  <dimension ref="A1:CI64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="57" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="56" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="5" width="22.7109375" customWidth="1"/>
@@ -2192,7 +2228,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:87" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53">
+      <c r="A1" s="52">
         <v>42284</v>
       </c>
       <c r="B1" s="5"/>
@@ -2253,39 +2289,39 @@
       <c r="BV1" s="3"/>
       <c r="BW1" s="3"/>
     </row>
-    <row r="2" spans="1:87" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:87" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="BY2" s="44"/>
-      <c r="BZ2" s="44"/>
-      <c r="CA2" s="44"/>
-      <c r="CB2" s="44"/>
-      <c r="CC2" s="44"/>
-      <c r="CD2" s="44"/>
-      <c r="CE2" s="44"/>
-      <c r="CF2" s="44"/>
-      <c r="CG2" s="44"/>
-      <c r="CH2" s="44"/>
-      <c r="CI2" s="44"/>
+      <c r="BY2" s="43"/>
+      <c r="BZ2" s="43"/>
+      <c r="CA2" s="43"/>
+      <c r="CB2" s="43"/>
+      <c r="CC2" s="43"/>
+      <c r="CD2" s="43"/>
+      <c r="CE2" s="43"/>
+      <c r="CF2" s="43"/>
+      <c r="CG2" s="43"/>
+      <c r="CH2" s="43"/>
+      <c r="CI2" s="43"/>
     </row>
     <row r="3" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
@@ -2295,7 +2331,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f t="shared" ref="C3:C62" si="0">CONCATENATE(B3,"-",A3)</f>
+        <f t="shared" ref="C3:C63" si="0">CONCATENATE(B3,"-",A3)</f>
         <v>CHMI-ALADIN53</v>
       </c>
       <c r="D3" s="23" t="s">
@@ -2393,7 +2429,7 @@
       <c r="CI5" s="22"/>
     </row>
     <row r="6" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="53" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="17" t="s">
@@ -3478,28 +3514,28 @@
       <c r="CH36" s="22"/>
       <c r="CI36" s="22"/>
     </row>
-    <row r="37" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>32</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C37" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ENEA-RegCM4-3</v>
+        <v>UM-RegCM4-3</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>155</v>
+        <v>210</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>78</v>
+        <v>211</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY37" s="22"/>
       <c r="BZ37" s="22"/>
@@ -3515,26 +3551,26 @@
     </row>
     <row r="38" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C38" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MPI-CSC-REMO2009</v>
+        <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY38" s="22"/>
       <c r="BZ38" s="22"/>
@@ -3560,13 +3596,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="28" t="s">
-        <v>103</v>
+      <c r="F39" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="G39" s="37" t="s">
         <v>68</v>
@@ -3595,13 +3631,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F40" s="20" t="s">
-        <v>110</v>
+      <c r="F40" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="G40" s="37" t="s">
         <v>68</v>
@@ -3618,28 +3654,28 @@
       <c r="CH40" s="22"/>
       <c r="CI40" s="22"/>
     </row>
-    <row r="41" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>181</v>
+        <v>44</v>
       </c>
       <c r="C41" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>Alaro0-RMIB-Ugent</v>
+        <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="F41" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G41" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY41" s="22"/>
       <c r="BZ41" s="22"/>
@@ -3653,28 +3689,28 @@
       <c r="CH41" s="22"/>
       <c r="CI41" s="22"/>
     </row>
-    <row r="42" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>137</v>
+    <row r="42" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>181</v>
       </c>
       <c r="C42" s="18" t="str">
-        <f>CONCATENATE(B42,"-",A42)</f>
-        <v>MGO-RRCM</v>
+        <f t="shared" si="0"/>
+        <v>Alaro0-RMIB-Ugent</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
       <c r="F42" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY42" s="22"/>
       <c r="BZ42" s="22"/>
@@ -3688,28 +3724,28 @@
       <c r="CH42" s="22"/>
       <c r="CI42" s="22"/>
     </row>
-    <row r="43" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>56</v>
+    <row r="43" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="C43" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>AUTH-LHTEE-WRF321B</v>
+        <f>CONCATENATE(B43,"-",A43)</f>
+        <v>MGO-RRCM</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>192</v>
+        <v>134</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="F43" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G43" s="37" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="BY43" s="22"/>
       <c r="BZ43" s="22"/>
@@ -3723,28 +3759,28 @@
       <c r="CH43" s="22"/>
       <c r="CI43" s="22"/>
     </row>
-    <row r="44" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>206</v>
+    <row r="44" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="C44" s="18" t="str">
-        <f>CONCATENATE(B44,"-",A44)</f>
-        <v>IPSL-WRF311</v>
+        <f t="shared" si="0"/>
+        <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>209</v>
+        <v>193</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>110</v>
       </c>
       <c r="G44" s="37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="BY44" s="22"/>
       <c r="BZ44" s="22"/>
@@ -3760,26 +3796,26 @@
     </row>
     <row r="45" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>60</v>
+        <v>206</v>
       </c>
       <c r="C45" s="18" t="str">
         <f>CONCATENATE(B45,"-",A45)</f>
-        <v>IPSL-INERIS-WRF311F</v>
+        <v>IPSL-WRF311</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>160</v>
+        <v>205</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>184</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
       <c r="G45" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY45" s="22"/>
       <c r="BZ45" s="22"/>
@@ -3795,26 +3831,26 @@
     </row>
     <row r="46" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>206</v>
+        <v>60</v>
       </c>
       <c r="C46" s="18" t="str">
-        <f t="shared" ref="C46" si="2">CONCATENATE(B46,"-",A46)</f>
-        <v>IPSL-WRF311NEMO</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>207</v>
+        <f>CONCATENATE(B46,"-",A46)</f>
+        <v>IPSL-INERIS-WRF311F</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>160</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>184</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>208</v>
+        <v>107</v>
       </c>
       <c r="G46" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY46" s="22"/>
       <c r="BZ46" s="22"/>
@@ -3828,28 +3864,28 @@
       <c r="CH46" s="22"/>
       <c r="CI46" s="22"/>
     </row>
-    <row r="47" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>8</v>
+    <row r="47" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>206</v>
       </c>
       <c r="C47" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UM-WRF331</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>110</v>
+        <f t="shared" ref="C47" si="2">CONCATENATE(B47,"-",A47)</f>
+        <v>IPSL-WRF311NEMO</v>
+      </c>
+      <c r="D47" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>208</v>
       </c>
       <c r="G47" s="37" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="BY47" s="22"/>
       <c r="BZ47" s="22"/>
@@ -3864,27 +3900,27 @@
       <c r="CI47" s="22"/>
     </row>
     <row r="48" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="29" t="s">
-        <v>16</v>
+      <c r="B48" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="C48" s="18" t="str">
-        <f t="shared" ref="C48" si="3">CONCATENATE(B48,"-",A48)</f>
-        <v>BCCR-WRF331</v>
+        <f t="shared" si="0"/>
+        <v>UM-WRF331</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>119</v>
+        <v>195</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>194</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G48" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY48" s="22"/>
       <c r="BZ48" s="22"/>
@@ -3900,26 +3936,26 @@
     </row>
     <row r="49" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C49" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>MIUB-WRF331A</v>
+        <f t="shared" ref="C49" si="3">CONCATENATE(B49,"-",A49)</f>
+        <v>BCCR-WRF331</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G49" s="37" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="BY49" s="22"/>
       <c r="BZ49" s="22"/>
@@ -3934,27 +3970,27 @@
       <c r="CI49" s="22"/>
     </row>
     <row r="50" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="25" t="s">
-        <v>11</v>
+      <c r="B50" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="C50" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CRP-GL-WRF331A</v>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="D50" s="23" t="s">
         <v>187</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F50" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G50" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY50" s="22"/>
       <c r="BZ50" s="22"/>
@@ -3968,28 +4004,28 @@
       <c r="CH50" s="22"/>
       <c r="CI50" s="22"/>
     </row>
-    <row r="51" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
+    <row r="51" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="17" t="s">
-        <v>55</v>
+      <c r="B51" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="C51" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AUTH-Met-WRF331A</v>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>189</v>
       </c>
       <c r="F51" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G51" s="37" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="BY51" s="22"/>
       <c r="BZ51" s="22"/>
@@ -4003,28 +4039,28 @@
       <c r="CH51" s="22"/>
       <c r="CI51" s="22"/>
     </row>
-    <row r="52" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="29" t="s">
-        <v>16</v>
+    <row r="52" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C52" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>BCCR-WRF331C</v>
+        <v>AUTH-Met-WRF331A</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>119</v>
+        <v>191</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="G52" s="37" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="BY52" s="22"/>
       <c r="BZ52" s="22"/>
@@ -4039,27 +4075,27 @@
       <c r="CI52" s="22"/>
     </row>
     <row r="53" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>52</v>
+      <c r="A53" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C53" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCAN-WRF331G</v>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>106</v>
+        <v>120</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="G53" s="37" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="BZ53" s="22"/>
@@ -4074,24 +4110,24 @@
       <c r="CI53" s="22"/>
     </row>
     <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
-        <v>67</v>
+      <c r="A54" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C54" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>NUIM-WRF341E</v>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>110</v>
+        <v>183</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="G54" s="37" t="s">
         <v>140</v>
@@ -4109,21 +4145,21 @@
       <c r="CI54" s="22"/>
     </row>
     <row r="55" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>17</v>
+      <c r="A55" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C55" s="18" t="str">
-        <f>CONCATENATE(B55,"-",A55)</f>
-        <v>IDL-WRF350D</v>
+        <f t="shared" si="0"/>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>177</v>
+        <v>79</v>
       </c>
       <c r="F55" s="20" t="s">
         <v>110</v>
@@ -4144,27 +4180,27 @@
       <c r="CI55" s="22"/>
     </row>
     <row r="56" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>52</v>
+      <c r="A56" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C56" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF350I</v>
+        <f>CONCATENATE(B56,"-",A56)</f>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F56" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G56" s="37" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="BY56" s="22"/>
       <c r="BZ56" s="22"/>
@@ -4178,28 +4214,28 @@
       <c r="CH56" s="22"/>
       <c r="CI56" s="22"/>
     </row>
-    <row r="57" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="C57" s="18" t="str">
-        <f t="shared" ref="C57" si="4">CONCATENATE(B57,"-",A57)</f>
-        <v>UNSW-WRF360J</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF350I</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="E57" s="50" t="s">
-        <v>117</v>
+        <v>185</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>183</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G57" s="37" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="BY57" s="22"/>
       <c r="BZ57" s="22"/>
@@ -4215,19 +4251,19 @@
     </row>
     <row r="58" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>141</v>
       </c>
       <c r="C58" s="18" t="str">
-        <f>CONCATENATE(B58,"-",A58)</f>
-        <v>UNSW-WRF360K</v>
+        <f t="shared" ref="C58" si="4">CONCATENATE(B58,"-",A58)</f>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D58" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="E58" s="50" t="s">
+      <c r="E58" s="49" t="s">
         <v>117</v>
       </c>
       <c r="F58" s="20" t="s">
@@ -4250,19 +4286,19 @@
     </row>
     <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B59" s="17" t="s">
         <v>141</v>
       </c>
       <c r="C59" s="18" t="str">
-        <f t="shared" ref="C59" si="5">CONCATENATE(B59,"-",A59)</f>
-        <v>UNSW-WRF360L</v>
+        <f>CONCATENATE(B59,"-",A59)</f>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D59" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="E59" s="50" t="s">
+      <c r="E59" s="49" t="s">
         <v>117</v>
       </c>
       <c r="F59" s="20" t="s">
@@ -4283,28 +4319,28 @@
       <c r="CH59" s="22"/>
       <c r="CI59" s="22"/>
     </row>
-    <row r="60" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C60" s="18" t="str">
-        <f>CONCATENATE(B60,"-",A60)</f>
-        <v>MU-WRF360M</v>
+        <f t="shared" ref="C60" si="5">CONCATENATE(B60,"-",A60)</f>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>131</v>
+        <v>116</v>
+      </c>
+      <c r="E60" s="49" t="s">
+        <v>117</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="G60" s="37" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="BY60" s="22"/>
       <c r="BZ60" s="22"/>
@@ -4318,28 +4354,28 @@
       <c r="CH60" s="22"/>
       <c r="CI60" s="22"/>
     </row>
-    <row r="61" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B61" s="29" t="s">
-        <v>16</v>
+    <row r="61" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="C61" s="18" t="str">
-        <f t="shared" ref="C61" si="6">CONCATENATE(B61,"-",A61)</f>
-        <v>BCCR-WRF361</v>
+        <f>CONCATENATE(B61,"-",A61)</f>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>119</v>
+        <v>132</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G61" s="37" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="BY61" s="22"/>
       <c r="BZ61" s="22"/>
@@ -4353,28 +4389,28 @@
       <c r="CH61" s="22"/>
       <c r="CI61" s="22"/>
     </row>
-    <row r="62" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B62" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>UHOH-WRF361H</v>
+    <row r="62" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="18" t="str">
+        <f t="shared" ref="C62" si="6">CONCATENATE(B62,"-",A62)</f>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E62" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="F62" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G62" s="38" t="s">
-        <v>139</v>
+        <v>120</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G62" s="37" t="s">
+        <v>68</v>
       </c>
       <c r="BY62" s="22"/>
       <c r="BZ62" s="22"/>
@@ -4388,14 +4424,29 @@
       <c r="CH62" s="22"/>
       <c r="CI62" s="22"/>
     </row>
-    <row r="63" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="56"/>
-      <c r="B63" s="45"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="48"/>
+    <row r="63" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>UHOH-WRF361H</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G63" s="38" t="s">
+        <v>139</v>
+      </c>
       <c r="BY63" s="22"/>
       <c r="BZ63" s="22"/>
       <c r="CA63" s="22"/>
@@ -4408,178 +4459,204 @@
       <c r="CH63" s="22"/>
       <c r="CI63" s="22"/>
     </row>
+    <row r="64" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="55"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="46"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="47"/>
+      <c r="BY64" s="22"/>
+      <c r="BZ64" s="22"/>
+      <c r="CA64" s="22"/>
+      <c r="CB64" s="22"/>
+      <c r="CC64" s="22"/>
+      <c r="CD64" s="22"/>
+      <c r="CE64" s="22"/>
+      <c r="CF64" s="22"/>
+      <c r="CG64" s="22"/>
+      <c r="CH64" s="22"/>
+      <c r="CI64" s="22"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E35:E40 F50:G50 A62:C63 B60:C60 E62:G63 E60:G60 B3:C15 A43:C43 F49 F51 F56 C17 F55:G55 E53:E56 A17:A22 F17:G22 E19:E22 A24:A41 B20:C42 F41:F43 G36:G41 F47 A47:C47 A49:C56 E52:G54">
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E35:E36 F51:G51 A63:C64 B61:C61 E63:G64 E61:G61 B3:C15 A44:C44 F50 F52 F57 C17 F56:G56 E54:E57 A17:A22 F17:G22 E19:E22 B20:C43 F42:F44 G36:G42 F48 A48:C48 A50:C57 E53:G55 A24:A42 E38:E41">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A15 G34 F15:G15 E23:G33 E3:G14">
-    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="39" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:F40">
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="F34:F41">
+    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F34)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F60:G60 B60:C60">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F59:G59 B59:C59">
-    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="34" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B59)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58:G58 B58:C58">
-    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F57:G57 A57:C57">
-    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:C61 E61:G61">
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="F58:G58 A58:C58">
+    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A49:C49 E49:G49">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:C62 E62:G62">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
+  <conditionalFormatting sqref="A61">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G43 G47">
-    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44 G48">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G50">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G52">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G57">
+    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A44:C44 E44:G44">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A44)))</formula>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:C45 E45:G45">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47:C47 E47:G47">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:C46 E46:G46">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A46)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A45:C45 E45:G45">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A45)))</formula>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",D47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+  <conditionalFormatting sqref="E37">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D44" r:id="rId1"/>
-    <hyperlink ref="D46" r:id="rId2"/>
+    <hyperlink ref="D45" r:id="rId1"/>
+    <hyperlink ref="D47" r:id="rId2"/>
+    <hyperlink ref="D37" r:id="rId3" display="javascript:_e(%7B%7D,'cvml','ambrya@umich.edu');"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Editing error correction for RMIB-UGent
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="214">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -604,9 +604,6 @@
     <t>RMIB-Ugent</t>
   </si>
   <si>
-    <t>Alaro0</t>
-  </si>
-  <si>
     <t>Royal Meteorological Institute of Belgium and Ghent University</t>
   </si>
   <si>
@@ -698,6 +695,12 @@
   </si>
   <si>
     <t>WRF361F</t>
+  </si>
+  <si>
+    <t>ALARO-0</t>
+  </si>
+  <si>
+    <t>"EUR-11 EUR-44"</t>
   </si>
 </sst>
 </file>
@@ -1203,6 +1206,27 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1210,33 +1234,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1248,67 +1251,7 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1965,20 +1908,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2004,20 +1947,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2040,127 +1983,127 @@
       <c r="A5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="64"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="62"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="62"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="62"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="64"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="69"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="50"/>
@@ -2175,32 +2118,32 @@
       <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2219,8 +2162,8 @@
   </sheetPr>
   <dimension ref="A1:CI65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,7 +2321,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>110</v>
@@ -2448,10 +2391,10 @@
         <v>146</v>
       </c>
       <c r="E5" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>201</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>202</v>
       </c>
       <c r="G5" s="37" t="s">
         <v>140</v>
@@ -2483,10 +2426,10 @@
         <v>145</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G6" s="37" t="s">
         <v>140</v>
@@ -2518,7 +2461,7 @@
         <v>144</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>110</v>
@@ -2621,7 +2564,7 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>61</v>
@@ -3346,7 +3289,7 @@
     </row>
     <row r="31" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>13</v>
@@ -3359,7 +3302,7 @@
         <v>146</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>170</v>
@@ -3461,7 +3404,7 @@
         <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>156</v>
@@ -3566,13 +3509,13 @@
         <v>UM-RegCM4-3</v>
       </c>
       <c r="D37" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E37" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="F37" s="20" t="s">
         <v>209</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>210</v>
       </c>
       <c r="G37" s="37" t="s">
         <v>68</v>
@@ -3731,23 +3674,23 @@
     </row>
     <row r="42" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B42" s="17" t="s">
-        <v>181</v>
-      </c>
       <c r="C42" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>Alaro0-RMIB-Ugent</v>
+        <v>RMIB-Ugent-ALARO-0</v>
       </c>
       <c r="D42" s="23" t="s">
         <v>179</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>110</v>
+        <v>213</v>
       </c>
       <c r="G42" s="37" t="s">
         <v>140</v>
@@ -3811,10 +3754,10 @@
         <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F44" s="20" t="s">
         <v>110</v>
@@ -3836,23 +3779,23 @@
     </row>
     <row r="45" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C45" s="18" t="str">
         <f>CONCATENATE(B45,"-",A45)</f>
         <v>IPSL-WRF311</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G45" s="37" t="s">
         <v>140</v>
@@ -3871,23 +3814,23 @@
     </row>
     <row r="46" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C46" s="18" t="str">
         <f t="shared" ref="C46" si="2">CONCATENATE(B46,"-",A46)</f>
         <v>IPSL-WRF311NEMO</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G46" s="37" t="s">
         <v>140</v>
@@ -3916,10 +3859,10 @@
         <v>UM-WRF331</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F47" s="20" t="s">
         <v>110</v>
@@ -3986,10 +3929,10 @@
         <v>MIUB-WRF331A</v>
       </c>
       <c r="D49" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="E49" s="24" t="s">
         <v>187</v>
-      </c>
-      <c r="E49" s="24" t="s">
-        <v>188</v>
       </c>
       <c r="F49" s="20" t="s">
         <v>110</v>
@@ -4021,10 +3964,10 @@
         <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F50" s="20" t="s">
         <v>110</v>
@@ -4056,10 +3999,10 @@
         <v>AUTH-Met-WRF331A</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F51" s="20" t="s">
         <v>110</v>
@@ -4116,7 +4059,7 @@
     </row>
     <row r="53" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B53" s="25" t="s">
         <v>60</v>
@@ -4129,7 +4072,7 @@
         <v>160</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F53" s="19" t="s">
         <v>107</v>
@@ -4161,10 +4104,10 @@
         <v>UCAN-WRF331G</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F54" s="19" t="s">
         <v>106</v>
@@ -4266,10 +4209,10 @@
         <v>UCAN-WRF350I</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F57" s="20" t="s">
         <v>110</v>
@@ -4466,7 +4409,7 @@
     </row>
     <row r="63" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B63" s="25" t="s">
         <v>60</v>
@@ -4479,7 +4422,7 @@
         <v>160</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F63" s="19" t="s">
         <v>107</v>
@@ -4556,162 +4499,162 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E35:E36 F50:G50 A64:C65 B61:C61 E64:G65 E61:G61 B3:C15 A44:C44 F49 F51 F57 C17 F56:G56 E54:E57 A17:A22 F17:G22 E19:E22 B20:C43 F42:F44 G36:G42 F47 A47:C47 E52:G52 A24:A42 E38:E41 A49:C52 A54:C57 E54:G55">
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A15 G34 F15:G15 E23:G33 E3:G14">
-    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="34" priority="41" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:F41">
-    <cfRule type="containsText" dxfId="33" priority="40" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="40" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:G60 B60:C60">
-    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:G59 B59:C59">
-    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58:G58 A58:C58">
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="35" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:C62 E62:G62">
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="34" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="25" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44 G47">
-    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="22" priority="28" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="28" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:C45 E45:G45">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:C46 E46:G46">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E37)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Trying again due to non-updated web page (wrong data manually typed into xls)
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10755" yWindow="4065" windowWidth="22320" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="315" windowWidth="22320" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="7" r:id="rId1"/>
@@ -1206,6 +1206,27 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1215,31 +1236,10 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1908,20 +1908,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1929,7 +1929,7 @@
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <f>AllEntries!A1</f>
-        <v>42284</v>
+        <v>42325</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1947,20 +1947,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1983,127 +1983,127 @@
       <c r="A5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="64"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="62"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="62"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="61"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="61"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="61"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="62"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="61"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="69"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="64"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="50"/>
@@ -2118,32 +2118,32 @@
       <c r="J14" s="50"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2162,9 +2162,7 @@
   </sheetPr>
   <dimension ref="A1:CI65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2212,7 +2210,7 @@
   <sheetData>
     <row r="1" spans="1:87" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52">
-        <v>42284</v>
+        <v>42325</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>

</xml_diff>

<commit_message>
Update of AUTH information
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="224">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -728,6 +728,9 @@
   </si>
   <si>
     <t>Helmholtz-Zentrum Geesthacht, Climate Service Center Germany</t>
+  </si>
+  <si>
+    <t>WRF371</t>
   </si>
 </sst>
 </file>
@@ -928,7 +931,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1067,6 +1070,45 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1080,7 +1122,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1167,21 +1209,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1197,36 +1227,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1236,6 +1242,27 @@
     <xf numFmtId="17" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1243,12 +1270,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1257,20 +1278,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1281,7 +1308,27 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1978,20 +2025,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2017,20 +2064,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2053,167 +2100,167 @@
       <c r="A5" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="62"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="62"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="51"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="51"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="62"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="51"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="65"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2230,15 +2277,15 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI67"/>
+  <dimension ref="A1:CI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A52" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="56" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="44" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="5" width="22.7109375" customWidth="1"/>
@@ -2281,7 +2328,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:87" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52">
+      <c r="A1" s="42">
         <v>42325</v>
       </c>
       <c r="B1" s="5"/>
@@ -2342,39 +2389,39 @@
       <c r="BV1" s="3"/>
       <c r="BW1" s="3"/>
     </row>
-    <row r="2" spans="1:87" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+    <row r="2" spans="1:87" s="38" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="BY2" s="43"/>
-      <c r="BZ2" s="43"/>
-      <c r="CA2" s="43"/>
-      <c r="CB2" s="43"/>
-      <c r="CC2" s="43"/>
-      <c r="CD2" s="43"/>
-      <c r="CE2" s="43"/>
-      <c r="CF2" s="43"/>
-      <c r="CG2" s="43"/>
-      <c r="CH2" s="43"/>
-      <c r="CI2" s="43"/>
+      <c r="BY2" s="39"/>
+      <c r="BZ2" s="39"/>
+      <c r="CA2" s="39"/>
+      <c r="CB2" s="39"/>
+      <c r="CC2" s="39"/>
+      <c r="CD2" s="39"/>
+      <c r="CE2" s="39"/>
+      <c r="CF2" s="39"/>
+      <c r="CG2" s="39"/>
+      <c r="CH2" s="39"/>
+      <c r="CI2" s="39"/>
     </row>
     <row r="3" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
@@ -2384,7 +2431,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f t="shared" ref="C3:C66" si="0">CONCATENATE(B3,"-",A3)</f>
+        <f t="shared" ref="C3:C58" si="0">CONCATENATE(B3,"-",A3)</f>
         <v>CHMI-ALADIN53</v>
       </c>
       <c r="D3" s="23" t="s">
@@ -2396,7 +2443,7 @@
       <c r="F3" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY3" s="22"/>
@@ -2431,7 +2478,7 @@
       <c r="F4" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY4" s="22"/>
@@ -2466,7 +2513,7 @@
       <c r="F5" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY5" s="22"/>
@@ -2482,7 +2529,7 @@
       <c r="CI5" s="22"/>
     </row>
     <row r="6" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="43" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="17" t="s">
@@ -2501,7 +2548,7 @@
       <c r="F6" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY6" s="22"/>
@@ -2536,7 +2583,7 @@
       <c r="F7" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="34" t="s">
         <v>68</v>
       </c>
       <c r="M7" s="26"/>
@@ -2572,7 +2619,7 @@
       <c r="F8" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY8" s="22"/>
@@ -2607,7 +2654,7 @@
       <c r="F9" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="34" t="s">
         <v>138</v>
       </c>
       <c r="BY9" s="22"/>
@@ -2642,7 +2689,7 @@
       <c r="F10" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY10" s="22"/>
@@ -2677,7 +2724,7 @@
       <c r="F11" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY11" s="22"/>
@@ -2712,7 +2759,7 @@
       <c r="F12" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY12" s="22"/>
@@ -2747,7 +2794,7 @@
       <c r="F13" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY13" s="22"/>
@@ -2782,7 +2829,7 @@
       <c r="F14" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY14" s="22"/>
@@ -2817,7 +2864,7 @@
       <c r="F15" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY15" s="22"/>
@@ -2852,7 +2899,7 @@
       <c r="F16" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G16" s="37" t="s">
+      <c r="G16" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY16" s="22"/>
@@ -2887,7 +2934,7 @@
       <c r="F17" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY17" s="22"/>
@@ -2922,7 +2969,7 @@
       <c r="F18" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY18" s="22"/>
@@ -2957,7 +3004,7 @@
       <c r="F19" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY19" s="22"/>
@@ -2992,7 +3039,7 @@
       <c r="F20" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY20" s="22"/>
@@ -3027,7 +3074,7 @@
       <c r="F21" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY21" s="22"/>
@@ -3062,7 +3109,7 @@
       <c r="F22" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY22" s="22"/>
@@ -3097,7 +3144,7 @@
       <c r="F23" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G23" s="37" t="s">
+      <c r="G23" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY23" s="22"/>
@@ -3113,7 +3160,7 @@
       <c r="CI23" s="22"/>
     </row>
     <row r="24" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="46" t="s">
         <v>219</v>
       </c>
       <c r="B24" s="27" t="s">
@@ -3131,7 +3178,7 @@
       <c r="F24" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY24" s="22"/>
@@ -3166,7 +3213,7 @@
       <c r="F25" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="34" t="s">
         <v>138</v>
       </c>
       <c r="BY25" s="22"/>
@@ -3201,7 +3248,7 @@
       <c r="F26" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="37" t="s">
+      <c r="G26" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY26" s="22"/>
@@ -3236,7 +3283,7 @@
       <c r="F27" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="37" t="s">
+      <c r="G27" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY27" s="22"/>
@@ -3271,7 +3318,7 @@
       <c r="F28" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="37" t="s">
+      <c r="G28" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY28" s="22"/>
@@ -3306,7 +3353,7 @@
       <c r="F29" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY29" s="22"/>
@@ -3341,7 +3388,7 @@
       <c r="F30" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="G30" s="37" t="s">
+      <c r="G30" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY30" s="22"/>
@@ -3376,7 +3423,7 @@
       <c r="F31" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="G31" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY31" s="22"/>
@@ -3411,7 +3458,7 @@
       <c r="F32" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY32" s="22"/>
@@ -3446,7 +3493,7 @@
       <c r="F33" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G33" s="37" t="s">
+      <c r="G33" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY33" s="22"/>
@@ -3481,7 +3528,7 @@
       <c r="F34" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G34" s="37" t="s">
+      <c r="G34" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY34" s="22"/>
@@ -3516,7 +3563,7 @@
       <c r="F35" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G35" s="37" t="s">
+      <c r="G35" s="34" t="s">
         <v>138</v>
       </c>
       <c r="BY35" s="22"/>
@@ -3551,7 +3598,7 @@
       <c r="F36" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G36" s="37" t="s">
+      <c r="G36" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY36" s="22"/>
@@ -3586,7 +3633,7 @@
       <c r="F37" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G37" s="37" t="s">
+      <c r="G37" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY37" s="22"/>
@@ -3621,7 +3668,7 @@
       <c r="F38" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="G38" s="37" t="s">
+      <c r="G38" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY38" s="22"/>
@@ -3656,7 +3703,7 @@
       <c r="F39" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="G39" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY39" s="22"/>
@@ -3691,7 +3738,7 @@
       <c r="F40" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G40" s="37" t="s">
+      <c r="G40" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY40" s="22"/>
@@ -3726,7 +3773,7 @@
       <c r="F41" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G41" s="37" t="s">
+      <c r="G41" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY41" s="22"/>
@@ -3761,7 +3808,7 @@
       <c r="F42" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="G42" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY42" s="22"/>
@@ -3796,7 +3843,7 @@
       <c r="F43" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G43" s="37" t="s">
+      <c r="G43" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY43" s="22"/>
@@ -3831,7 +3878,7 @@
       <c r="F44" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="G44" s="37" t="s">
+      <c r="G44" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY44" s="22"/>
@@ -3866,7 +3913,7 @@
       <c r="F45" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G45" s="37" t="s">
+      <c r="G45" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY45" s="22"/>
@@ -3901,7 +3948,7 @@
       <c r="F46" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G46" s="37" t="s">
+      <c r="G46" s="34" t="s">
         <v>138</v>
       </c>
       <c r="BY46" s="22"/>
@@ -3936,7 +3983,7 @@
       <c r="F47" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="G47" s="37" t="s">
+      <c r="G47" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY47" s="22"/>
@@ -3971,7 +4018,7 @@
       <c r="F48" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="G48" s="37" t="s">
+      <c r="G48" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY48" s="22"/>
@@ -4006,7 +4053,7 @@
       <c r="F49" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G49" s="37" t="s">
+      <c r="G49" s="34" t="s">
         <v>138</v>
       </c>
       <c r="BY49" s="22"/>
@@ -4041,7 +4088,7 @@
       <c r="F50" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="G50" s="37" t="s">
+      <c r="G50" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY50" s="22"/>
@@ -4076,7 +4123,7 @@
       <c r="F51" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G51" s="37" t="s">
+      <c r="G51" s="34" t="s">
         <v>138</v>
       </c>
       <c r="BY51" s="22"/>
@@ -4111,7 +4158,7 @@
       <c r="F52" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="37" t="s">
+      <c r="G52" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY52" s="22"/>
@@ -4126,28 +4173,28 @@
       <c r="CH52" s="22"/>
       <c r="CI52" s="22"/>
     </row>
-    <row r="53" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>55</v>
+    <row r="53" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C53" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AUTH-Met-WRF331A</v>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="E53" s="23" t="s">
-        <v>189</v>
+        <v>120</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>119</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G53" s="37" t="s">
-        <v>138</v>
+        <v>124</v>
+      </c>
+      <c r="G53" s="34" t="s">
+        <v>68</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="BZ53" s="22"/>
@@ -4161,27 +4208,27 @@
       <c r="CH53" s="22"/>
       <c r="CI53" s="22"/>
     </row>
-    <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>16</v>
+    <row r="54" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>60</v>
       </c>
       <c r="C54" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>BCCR-WRF331C</v>
+        <f>CONCATENATE(B54,"-",A54)</f>
+        <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="G54" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G54" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY54" s="22"/>
@@ -4196,28 +4243,28 @@
       <c r="CH54" s="22"/>
       <c r="CI54" s="22"/>
     </row>
-    <row r="55" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="C55" s="18" t="str">
-        <f>CONCATENATE(B55,"-",A55)</f>
-        <v>IPSL-INERIS-WRF331F</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="G55" s="37" t="s">
-        <v>68</v>
+        <v>106</v>
+      </c>
+      <c r="G55" s="34" t="s">
+        <v>140</v>
       </c>
       <c r="BY55" s="22"/>
       <c r="BZ55" s="22"/>
@@ -4232,26 +4279,26 @@
       <c r="CI55" s="22"/>
     </row>
     <row r="56" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
-        <v>53</v>
+      <c r="A56" s="31" t="s">
+        <v>67</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C56" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCAN-WRF331G</v>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F56" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="G56" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G56" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY56" s="22"/>
@@ -4267,26 +4314,26 @@
       <c r="CI56" s="22"/>
     </row>
     <row r="57" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>24</v>
+      <c r="A57" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C57" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>NUIM-WRF341E</v>
+        <f>CONCATENATE(B57,"-",A57)</f>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="F57" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G57" s="37" t="s">
+      <c r="G57" s="34" t="s">
         <v>140</v>
       </c>
       <c r="BY57" s="22"/>
@@ -4302,27 +4349,27 @@
       <c r="CI57" s="22"/>
     </row>
     <row r="58" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>17</v>
+      <c r="A58" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="C58" s="18" t="str">
-        <f>CONCATENATE(B58,"-",A58)</f>
-        <v>IDL-WRF350D</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF350I</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="F58" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G58" s="37" t="s">
-        <v>140</v>
+      <c r="G58" s="34" t="s">
+        <v>138</v>
       </c>
       <c r="BY58" s="22"/>
       <c r="BZ58" s="22"/>
@@ -4336,28 +4383,28 @@
       <c r="CH58" s="22"/>
       <c r="CI58" s="22"/>
     </row>
-    <row r="59" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="C59" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF350I</v>
+        <f t="shared" ref="C59" si="4">CONCATENATE(B59,"-",A59)</f>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>182</v>
+        <v>116</v>
+      </c>
+      <c r="E59" s="40" t="s">
+        <v>117</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G59" s="37" t="s">
-        <v>138</v>
+        <v>118</v>
+      </c>
+      <c r="G59" s="34" t="s">
+        <v>115</v>
       </c>
       <c r="BY59" s="22"/>
       <c r="BZ59" s="22"/>
@@ -4373,25 +4420,25 @@
     </row>
     <row r="60" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B60" s="17" t="s">
         <v>141</v>
       </c>
       <c r="C60" s="18" t="str">
-        <f t="shared" ref="C60" si="4">CONCATENATE(B60,"-",A60)</f>
-        <v>UNSW-WRF360J</v>
+        <f>CONCATENATE(B60,"-",A60)</f>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D60" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="49" t="s">
+      <c r="E60" s="40" t="s">
         <v>117</v>
       </c>
       <c r="F60" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="G60" s="37" t="s">
+      <c r="G60" s="34" t="s">
         <v>115</v>
       </c>
       <c r="BY60" s="22"/>
@@ -4408,25 +4455,25 @@
     </row>
     <row r="61" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>141</v>
       </c>
       <c r="C61" s="18" t="str">
-        <f>CONCATENATE(B61,"-",A61)</f>
-        <v>UNSW-WRF360K</v>
+        <f t="shared" ref="C61" si="5">CONCATENATE(B61,"-",A61)</f>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D61" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="E61" s="49" t="s">
+      <c r="E61" s="40" t="s">
         <v>117</v>
       </c>
       <c r="F61" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="G61" s="37" t="s">
+      <c r="G61" s="34" t="s">
         <v>115</v>
       </c>
       <c r="BY61" s="22"/>
@@ -4441,28 +4488,28 @@
       <c r="CH61" s="22"/>
       <c r="CI61" s="22"/>
     </row>
-    <row r="62" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C62" s="18" t="str">
-        <f t="shared" ref="C62" si="5">CONCATENATE(B62,"-",A62)</f>
-        <v>UNSW-WRF360L</v>
+        <f>CONCATENATE(B62,"-",A62)</f>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="E62" s="49" t="s">
-        <v>117</v>
+        <v>132</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="G62" s="37" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="G62" s="34" t="s">
+        <v>140</v>
       </c>
       <c r="BY62" s="22"/>
       <c r="BZ62" s="22"/>
@@ -4476,28 +4523,28 @@
       <c r="CH62" s="22"/>
       <c r="CI62" s="22"/>
     </row>
-    <row r="63" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>133</v>
+    <row r="63" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C63" s="18" t="str">
-        <f>CONCATENATE(B63,"-",A63)</f>
-        <v>MU-WRF360M</v>
+        <f t="shared" ref="C63" si="6">CONCATENATE(B63,"-",A63)</f>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>131</v>
+        <v>120</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>119</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G63" s="37" t="s">
-        <v>140</v>
+        <v>123</v>
+      </c>
+      <c r="G63" s="34" t="s">
+        <v>68</v>
       </c>
       <c r="BY63" s="22"/>
       <c r="BZ63" s="22"/>
@@ -4511,27 +4558,27 @@
       <c r="CH63" s="22"/>
       <c r="CI63" s="22"/>
     </row>
-    <row r="64" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>16</v>
+    <row r="64" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>60</v>
       </c>
       <c r="C64" s="18" t="str">
-        <f t="shared" ref="C64" si="6">CONCATENATE(B64,"-",A64)</f>
-        <v>BCCR-WRF361</v>
+        <f>CONCATENATE(B64,"-",A64)</f>
+        <v>IPSL-INERIS-WRF361F</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="G64" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G64" s="34" t="s">
         <v>68</v>
       </c>
       <c r="BY64" s="22"/>
@@ -4546,28 +4593,28 @@
       <c r="CH64" s="22"/>
       <c r="CI64" s="22"/>
     </row>
-    <row r="65" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="B65" s="25" t="s">
-        <v>60</v>
+    <row r="65" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="C65" s="18" t="str">
         <f>CONCATENATE(B65,"-",A65)</f>
-        <v>IPSL-INERIS-WRF361F</v>
+        <v>UHOH-WRF361H</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>160</v>
+        <v>87</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="G65" s="37" t="s">
-        <v>68</v>
+        <v>89</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>139</v>
       </c>
       <c r="BY65" s="22"/>
       <c r="BZ65" s="22"/>
@@ -4581,28 +4628,28 @@
       <c r="CH65" s="22"/>
       <c r="CI65" s="22"/>
     </row>
-    <row r="66" spans="1:87" s="21" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>UHOH-WRF361H</v>
-      </c>
-      <c r="D66" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E66" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="F66" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G66" s="38" t="s">
-        <v>139</v>
+    <row r="66" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="B66" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C66" s="61" t="str">
+        <f>CONCATENATE(B66,"-",A66)</f>
+        <v>AUTH-Met-WRF371</v>
+      </c>
+      <c r="D66" s="62" t="s">
+        <v>190</v>
+      </c>
+      <c r="E66" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="F66" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="G66" s="64" t="s">
+        <v>68</v>
       </c>
       <c r="BY66" s="22"/>
       <c r="BZ66" s="22"/>
@@ -4616,205 +4663,190 @@
       <c r="CH66" s="22"/>
       <c r="CI66" s="22"/>
     </row>
-    <row r="67" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="55"/>
-      <c r="B67" s="44"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="47"/>
-      <c r="BY67" s="22"/>
-      <c r="BZ67" s="22"/>
-      <c r="CA67" s="22"/>
-      <c r="CB67" s="22"/>
-      <c r="CC67" s="22"/>
-      <c r="CD67" s="22"/>
-      <c r="CE67" s="22"/>
-      <c r="CF67" s="22"/>
-      <c r="CG67" s="22"/>
-      <c r="CH67" s="22"/>
-      <c r="CI67" s="22"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="E36:E37 F52:G52 A66:C67 B63:C63 E66:G67 E63:G63 B3:C15 A46:C46 F51 F53 F59 C17 F58:G58 E56:E59 A17:A22 F17:G22 E19:E22 B20:C45 F44:F46 G37:G39 F49 A49:C49 E54:G54 A25:A44 E39 A51:C54 A56:C59 E56:G57 E41:E43 G41:G44">
-    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E36:E37 F52:G52 B62:C62 E62:G62 B3:C15 A46:C46 F51 F58 C17 F57:G57 E55:E58 A17:A22 F17:G22 E19:E22 B20:C45 F44:F46 G37:G39 F49 A49:C49 E53:G53 A25:A44 E39 A55:C58 E55:G56 E41:E43 G41:G44 A65:C65 E65:G65 A51:C53">
+    <cfRule type="containsText" dxfId="36" priority="44" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A15 G35 F15:G15 E23:G34 E3:G14">
-    <cfRule type="containsText" dxfId="36" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="35" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="46" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F43">
-    <cfRule type="containsText" dxfId="34" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F62:G62 B62:C62">
-    <cfRule type="containsText" dxfId="33" priority="40" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F61:G61 B61:C61">
-    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B61)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F60:G60 A60:C60">
-    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="F60:G60 B60:C60">
+    <cfRule type="containsText" dxfId="31" priority="42" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F59:G59 A59:C59">
+    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:C50 E50:G50">
+    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:C63 E63:G63">
+    <cfRule type="containsText" dxfId="28" priority="39" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="containsText" dxfId="27" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:C50 E50:G50">
-    <cfRule type="containsText" dxfId="30" priority="37" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64:C64 E64:G64">
-    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
-    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="25" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46 G49">
-    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="34" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="23" priority="30" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G59">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G59)))</formula>
+  <conditionalFormatting sqref="G58">
+    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E59)))</formula>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="19" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:C47 E47:G47">
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65:C65 E65:G65">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A65)))</formula>
+  <conditionalFormatting sqref="A64:C64 E64:G64">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55:C55 E55:G55">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
+  <conditionalFormatting sqref="A54:C54 E54:G54">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F66 A66:C66">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Filling out ToU information
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="225">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>MIUB</t>
-  </si>
-  <si>
-    <t>AUTH-Met</t>
   </si>
   <si>
     <t>AUTH-LHTEE</t>
@@ -731,6 +728,12 @@
   </si>
   <si>
     <t>WRF371</t>
+  </si>
+  <si>
+    <t>"EUR-44 SAM-44 AFR-44"</t>
+  </si>
+  <si>
+    <t>AUTH-MC</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1125,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1242,6 +1245,51 @@
     <xf numFmtId="17" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1251,53 +1299,11 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1308,37 +1314,7 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2025,20 +2001,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
+      <c r="A1" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2064,25 +2040,25 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
+      <c r="A3" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -2098,129 +2074,129 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="53"/>
+        <v>110</v>
+      </c>
+      <c r="B5" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
+      <c r="B6" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="51"/>
+      <c r="B7" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
+        <v>91</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
+        <v>70</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="51"/>
+        <v>92</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+        <v>93</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="61"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
+      <c r="A13" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2235,32 +2211,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
+      <c r="A15" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2279,8 +2255,8 @@
   </sheetPr>
   <dimension ref="A1:CI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A52" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2367,7 @@
     </row>
     <row r="2" spans="1:87" s="38" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>28</v>
@@ -2400,16 +2376,16 @@
         <v>27</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="37" t="s">
         <v>99</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>100</v>
       </c>
       <c r="BY2" s="39"/>
       <c r="BZ2" s="39"/>
@@ -2425,7 +2401,7 @@
     </row>
     <row r="3" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>14</v>
@@ -2438,13 +2414,13 @@
         <v>29</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY3" s="22"/>
       <c r="BZ3" s="22"/>
@@ -2473,13 +2449,13 @@
         <v>48</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY4" s="22"/>
       <c r="BZ4" s="22"/>
@@ -2505,16 +2481,16 @@
         <v>CNRM-ALADIN52</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E5" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>201</v>
-      </c>
       <c r="G5" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY5" s="22"/>
       <c r="BZ5" s="22"/>
@@ -2530,7 +2506,7 @@
     </row>
     <row r="6" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>13</v>
@@ -2540,16 +2516,16 @@
         <v>CNRM-ALADIN53</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY6" s="22"/>
       <c r="BZ6" s="22"/>
@@ -2575,16 +2551,16 @@
         <v>CNRM-ARPEGE52</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M7" s="26"/>
       <c r="BY7" s="22"/>
@@ -2611,16 +2587,16 @@
         <v>CCCma-CanRCM4</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY8" s="22"/>
       <c r="BZ8" s="22"/>
@@ -2639,23 +2615,23 @@
         <v>6</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CSIRO-CCAM</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>85</v>
+      <c r="D9" s="54" t="s">
+        <v>84</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BY9" s="22"/>
       <c r="BZ9" s="22"/>
@@ -2681,16 +2657,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY10" s="22"/>
       <c r="BZ10" s="22"/>
@@ -2716,16 +2692,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY11" s="22"/>
       <c r="BZ11" s="22"/>
@@ -2751,16 +2727,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY12" s="22"/>
       <c r="BZ12" s="22"/>
@@ -2786,16 +2762,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY13" s="22"/>
       <c r="BZ13" s="22"/>
@@ -2821,16 +2797,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY14" s="22"/>
       <c r="BZ14" s="22"/>
@@ -2856,16 +2832,16 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY15" s="22"/>
       <c r="BZ15" s="22"/>
@@ -2884,23 +2860,23 @@
         <v>30</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="18" t="str">
         <f t="shared" ref="C16" si="1">CONCATENATE(B16,"-",A16)</f>
         <v>OURANOS-CRCM5</v>
       </c>
       <c r="D16" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>174</v>
-      </c>
       <c r="F16" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY16" s="22"/>
       <c r="BZ16" s="22"/>
@@ -2926,16 +2902,16 @@
         <v>UQAM-CRCM5</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY17" s="22"/>
       <c r="BZ17" s="22"/>
@@ -2951,26 +2927,26 @@
     </row>
     <row r="18" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UNIBELGRADE-EBU1</v>
       </c>
       <c r="D18" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="F18" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="F18" s="20" t="s">
-        <v>170</v>
-      </c>
       <c r="G18" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY18" s="22"/>
       <c r="BZ18" s="22"/>
@@ -2986,26 +2962,26 @@
     </row>
     <row r="19" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>166</v>
       </c>
       <c r="C19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UNIBELGRADE-EBUPOM2c1</v>
       </c>
       <c r="D19" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="F19" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="F19" s="20" t="s">
-        <v>170</v>
-      </c>
       <c r="G19" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY19" s="22"/>
       <c r="BZ19" s="22"/>
@@ -3031,16 +3007,16 @@
         <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY20" s="22"/>
       <c r="BZ20" s="22"/>
@@ -3069,13 +3045,13 @@
         <v>34</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY21" s="22"/>
       <c r="BZ21" s="22"/>
@@ -3101,16 +3077,16 @@
         <v>DMI-HIRHAM5</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY22" s="22"/>
       <c r="BZ22" s="22"/>
@@ -3139,13 +3115,13 @@
         <v>35</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY23" s="22"/>
       <c r="BZ23" s="22"/>
@@ -3161,25 +3137,25 @@
     </row>
     <row r="24" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B24" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="D24" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="E24" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="F24" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="F24" s="20" t="s">
-        <v>218</v>
-      </c>
       <c r="G24" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY24" s="22"/>
       <c r="BZ24" s="22"/>
@@ -3205,16 +3181,16 @@
         <v>UCLM-PROMES</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="BY25" s="22"/>
       <c r="BZ25" s="22"/>
@@ -3243,13 +3219,13 @@
         <v>42</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY26" s="22"/>
       <c r="BZ26" s="22"/>
@@ -3265,7 +3241,7 @@
     </row>
     <row r="27" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>22</v>
@@ -3278,13 +3254,13 @@
         <v>42</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY27" s="22"/>
       <c r="BZ27" s="22"/>
@@ -3313,13 +3289,13 @@
         <v>42</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY28" s="22"/>
       <c r="BZ28" s="22"/>
@@ -3348,13 +3324,13 @@
         <v>26</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY29" s="22"/>
       <c r="BZ29" s="22"/>
@@ -3380,16 +3356,16 @@
         <v>SMHI-RCA4-SN</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY30" s="22"/>
       <c r="BZ30" s="22"/>
@@ -3415,16 +3391,16 @@
         <v>SMHI-RCAO</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G31" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY31" s="22"/>
       <c r="BZ31" s="22"/>
@@ -3440,7 +3416,7 @@
     </row>
     <row r="32" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>13</v>
@@ -3450,16 +3426,16 @@
         <v>CNRM-RCSM4</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY32" s="22"/>
       <c r="BZ32" s="22"/>
@@ -3485,16 +3461,16 @@
         <v>SMHI-RCAO-SN</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G33" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY33" s="22"/>
       <c r="BZ33" s="22"/>
@@ -3510,26 +3486,26 @@
     </row>
     <row r="34" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" s="18" t="str">
         <f t="shared" si="0"/>
         <v>IITM-RegCM4-1</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY34" s="22"/>
       <c r="BZ34" s="22"/>
@@ -3555,16 +3531,16 @@
         <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BY35" s="22"/>
       <c r="BZ35" s="22"/>
@@ -3590,16 +3566,16 @@
         <v>DHMZ-RegCM4-2</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY36" s="22"/>
       <c r="BZ36" s="22"/>
@@ -3625,16 +3601,16 @@
         <v>ICTP-RegCM4-3</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY37" s="22"/>
       <c r="BZ37" s="22"/>
@@ -3660,16 +3636,16 @@
         <v>UM-RegCM4-3</v>
       </c>
       <c r="D38" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="E38" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="F38" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="F38" s="20" t="s">
-        <v>209</v>
-      </c>
       <c r="G38" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY38" s="22"/>
       <c r="BZ38" s="22"/>
@@ -3688,23 +3664,23 @@
         <v>32</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" s="18" t="str">
         <f t="shared" si="0"/>
         <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY39" s="22"/>
       <c r="BZ39" s="22"/>
@@ -3723,23 +3699,23 @@
         <v>45</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C40" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-REMO2009</v>
       </c>
       <c r="D40" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="E40" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="E40" s="19" t="s">
-        <v>222</v>
-      </c>
       <c r="F40" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY40" s="22"/>
       <c r="BZ40" s="22"/>
@@ -3765,16 +3741,16 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY41" s="22"/>
       <c r="BZ41" s="22"/>
@@ -3800,16 +3776,16 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY42" s="22"/>
       <c r="BZ42" s="22"/>
@@ -3835,16 +3811,16 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY43" s="22"/>
       <c r="BZ43" s="22"/>
@@ -3860,26 +3836,26 @@
     </row>
     <row r="44" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C44" s="18" t="str">
         <f t="shared" si="0"/>
         <v>RMIB-Ugent-ALARO-0</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY44" s="22"/>
       <c r="BZ44" s="22"/>
@@ -3895,26 +3871,26 @@
     </row>
     <row r="45" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C45" s="18" t="str">
         <f>CONCATENATE(B45,"-",A45)</f>
         <v>MGO-RRCM</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY45" s="22"/>
       <c r="BZ45" s="22"/>
@@ -3930,26 +3906,26 @@
     </row>
     <row r="46" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="18" t="str">
         <f t="shared" si="0"/>
         <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BY46" s="22"/>
       <c r="BZ46" s="22"/>
@@ -3965,26 +3941,26 @@
     </row>
     <row r="47" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C47" s="18" t="str">
         <f>CONCATENATE(B47,"-",A47)</f>
         <v>IPSL-WRF311</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G47" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY47" s="22"/>
       <c r="BZ47" s="22"/>
@@ -4000,26 +3976,26 @@
     </row>
     <row r="48" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C48" s="18" t="str">
         <f t="shared" ref="C48" si="2">CONCATENATE(B48,"-",A48)</f>
         <v>IPSL-WRF311NEMO</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G48" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY48" s="22"/>
       <c r="BZ48" s="22"/>
@@ -4045,16 +4021,16 @@
         <v>UM-WRF331</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G49" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BY49" s="22"/>
       <c r="BZ49" s="22"/>
@@ -4080,16 +4056,16 @@
         <v>BCCR-WRF331</v>
       </c>
       <c r="D50" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E50" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F50" s="20" t="s">
-        <v>121</v>
-      </c>
       <c r="G50" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY50" s="22"/>
       <c r="BZ50" s="22"/>
@@ -4115,16 +4091,16 @@
         <v>MIUB-WRF331A</v>
       </c>
       <c r="D51" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E51" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E51" s="24" t="s">
-        <v>187</v>
-      </c>
       <c r="F51" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G51" s="34" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="BY51" s="22"/>
       <c r="BZ51" s="22"/>
@@ -4150,16 +4126,16 @@
         <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G52" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY52" s="22"/>
       <c r="BZ52" s="22"/>
@@ -4185,16 +4161,16 @@
         <v>BCCR-WRF331C</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="BZ53" s="22"/>
@@ -4210,26 +4186,26 @@
     </row>
     <row r="54" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" s="18" t="str">
         <f>CONCATENATE(B54,"-",A54)</f>
         <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY54" s="22"/>
       <c r="BZ54" s="22"/>
@@ -4255,16 +4231,16 @@
         <v>UCAN-WRF331G</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY55" s="22"/>
       <c r="BZ55" s="22"/>
@@ -4280,7 +4256,7 @@
     </row>
     <row r="56" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>24</v>
@@ -4290,16 +4266,16 @@
         <v>NUIM-WRF341E</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G56" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY56" s="22"/>
       <c r="BZ56" s="22"/>
@@ -4315,7 +4291,7 @@
     </row>
     <row r="57" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57" s="25" t="s">
         <v>17</v>
@@ -4325,16 +4301,16 @@
         <v>IDL-WRF350D</v>
       </c>
       <c r="D57" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="E57" s="19" t="s">
-        <v>177</v>
-      </c>
       <c r="F57" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY57" s="22"/>
       <c r="BZ57" s="22"/>
@@ -4350,7 +4326,7 @@
     </row>
     <row r="58" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>52</v>
@@ -4360,16 +4336,16 @@
         <v>UCAN-WRF350I</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>110</v>
+        <v>223</v>
       </c>
       <c r="G58" s="34" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="BY58" s="22"/>
       <c r="BZ58" s="22"/>
@@ -4385,26 +4361,26 @@
     </row>
     <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C59" s="18" t="str">
         <f t="shared" ref="C59" si="4">CONCATENATE(B59,"-",A59)</f>
         <v>UNSW-WRF360J</v>
       </c>
       <c r="D59" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="E59" s="40" t="s">
+      <c r="F59" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F59" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="G59" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BY59" s="22"/>
       <c r="BZ59" s="22"/>
@@ -4420,26 +4396,26 @@
     </row>
     <row r="60" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C60" s="18" t="str">
         <f>CONCATENATE(B60,"-",A60)</f>
         <v>UNSW-WRF360K</v>
       </c>
       <c r="D60" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E60" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="E60" s="40" t="s">
+      <c r="F60" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F60" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="G60" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BY60" s="22"/>
       <c r="BZ60" s="22"/>
@@ -4455,26 +4431,26 @@
     </row>
     <row r="61" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C61" s="18" t="str">
         <f t="shared" ref="C61" si="5">CONCATENATE(B61,"-",A61)</f>
         <v>UNSW-WRF360L</v>
       </c>
       <c r="D61" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E61" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="E61" s="40" t="s">
+      <c r="F61" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F61" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="G61" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BY61" s="22"/>
       <c r="BZ61" s="22"/>
@@ -4490,26 +4466,26 @@
     </row>
     <row r="62" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C62" s="18" t="str">
         <f>CONCATENATE(B62,"-",A62)</f>
         <v>MU-WRF360M</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G62" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BY62" s="22"/>
       <c r="BZ62" s="22"/>
@@ -4525,7 +4501,7 @@
     </row>
     <row r="63" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B63" s="29" t="s">
         <v>16</v>
@@ -4535,16 +4511,16 @@
         <v>BCCR-WRF361</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E63" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY63" s="22"/>
       <c r="BZ63" s="22"/>
@@ -4560,26 +4536,26 @@
     </row>
     <row r="64" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C64" s="18" t="str">
         <f>CONCATENATE(B64,"-",A64)</f>
         <v>IPSL-INERIS-WRF361F</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BY64" s="22"/>
       <c r="BZ64" s="22"/>
@@ -4594,8 +4570,8 @@
       <c r="CI64" s="22"/>
     </row>
     <row r="65" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="65" t="s">
-        <v>88</v>
+      <c r="A65" s="53" t="s">
+        <v>87</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>9</v>
@@ -4605,16 +4581,16 @@
         <v>UHOH-WRF361H</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY65" s="22"/>
       <c r="BZ65" s="22"/>
@@ -4629,27 +4605,27 @@
       <c r="CI65" s="22"/>
     </row>
     <row r="66" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="59" t="s">
-        <v>223</v>
-      </c>
-      <c r="B66" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="C66" s="61" t="str">
+      <c r="A66" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="B66" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="C66" s="49" t="str">
         <f>CONCATENATE(B66,"-",A66)</f>
-        <v>AUTH-Met-WRF371</v>
-      </c>
-      <c r="D66" s="62" t="s">
-        <v>190</v>
-      </c>
-      <c r="E66" s="62" t="s">
+        <v>AUTH-MC-WRF371</v>
+      </c>
+      <c r="D66" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="F66" s="63" t="s">
-        <v>106</v>
-      </c>
-      <c r="G66" s="64" t="s">
-        <v>68</v>
+      <c r="E66" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F66" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="G66" s="52" t="s">
+        <v>67</v>
       </c>
       <c r="BY66" s="22"/>
       <c r="BZ66" s="22"/>
@@ -4665,197 +4641,198 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E36:E37 F52:G52 B62:C62 E62:G62 B3:C15 A46:C46 F51 F58 C17 F57:G57 E55:E58 A17:A22 F17:G22 E19:E22 B20:C45 F44:F46 G37:G39 F49 A49:C49 E53:G53 A25:A44 E39 A55:C58 E55:G56 E41:E43 G41:G44 A65:C65 E65:G65 A51:C53">
-    <cfRule type="containsText" dxfId="36" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A15 G35 F15:G15 E23:G34 E3:G14">
-    <cfRule type="containsText" dxfId="35" priority="47" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A3:A15 G35 F15:G15 E3:G14 E23:G34">
+    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="containsText" dxfId="34" priority="46" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="48" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F43">
-    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61:G61 B61:C61">
-    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:G60 B60:C60">
-    <cfRule type="containsText" dxfId="31" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="44" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:G59 A59:C59">
-    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:C50 E50:G50">
-    <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:C63 E63:G63">
-    <cfRule type="containsText" dxfId="28" priority="39" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="41" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="27" priority="38" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="40" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="26" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="39" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="25" priority="36" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46 G49">
-    <cfRule type="containsText" dxfId="23" priority="34" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G46)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
-    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="20" priority="29" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="13" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:C47 E47:G47">
-    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64:C64 E64:G64">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66 A66:C66">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G51">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G66)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D47" r:id="rId1"/>
     <hyperlink ref="D48" r:id="rId2"/>
     <hyperlink ref="D38" r:id="rId3" display="javascript:_e(%7B%7D,'cvml','ambrya@umich.edu');"/>
+    <hyperlink ref="D9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ToU added for CCAM
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -1269,6 +1269,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1276,33 +1297,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1314,7 +1314,17 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2001,20 +2011,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2040,20 +2050,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2076,127 +2086,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="61"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2211,32 +2221,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2255,8 +2265,8 @@
   </sheetPr>
   <dimension ref="A1:CI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2631,7 +2641,7 @@
         <v>109</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="BY9" s="22"/>
       <c r="BZ9" s="22"/>
@@ -4641,187 +4651,187 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E36:E37 F52:G52 B62:C62 E62:G62 B3:C15 A46:C46 F51 F58 C17 F57:G57 E55:E58 A17:A22 F17:G22 E19:E22 B20:C45 F44:F46 G37:G39 F49 A49:C49 E53:G53 A25:A44 E39 A55:C58 E55:G56 E41:E43 G41:G44 A65:C65 E65:G65 A51:C53">
-    <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="37" priority="46" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A15 G35 F15:G15 E3:G14 E23:G34">
-    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A3:A15 G35 F15:G15 E23:G34 E3:G14">
+    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="containsText" dxfId="34" priority="48" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F43">
-    <cfRule type="containsText" dxfId="33" priority="47" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61:G61 B61:C61">
-    <cfRule type="containsText" dxfId="32" priority="45" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:G60 B60:C60">
-    <cfRule type="containsText" dxfId="31" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:G59 A59:C59">
-    <cfRule type="containsText" dxfId="30" priority="43" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:C50 E50:G50">
-    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:C63 E63:G63">
-    <cfRule type="containsText" dxfId="28" priority="41" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="41" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="27" priority="40" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="40" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="26" priority="39" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="25" priority="38" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="24" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46 G49">
-    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="22" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:C47 E47:G47">
-    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64:C64 E64:G64">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66 A66:C66">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
All CCLM simulations now have unrestricted access
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="315" windowWidth="22320" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="315" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="7" r:id="rId1"/>
@@ -1269,6 +1269,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1278,31 +1299,10 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1314,7 +1314,17 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2011,20 +2021,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2050,20 +2060,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2086,127 +2096,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="59"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="59"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="59"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="59"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="66"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="61"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2221,32 +2231,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2265,8 +2275,8 @@
   </sheetPr>
   <dimension ref="A1:CI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,7 +2686,7 @@
         <v>101</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY10" s="22"/>
       <c r="BZ10" s="22"/>
@@ -2711,7 +2721,7 @@
         <v>109</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY11" s="22"/>
       <c r="BZ11" s="22"/>
@@ -2746,7 +2756,7 @@
         <v>109</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY12" s="22"/>
       <c r="BZ12" s="22"/>
@@ -2781,7 +2791,7 @@
         <v>109</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY13" s="22"/>
       <c r="BZ13" s="22"/>
@@ -2816,7 +2826,7 @@
         <v>109</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY14" s="22"/>
       <c r="BZ14" s="22"/>
@@ -2851,7 +2861,7 @@
         <v>109</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY15" s="22"/>
       <c r="BZ15" s="22"/>
@@ -4651,188 +4661,193 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E36:E37 F52:G52 B62:C62 E62:G62 B3:C15 A46:C46 F51 F58 C17 F57:G57 E55:E58 A17:A22 F17:G22 E19:E22 B20:C45 F44:F46 G37:G39 F49 A49:C49 E53:G53 A25:A44 E39 A55:C58 E55:G56 E41:E43 G41:G44 A65:C65 E65:G65 A51:C53">
-    <cfRule type="containsText" dxfId="37" priority="46" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="38" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A15 G35 F15:G15 E23:G34 E3:G14">
-    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A3:A15 G35 F15 E23:G34 E3:G10 E11:F14">
+    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F43">
-    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61:G61 B61:C61">
-    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="46" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:G60 B60:C60">
-    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:G59 A59:C59">
-    <cfRule type="containsText" dxfId="31" priority="43" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:C50 E50:G50">
-    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:C63 E63:G63">
-    <cfRule type="containsText" dxfId="29" priority="41" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="28" priority="40" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="41" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="40" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="26" priority="38" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46 G49">
-    <cfRule type="containsText" dxfId="24" priority="36" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="32" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:C47 E47:G47">
-    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64:C64 E64:G64">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66 A66:C66">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G15">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Update of ToU for Universidad de Murcia
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -1269,6 +1269,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1276,33 +1297,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1314,7 +1314,17 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2021,20 +2031,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2060,20 +2070,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2096,127 +2106,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="61"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2231,32 +2241,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2275,8 +2285,8 @@
   </sheetPr>
   <dimension ref="A1:CI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4047,10 +4057,10 @@
         <v>192</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G49" s="34" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="BY49" s="22"/>
       <c r="BZ49" s="22"/>
@@ -4661,193 +4671,198 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E36:E37 F52:G52 B62:C62 E62:G62 B3:C15 A46:C46 F51 F58 C17 F57:G57 E55:E58 A17:A22 F17:G22 E19:E22 B20:C45 F44:F46 G37:G39 F49 A49:C49 E53:G53 A25:A44 E39 A55:C58 E55:G56 E41:E43 G41:G44 A65:C65 E65:G65 A51:C53">
-    <cfRule type="containsText" dxfId="38" priority="47" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="39" priority="48" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A15 G35 F15 E23:G34 E3:G10 E11:F14">
-    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="38" priority="51" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F43">
-    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61:G61 B61:C61">
-    <cfRule type="containsText" dxfId="34" priority="46" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="35" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:G60 B60:C60">
-    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="46" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:G59 A59:C59">
-    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:C50 E50:G50">
-    <cfRule type="containsText" dxfId="31" priority="43" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:C63 E63:G63">
-    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="containsText" dxfId="29" priority="41" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="28" priority="40" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="41" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="40" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="26" priority="38" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="39" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G46 G49">
-    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="G46">
+    <cfRule type="containsText" dxfId="26" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="24" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:G16 A16">
-    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B19">
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:C47 E47:G47">
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64:C64 E64:G64">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66 A66:C66">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G15">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G49">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Added CRCM5-SN, spectrally nudged version of UQAM CRCM5
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -33,7 +33,7 @@
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AU$1</definedName>
     <definedName name="Print_Area" localSheetId="0">ReadMe!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="231">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>"MENA"</t>
+  </si>
+  <si>
+    <t>CRCM5-SN</t>
   </si>
 </sst>
 </file>
@@ -1284,6 +1287,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1291,33 +1315,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2066,20 +2069,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2105,20 +2108,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2141,127 +2144,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="61"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2276,32 +2279,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2318,10 +2321,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI67"/>
+  <dimension ref="A1:CI68"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,7 +2475,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f t="shared" ref="C3:C59" si="0">CONCATENATE(B3,"-",A3)</f>
+        <f t="shared" ref="C3:C60" si="0">CONCATENATE(B3,"-",A3)</f>
         <v>CHMI-ALADIN53</v>
       </c>
       <c r="D3" s="23" t="s">
@@ -2990,28 +2993,26 @@
       <c r="CH17" s="22"/>
       <c r="CI17" s="22"/>
     </row>
-    <row r="18" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="C18" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UNIBELGRADE-EBU1</v>
+        <v>UQAM-CRCM5-SN</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>169</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F18" s="20"/>
       <c r="G18" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY18" s="22"/>
       <c r="BZ18" s="22"/>
@@ -3027,14 +3028,14 @@
     </row>
     <row r="19" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>165</v>
       </c>
       <c r="C19" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UNIBELGRADE-EBUPOM2c1</v>
+        <v>UNIBELGRADE-EBU1</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>167</v>
@@ -3060,28 +3061,28 @@
       <c r="CH19" s="22"/>
       <c r="CI19" s="22"/>
     </row>
-    <row r="20" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>39</v>
+    <row r="20" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>164</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="C20" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MOHC-HadGEM3-RA</v>
+        <v>UNIBELGRADE-EBUPOM2c1</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>72</v>
+        <v>168</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY20" s="22"/>
       <c r="BZ20" s="22"/>
@@ -3097,23 +3098,23 @@
     </row>
     <row r="21" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MOHC-HadRM3P</v>
+        <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="19" t="s">
-        <v>108</v>
+      <c r="F21" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G21" s="34" t="s">
         <v>67</v>
@@ -3132,23 +3133,23 @@
     </row>
     <row r="22" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="C22" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DMI-HIRHAM5</v>
+        <v>MOHC-HadRM3P</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>171</v>
+        <v>34</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>177</v>
+        <v>72</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="G22" s="34" t="s">
         <v>67</v>
@@ -3165,25 +3166,25 @@
       <c r="CH22" s="22"/>
       <c r="CI22" s="22"/>
     </row>
-    <row r="23" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C23" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AWI-HIRHAM5</v>
+        <v>DMI-HIRHAM5</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>35</v>
+        <v>171</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>67</v>
@@ -3200,24 +3201,25 @@
       <c r="CH23" s="22"/>
       <c r="CI23" s="22"/>
     </row>
-    <row r="24" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
-        <v>218</v>
+    <row r="24" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>0</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>214</v>
+        <v>36</v>
+      </c>
+      <c r="C24" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>AWI-HIRHAM5</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>215</v>
+        <v>35</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>216</v>
+        <v>74</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>217</v>
+        <v>109</v>
       </c>
       <c r="G24" s="34" t="s">
         <v>67</v>
@@ -3235,24 +3237,23 @@
       <c r="CI24" s="22"/>
     </row>
     <row r="25" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCLM-PROMES</v>
+      <c r="A25" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>214</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>163</v>
+        <v>215</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>63</v>
+        <v>216</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>109</v>
+        <v>217</v>
       </c>
       <c r="G25" s="34" t="s">
         <v>67</v>
@@ -3269,25 +3270,25 @@
       <c r="CH25" s="22"/>
       <c r="CI25" s="22"/>
     </row>
-    <row r="26" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>22</v>
+    <row r="26" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C26" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO21P</v>
+        <v>UCLM-PROMES</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>61</v>
+        <v>163</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>67</v>
@@ -3306,14 +3307,14 @@
     </row>
     <row r="27" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO22E</v>
+        <v>KNMI-RACMO21P</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>42</v>
@@ -3322,7 +3323,7 @@
         <v>61</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G27" s="34" t="s">
         <v>67</v>
@@ -3341,14 +3342,14 @@
     </row>
     <row r="28" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO22T</v>
+        <v>KNMI-RACMO22E</v>
       </c>
       <c r="D28" s="23" t="s">
         <v>42</v>
@@ -3357,7 +3358,7 @@
         <v>61</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G28" s="34" t="s">
         <v>67</v>
@@ -3375,24 +3376,24 @@
       <c r="CI28" s="22"/>
     </row>
     <row r="29" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>15</v>
+      <c r="A29" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="C29" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCA4</v>
+        <v>KNMI-RACMO22T</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>62</v>
+        <v>42</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>61</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G29" s="34" t="s">
         <v>67</v>
@@ -3411,23 +3412,23 @@
     </row>
     <row r="30" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="B30" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCA4-SN</v>
+        <v>SMHI-RCA4</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>162</v>
+        <v>26</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="28" t="s">
-        <v>103</v>
+      <c r="F30" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="G30" s="34" t="s">
         <v>67</v>
@@ -3446,14 +3447,14 @@
     </row>
     <row r="31" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO</v>
+        <v>SMHI-RCA4-SN</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>162</v>
@@ -3461,8 +3462,8 @@
       <c r="E31" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="20" t="s">
-        <v>109</v>
+      <c r="F31" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="G31" s="34" t="s">
         <v>67</v>
@@ -3481,26 +3482,26 @@
     </row>
     <row r="32" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>198</v>
+        <v>37</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C32" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CNRM-RCSM4</v>
+        <v>SMHI-RCAO</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>199</v>
+        <v>62</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY32" s="22"/>
       <c r="BZ32" s="22"/>
@@ -3516,26 +3517,26 @@
     </row>
     <row r="33" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO-SN</v>
+        <v>CNRM-RCSM4</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>62</v>
+        <v>199</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="G33" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY33" s="22"/>
       <c r="BZ33" s="22"/>
@@ -3549,28 +3550,28 @@
       <c r="CH33" s="22"/>
       <c r="CI33" s="22"/>
     </row>
-    <row r="34" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>226</v>
+        <v>15</v>
       </c>
       <c r="C34" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CMCC-REMHI</v>
+        <v>SMHI-RCAO-SN</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>227</v>
+        <v>162</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>228</v>
+        <v>62</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>229</v>
+        <v>109</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY34" s="22"/>
       <c r="BZ34" s="22"/>
@@ -3586,23 +3587,23 @@
     </row>
     <row r="35" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>81</v>
+        <v>225</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>80</v>
+        <v>226</v>
       </c>
       <c r="C35" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>IITM-RegCM4-1</v>
+        <v>CMCC-REMHI</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>161</v>
+        <v>227</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>79</v>
+        <v>228</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>109</v>
+        <v>229</v>
       </c>
       <c r="G35" s="34" t="s">
         <v>139</v>
@@ -3621,26 +3622,26 @@
     </row>
     <row r="36" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C36" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CUNI-RegCM4-2</v>
+        <v>IITM-RegCM4-1</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="F36" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="BY36" s="22"/>
       <c r="BZ36" s="22"/>
@@ -3659,23 +3660,23 @@
         <v>49</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C37" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DHMZ-RegCM4-2</v>
+        <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="F37" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BY37" s="22"/>
       <c r="BZ37" s="22"/>
@@ -3691,26 +3692,26 @@
     </row>
     <row r="38" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C38" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ICTP-RegCM4-3</v>
+        <v>DHMZ-RegCM4-2</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY38" s="22"/>
       <c r="BZ38" s="22"/>
@@ -3729,20 +3730,20 @@
         <v>32</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C39" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UM-RegCM4-3</v>
+        <v>ICTP-RegCM4-3</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>206</v>
+        <v>76</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>207</v>
+        <v>75</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>208</v>
+        <v>109</v>
       </c>
       <c r="G39" s="34" t="s">
         <v>67</v>
@@ -3759,28 +3760,28 @@
       <c r="CH39" s="22"/>
       <c r="CI39" s="22"/>
     </row>
-    <row r="40" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C40" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ENEA-RegCM4-3</v>
+        <v>UM-RegCM4-3</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>154</v>
+        <v>206</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>77</v>
+        <v>207</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY40" s="22"/>
       <c r="BZ40" s="22"/>
@@ -3794,28 +3795,28 @@
       <c r="CH40" s="22"/>
       <c r="CI40" s="22"/>
     </row>
-    <row r="41" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>219</v>
+        <v>65</v>
       </c>
       <c r="C41" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>GERICS-REMO2009</v>
+        <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>220</v>
+        <v>154</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>221</v>
+        <v>77</v>
       </c>
       <c r="F41" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY41" s="22"/>
       <c r="BZ41" s="22"/>
@@ -3829,22 +3830,22 @@
       <c r="CH41" s="22"/>
       <c r="CI41" s="22"/>
     </row>
-    <row r="42" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>44</v>
+        <v>219</v>
       </c>
       <c r="C42" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MPI-CSC-REMO2009</v>
+        <v>GERICS-REMO2009</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>153</v>
+        <v>220</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>64</v>
+        <v>221</v>
       </c>
       <c r="F42" s="20" t="s">
         <v>109</v>
@@ -3876,13 +3877,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="28" t="s">
-        <v>102</v>
+      <c r="F43" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G43" s="34" t="s">
         <v>67</v>
@@ -3911,13 +3912,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F44" s="20" t="s">
-        <v>109</v>
+      <c r="F44" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="G44" s="34" t="s">
         <v>67</v>
@@ -3934,28 +3935,28 @@
       <c r="CH44" s="22"/>
       <c r="CI44" s="22"/>
     </row>
-    <row r="45" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>211</v>
+        <v>45</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>179</v>
+        <v>44</v>
       </c>
       <c r="C45" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>RMIB-Ugent-ALARO-0</v>
+        <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>180</v>
+        <v>64</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>212</v>
+        <v>109</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY45" s="22"/>
       <c r="BZ45" s="22"/>
@@ -3969,28 +3970,28 @@
       <c r="CH45" s="22"/>
       <c r="CI45" s="22"/>
     </row>
-    <row r="46" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B46" s="27" t="s">
-        <v>136</v>
+    <row r="46" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="C46" s="18" t="str">
-        <f>CONCATENATE(B46,"-",A46)</f>
-        <v>MGO-RRCM</v>
+        <f t="shared" si="0"/>
+        <v>RMIB-Ugent-ALARO-0</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>109</v>
+        <v>212</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY46" s="22"/>
       <c r="BZ46" s="22"/>
@@ -4004,28 +4005,28 @@
       <c r="CH46" s="22"/>
       <c r="CI46" s="22"/>
     </row>
-    <row r="47" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>55</v>
+    <row r="47" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="C47" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>AUTH-LHTEE-WRF321B</v>
+        <f>CONCATENATE(B47,"-",A47)</f>
+        <v>MGO-RRCM</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>190</v>
+        <v>133</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="F47" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G47" s="34" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="BY47" s="22"/>
       <c r="BZ47" s="22"/>
@@ -4039,28 +4040,28 @@
       <c r="CH47" s="22"/>
       <c r="CI47" s="22"/>
     </row>
-    <row r="48" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>203</v>
+    <row r="48" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C48" s="18" t="str">
-        <f>CONCATENATE(B48,"-",A48)</f>
-        <v>IPSL-WRF311</v>
+        <f t="shared" si="0"/>
+        <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>205</v>
+        <v>191</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G48" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BY48" s="22"/>
       <c r="BZ48" s="22"/>
@@ -4076,14 +4077,14 @@
     </row>
     <row r="49" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B49" s="25" t="s">
         <v>203</v>
       </c>
       <c r="C49" s="18" t="str">
-        <f t="shared" ref="C49" si="2">CONCATENATE(B49,"-",A49)</f>
-        <v>IPSL-WRF311NEMO</v>
+        <f>CONCATENATE(B49,"-",A49)</f>
+        <v>IPSL-WRF311</v>
       </c>
       <c r="D49" s="23" t="s">
         <v>202</v>
@@ -4092,7 +4093,7 @@
         <v>182</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G49" s="34" t="s">
         <v>139</v>
@@ -4109,28 +4110,28 @@
       <c r="CH49" s="22"/>
       <c r="CI49" s="22"/>
     </row>
-    <row r="50" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>8</v>
+    <row r="50" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>203</v>
       </c>
       <c r="C50" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UM-WRF331</v>
+        <f t="shared" ref="C50" si="2">CONCATENATE(B50,"-",A50)</f>
+        <v>IPSL-WRF311NEMO</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="F50" s="20" t="s">
-        <v>105</v>
+        <v>202</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY50" s="22"/>
       <c r="BZ50" s="22"/>
@@ -4145,24 +4146,24 @@
       <c r="CI50" s="22"/>
     </row>
     <row r="51" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
+      <c r="A51" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="29" t="s">
-        <v>16</v>
+      <c r="B51" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="C51" s="18" t="str">
-        <f t="shared" ref="C51" si="3">CONCATENATE(B51,"-",A51)</f>
-        <v>BCCR-WRF331</v>
+        <f t="shared" si="0"/>
+        <v>UM-WRF331</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E51" s="24" t="s">
-        <v>118</v>
+        <v>193</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>192</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="G51" s="34" t="s">
         <v>67</v>
@@ -4181,23 +4182,23 @@
     </row>
     <row r="52" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C52" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>MIUB-WRF331A</v>
+        <f t="shared" ref="C52" si="3">CONCATENATE(B52,"-",A52)</f>
+        <v>BCCR-WRF331</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>186</v>
+        <v>118</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="G52" s="34" t="s">
         <v>67</v>
@@ -4215,24 +4216,24 @@
       <c r="CI52" s="22"/>
     </row>
     <row r="53" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="25" t="s">
-        <v>11</v>
+      <c r="B53" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="C53" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CRP-GL-WRF331A</v>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="D53" s="23" t="s">
         <v>185</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G53" s="34" t="s">
         <v>67</v>
@@ -4250,24 +4251,24 @@
       <c r="CI53" s="22"/>
     </row>
     <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>16</v>
+      <c r="A54" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="C54" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>BCCR-WRF331C</v>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
       <c r="E54" s="24" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="G54" s="34" t="s">
         <v>67</v>
@@ -4284,25 +4285,25 @@
       <c r="CH54" s="22"/>
       <c r="CI54" s="22"/>
     </row>
-    <row r="55" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
-        <v>209</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>59</v>
+    <row r="55" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C55" s="18" t="str">
-        <f>CONCATENATE(B55,"-",A55)</f>
-        <v>IPSL-INERIS-WRF331F</v>
+        <f t="shared" si="0"/>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>106</v>
+        <v>119</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="G55" s="34" t="s">
         <v>67</v>
@@ -4319,28 +4320,28 @@
       <c r="CH55" s="22"/>
       <c r="CI55" s="22"/>
     </row>
-    <row r="56" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>52</v>
+        <v>209</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="C56" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF331G</v>
+        <f>CONCATENATE(B56,"-",A56)</f>
+        <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G56" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY56" s="22"/>
       <c r="BZ56" s="22"/>
@@ -4355,24 +4356,24 @@
       <c r="CI56" s="22"/>
     </row>
     <row r="57" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="31" t="s">
-        <v>66</v>
+      <c r="A57" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C57" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>NUIM-WRF341E</v>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>109</v>
+        <v>181</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="G57" s="34" t="s">
         <v>139</v>
@@ -4390,21 +4391,21 @@
       <c r="CI57" s="22"/>
     </row>
     <row r="58" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>17</v>
+      <c r="A58" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C58" s="18" t="str">
-        <f>CONCATENATE(B58,"-",A58)</f>
-        <v>IDL-WRF350D</v>
+        <f t="shared" si="0"/>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>176</v>
+        <v>78</v>
       </c>
       <c r="F58" s="20" t="s">
         <v>109</v>
@@ -4425,24 +4426,24 @@
       <c r="CI58" s="22"/>
     </row>
     <row r="59" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>52</v>
+      <c r="A59" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C59" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF350I</v>
+        <f>CONCATENATE(B59,"-",A59)</f>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
       <c r="G59" s="34" t="s">
         <v>139</v>
@@ -4459,28 +4460,28 @@
       <c r="CH59" s="22"/>
       <c r="CI59" s="22"/>
     </row>
-    <row r="60" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A60" s="31" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
       <c r="C60" s="18" t="str">
-        <f t="shared" ref="C60" si="4">CONCATENATE(B60,"-",A60)</f>
-        <v>UNSW-WRF360J</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF350I</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E60" s="40" t="s">
-        <v>116</v>
+        <v>183</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>117</v>
+        <v>223</v>
       </c>
       <c r="G60" s="34" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="BY60" s="22"/>
       <c r="BZ60" s="22"/>
@@ -4496,14 +4497,14 @@
     </row>
     <row r="61" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>140</v>
       </c>
       <c r="C61" s="18" t="str">
-        <f>CONCATENATE(B61,"-",A61)</f>
-        <v>UNSW-WRF360K</v>
+        <f t="shared" ref="C61" si="4">CONCATENATE(B61,"-",A61)</f>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D61" s="23" t="s">
         <v>115</v>
@@ -4531,14 +4532,14 @@
     </row>
     <row r="62" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B62" s="17" t="s">
         <v>140</v>
       </c>
       <c r="C62" s="18" t="str">
-        <f t="shared" ref="C62" si="5">CONCATENATE(B62,"-",A62)</f>
-        <v>UNSW-WRF360L</v>
+        <f>CONCATENATE(B62,"-",A62)</f>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D62" s="23" t="s">
         <v>115</v>
@@ -4564,28 +4565,28 @@
       <c r="CH62" s="22"/>
       <c r="CI62" s="22"/>
     </row>
-    <row r="63" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C63" s="18" t="str">
-        <f>CONCATENATE(B63,"-",A63)</f>
-        <v>MU-WRF360M</v>
+        <f t="shared" ref="C63" si="5">CONCATENATE(B63,"-",A63)</f>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>130</v>
+        <v>115</v>
+      </c>
+      <c r="E63" s="40" t="s">
+        <v>116</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="BY63" s="22"/>
       <c r="BZ63" s="22"/>
@@ -4599,28 +4600,28 @@
       <c r="CH63" s="22"/>
       <c r="CI63" s="22"/>
     </row>
-    <row r="64" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>16</v>
+    <row r="64" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>132</v>
       </c>
       <c r="C64" s="18" t="str">
-        <f t="shared" ref="C64" si="6">CONCATENATE(B64,"-",A64)</f>
-        <v>BCCR-WRF361</v>
+        <f>CONCATENATE(B64,"-",A64)</f>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>118</v>
+        <v>131</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY64" s="22"/>
       <c r="BZ64" s="22"/>
@@ -4634,25 +4635,25 @@
       <c r="CH64" s="22"/>
       <c r="CI64" s="22"/>
     </row>
-    <row r="65" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="B65" s="25" t="s">
-        <v>59</v>
+    <row r="65" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C65" s="18" t="str">
-        <f>CONCATENATE(B65,"-",A65)</f>
-        <v>IPSL-INERIS-WRF361F</v>
+        <f t="shared" ref="C65" si="6">CONCATENATE(B65,"-",A65)</f>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>106</v>
+        <v>119</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="G65" s="34" t="s">
         <v>67</v>
@@ -4669,28 +4670,28 @@
       <c r="CH65" s="22"/>
       <c r="CI65" s="22"/>
     </row>
-    <row r="66" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>9</v>
+    <row r="66" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B66" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="C66" s="18" t="str">
         <f>CONCATENATE(B66,"-",A66)</f>
-        <v>UHOH-WRF361H</v>
+        <v>IPSL-INERIS-WRF361F</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F66" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G66" s="19" t="s">
-        <v>138</v>
+        <v>182</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G66" s="34" t="s">
+        <v>67</v>
       </c>
       <c r="BY66" s="22"/>
       <c r="BZ66" s="22"/>
@@ -4704,28 +4705,28 @@
       <c r="CH66" s="22"/>
       <c r="CI66" s="22"/>
     </row>
-    <row r="67" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="47" t="s">
-        <v>222</v>
-      </c>
-      <c r="B67" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="C67" s="49" t="str">
+    <row r="67" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="18" t="str">
         <f>CONCATENATE(B67,"-",A67)</f>
-        <v>AUTH-MC-WRF371</v>
-      </c>
-      <c r="D67" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="E67" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="F67" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="G67" s="52" t="s">
-        <v>67</v>
+        <v>UHOH-WRF361H</v>
+      </c>
+      <c r="D67" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G67" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="BY67" s="22"/>
       <c r="BZ67" s="22"/>
@@ -4739,90 +4740,125 @@
       <c r="CH67" s="22"/>
       <c r="CI67" s="22"/>
     </row>
+    <row r="68" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="B68" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="C68" s="49" t="str">
+        <f>CONCATENATE(B68,"-",A68)</f>
+        <v>AUTH-MC-WRF371</v>
+      </c>
+      <c r="D68" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="E68" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F68" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="G68" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="BY68" s="22"/>
+      <c r="BZ68" s="22"/>
+      <c r="CA68" s="22"/>
+      <c r="CB68" s="22"/>
+      <c r="CC68" s="22"/>
+      <c r="CD68" s="22"/>
+      <c r="CE68" s="22"/>
+      <c r="CF68" s="22"/>
+      <c r="CG68" s="22"/>
+      <c r="CH68" s="22"/>
+      <c r="CI68" s="22"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E37:E38 F53:G53 B63:C63 E63:G63 B3:C15 A47:C47 F52 F59 C17 F58:G58 E56:E59 A17:A22 F17:G22 E19:E22 B20:C46 F45:F47 G38:G40 F50 A50:C50 E54:G54 A25:A45 E40 A56:C59 E56:G57 E42:E44 G42:G45 A66:C66 E66:G66 A52:C54">
+  <conditionalFormatting sqref="E38:E39 F54:G54 B64:C64 E64:G64 B3:C15 A48:C48 F53 F60 C17:C18 F59:G59 E57:E60 A17:A23 E20:E23 B21:C47 F46:F48 G39:G41 F51 A51:C51 E55:G55 A26:A46 E41 A57:C60 E57:G58 E43:E45 G43:G46 A67:C67 E67:G67 A53:C55 F17:G23">
     <cfRule type="containsText" dxfId="41" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A15 G36 F15 E23:G33 E3:G10 E11:F14 E35:G35 F34:G34">
+  <conditionalFormatting sqref="A3:A15 G37 F15 E24:G34 E3:G10 E11:F14 E36:G36 F35:G35">
     <cfRule type="containsText" dxfId="40" priority="52" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
+  <conditionalFormatting sqref="G38">
     <cfRule type="containsText" dxfId="39" priority="51" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F36:F44">
+  <conditionalFormatting sqref="F37:F45">
     <cfRule type="containsText" dxfId="38" priority="50" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",F36)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",F37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F63:G63 B63:C63">
+    <cfRule type="containsText" dxfId="37" priority="48" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F62:G62 B62:C62">
-    <cfRule type="containsText" dxfId="37" priority="48" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="36" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F61:G61 B61:C61">
-    <cfRule type="containsText" dxfId="36" priority="47" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B61)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F60:G60 A60:C60">
+  <conditionalFormatting sqref="F61:G61 A61:C61">
     <cfRule type="containsText" dxfId="35" priority="46" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51:C51 E51:G51">
-    <cfRule type="containsText" dxfId="34" priority="45" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64:C64 E64:G64">
-    <cfRule type="containsText" dxfId="33" priority="44" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
-    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A52:C52 E52:G52">
+    <cfRule type="containsText" dxfId="34" priority="45" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65:C65 E65:G65">
+    <cfRule type="containsText" dxfId="33" priority="44" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="containsText" dxfId="31" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63">
-    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="A64">
+    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
     <cfRule type="containsText" dxfId="29" priority="40" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G48">
+    <cfRule type="containsText" dxfId="28" priority="39" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E60">
+    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47">
-    <cfRule type="containsText" dxfId="28" priority="39" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:C16">
@@ -4835,94 +4871,94 @@
       <formula>NOT(ISERROR(SEARCH("unrestricted",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="C19">
     <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",C18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B19">
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:B20">
     <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E18">
+  <conditionalFormatting sqref="E15:E19">
     <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
+  <conditionalFormatting sqref="E46">
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E52)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E53)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48:C48 E48:G48">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
+  <conditionalFormatting sqref="E54">
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:C49 E49:G49">
-    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E39)))</formula>
+  <conditionalFormatting sqref="A50:C50 E50:G50">
+    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65:C65 E65:G65">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A65)))</formula>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55:C55 E55:G55">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
+  <conditionalFormatting sqref="A66:C66 E66:G66">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
+  <conditionalFormatting sqref="A56:C56 E56:G56">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G41)))</formula>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67 A67:C67">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
+  <conditionalFormatting sqref="G42">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G67">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G67)))</formula>
+  <conditionalFormatting sqref="F68 A68:C68">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G59">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G59)))</formula>
+  <conditionalFormatting sqref="G68">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G52">
+  <conditionalFormatting sqref="G60">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G53">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G52)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G15">
@@ -4930,22 +4966,22 @@
       <formula>NOT(ISERROR(SEARCH("unrestricted",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
+  <conditionalFormatting sqref="G51">
     <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
+  <conditionalFormatting sqref="E35">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E34)))</formula>
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D48" r:id="rId1"/>
-    <hyperlink ref="D49" r:id="rId2"/>
-    <hyperlink ref="D39" r:id="rId3" display="javascript:_e(%7B%7D,'cvml','ambrya@umich.edu');"/>
+    <hyperlink ref="D49" r:id="rId1"/>
+    <hyperlink ref="D50" r:id="rId2"/>
+    <hyperlink ref="D40" r:id="rId3" display="javascript:_e(%7B%7D,'cvml','ambrya@umich.edu');"/>
     <hyperlink ref="D9" r:id="rId4"/>
-    <hyperlink ref="D34" r:id="rId5" display="mailto:e.bucchignani@cira.it"/>
+    <hyperlink ref="D35" r:id="rId5" display="mailto:e.bucchignani@cira.it"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Wrong capitalization: Ulg -> ULg
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="234">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -700,12 +700,6 @@
     <t>"EUR-11 EUR-44"</t>
   </si>
   <si>
-    <t>Ulg</t>
-  </si>
-  <si>
-    <t>Ulg-MAR36</t>
-  </si>
-  <si>
     <t>Xavier Fettweis xavier.fettweis@ulg.ac.be</t>
   </si>
   <si>
@@ -764,6 +758,9 @@
   </si>
   <si>
     <t>Helmholtz-Zentrum Geesthacht, Climate Service Center Germany, Alfred Wegener Institute, Helmholtz Centre for Polar and Marine Research</t>
+  </si>
+  <si>
+    <t>ULg</t>
   </si>
 </sst>
 </file>
@@ -1299,6 +1296,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1306,33 +1324,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1344,37 +1341,7 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="43">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2121,20 +2088,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2160,20 +2127,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2196,127 +2163,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="61"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2331,32 +2298,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2375,8 +2342,8 @@
   </sheetPr>
   <dimension ref="A1:CI70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47:G48"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,7 +3049,7 @@
     </row>
     <row r="19" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>7</v>
@@ -3325,22 +3292,23 @@
     </row>
     <row r="26" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B26" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C26" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>ULg-MAR36</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="E26" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="F26" s="20" t="s">
         <v>215</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>217</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>67</v>
@@ -3674,23 +3642,23 @@
     </row>
     <row r="36" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C36" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CMCC-REMHI</v>
       </c>
       <c r="D36" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="F36" s="20" t="s">
         <v>227</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>229</v>
       </c>
       <c r="G36" s="34" t="s">
         <v>139</v>
@@ -3922,17 +3890,17 @@
         <v>45</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C43" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-REMO2009</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F43" s="20" t="s">
         <v>109</v>
@@ -4062,17 +4030,17 @@
         <v>45</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C47" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-AWI-REMO2009</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="34" t="s">
@@ -4092,20 +4060,20 @@
     </row>
     <row r="48" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C48" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-AWI-ROM1.1</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="34" t="s">
@@ -4596,7 +4564,7 @@
         <v>181</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G62" s="34" t="s">
         <v>139</v>
@@ -4860,10 +4828,10 @@
     </row>
     <row r="70" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A70" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70" s="48" t="s">
         <v>222</v>
-      </c>
-      <c r="B70" s="48" t="s">
-        <v>224</v>
       </c>
       <c r="C70" s="49" t="str">
         <f>CONCATENATE(B70,"-",A70)</f>
@@ -4894,213 +4862,213 @@
       <c r="CI70" s="22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E39:E40 F56:G56 B66:C66 E66:G66 B3:C6 A50:C50 F55 F62 C18:C19 F61:G61 E59:E62 G40:G42 F53 A53:C53 E57:G57 E42 A59:C62 E59:G60 E44:E46 A69:C69 E69:G69 A55:C57 A18:A24 B8:C16 B22:C46 B49:C49 F49:F50 A27:A46 A7:C7 G44:G46 F7:G7 E21 F18:G21 C21 E22:G24 F47:G48">
-    <cfRule type="containsText" dxfId="45" priority="52" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E39:E40 F56:G56 B66:C66 E66:G66 B3:C6 A50:C50 F55 F62 C18:C19 F61:G61 E59:E62 G40:G42 F53 A53:C53 E57:G57 E42 A59:C62 E59:G60 E44:E46 A69:C69 E69:G69 A55:C57 A18:A24 B8:C16 B49:C49 F49:F50 A27:A46 A7:C7 G44:G46 F7:G7 E21 F18:G21 C21 E22:G24 F47:G48 B22:C46">
+    <cfRule type="containsText" dxfId="42" priority="52" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A6 G38 F16 E25:G35 E3:G6 E12:F15 E37:G37 F36:G36 E8:G11 A8:A16">
-    <cfRule type="containsText" dxfId="44" priority="55" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="41" priority="55" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="containsText" dxfId="43" priority="54" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="40" priority="54" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38:F46">
-    <cfRule type="containsText" dxfId="42" priority="53" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="39" priority="53" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:G65 B65:C65">
-    <cfRule type="containsText" dxfId="41" priority="51" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="38" priority="51" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64:G64 B64:C64">
-    <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63:G63 A63:C63">
-    <cfRule type="containsText" dxfId="39" priority="49" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:C67 E67:G67">
-    <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="46" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="containsText" dxfId="35" priority="45" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="44" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" dxfId="33" priority="43" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="32" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:G17 A17">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B21">
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:E20">
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:C51 E51:G51">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:C52 E52:G52">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:C68 E68:G68">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:C58 E58:G58">
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70 A70:C70">
-    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G55">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G16">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B48">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:E48">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E47)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
AWI entries corrected (empty fields replaced by )
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="315" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="636" yWindow="312" windowWidth="20736" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="7" r:id="rId1"/>
     <sheet name="AllEntries" sheetId="4" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="AFR_22" localSheetId="0">ReadMe!#REF!</definedName>
@@ -23,6 +24,8 @@
     <definedName name="ANT44tier1">#REF!</definedName>
     <definedName name="ARC_44">#REF!</definedName>
     <definedName name="ARC44tier1">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$70</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
     <definedName name="EUR_11" localSheetId="0">ReadMe!#REF!</definedName>
     <definedName name="EUR_11">AllEntries!#REF!</definedName>
     <definedName name="EUR11tier1" localSheetId="0">ReadMe!#REF!</definedName>
@@ -33,8 +36,6 @@
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AU$1</definedName>
     <definedName name="Print_Area" localSheetId="0">ReadMe!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$70</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="234">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -760,7 +761,7 @@
     <t>Helmholtz-Zentrum Geesthacht, Climate Service Center Germany, Alfred Wegener Institute, Helmholtz Centre for Polar and Marine Research</t>
   </si>
   <si>
-    <t>ULg</t>
+    <t>Ulg</t>
   </si>
 </sst>
 </file>
@@ -1296,6 +1297,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1305,53 +1327,22 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
+    <cellStyle name="Hyperlänk 2" xfId="3"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="4"/>
-    <cellStyle name="Hyperlänk 2" xfId="3"/>
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1789,9 +1780,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1829,7 +1820,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1901,7 +1892,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2081,27 +2072,27 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="15" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="15" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:15" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2126,21 +2117,21 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="57" t="s">
+    <row r="3" spans="1:15" s="9" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2159,131 +2150,131 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
+    </row>
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="59"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
+    </row>
+    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="59"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="59"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="59"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="66"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="61"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2298,32 +2289,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2343,51 +2334,51 @@
   <dimension ref="A1:CI70"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="44" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="14" width="20.85546875" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="44" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="14" width="20.88671875" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" customWidth="1"/>
+    <col min="17" max="17" width="20.44140625" customWidth="1"/>
+    <col min="18" max="18" width="16.88671875" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" customWidth="1"/>
     <col min="21" max="21" width="16" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" customWidth="1"/>
-    <col min="23" max="24" width="17.42578125" customWidth="1"/>
+    <col min="22" max="22" width="17.33203125" customWidth="1"/>
+    <col min="23" max="24" width="17.44140625" customWidth="1"/>
     <col min="25" max="25" width="12" customWidth="1"/>
-    <col min="26" max="26" width="15.28515625" customWidth="1"/>
-    <col min="27" max="27" width="12.42578125" customWidth="1"/>
-    <col min="28" max="28" width="15.7109375" customWidth="1"/>
-    <col min="29" max="29" width="15.28515625" customWidth="1"/>
+    <col min="26" max="26" width="15.33203125" customWidth="1"/>
+    <col min="27" max="27" width="12.44140625" customWidth="1"/>
+    <col min="28" max="28" width="15.6640625" customWidth="1"/>
+    <col min="29" max="29" width="15.33203125" customWidth="1"/>
     <col min="30" max="30" width="16" customWidth="1"/>
     <col min="31" max="31" width="17" customWidth="1"/>
     <col min="32" max="32" width="16" customWidth="1"/>
-    <col min="33" max="33" width="16.85546875" customWidth="1"/>
-    <col min="34" max="36" width="20.42578125" customWidth="1"/>
-    <col min="37" max="37" width="10.7109375" customWidth="1"/>
-    <col min="38" max="38" width="23.42578125" customWidth="1"/>
-    <col min="39" max="39" width="12.28515625" customWidth="1"/>
-    <col min="40" max="40" width="15.42578125" customWidth="1"/>
-    <col min="41" max="41" width="18.28515625" customWidth="1"/>
-    <col min="42" max="42" width="20.140625" customWidth="1"/>
+    <col min="33" max="33" width="16.88671875" customWidth="1"/>
+    <col min="34" max="36" width="20.44140625" customWidth="1"/>
+    <col min="37" max="37" width="10.6640625" customWidth="1"/>
+    <col min="38" max="38" width="23.44140625" customWidth="1"/>
+    <col min="39" max="39" width="12.33203125" customWidth="1"/>
+    <col min="40" max="40" width="15.44140625" customWidth="1"/>
+    <col min="41" max="41" width="18.33203125" customWidth="1"/>
+    <col min="42" max="42" width="20.109375" customWidth="1"/>
     <col min="43" max="43" width="16" customWidth="1"/>
-    <col min="44" max="44" width="13.7109375" customWidth="1"/>
-    <col min="45" max="45" width="22.42578125" customWidth="1"/>
-    <col min="46" max="46" width="16.140625" customWidth="1"/>
-    <col min="47" max="48" width="15.42578125" customWidth="1"/>
-    <col min="49" max="49" width="16.140625" customWidth="1"/>
-    <col min="77" max="87" width="8.85546875" style="3"/>
+    <col min="44" max="44" width="13.6640625" customWidth="1"/>
+    <col min="45" max="45" width="22.44140625" customWidth="1"/>
+    <col min="46" max="46" width="16.109375" customWidth="1"/>
+    <col min="47" max="48" width="15.44140625" customWidth="1"/>
+    <col min="49" max="49" width="16.109375" customWidth="1"/>
+    <col min="77" max="87" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:87" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2521,7 +2512,7 @@
       <c r="CH3" s="22"/>
       <c r="CI3" s="22"/>
     </row>
-    <row r="4" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:87" s="21" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
@@ -2556,7 +2547,7 @@
       <c r="CH4" s="22"/>
       <c r="CI4" s="22"/>
     </row>
-    <row r="5" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>4</v>
       </c>
@@ -2591,7 +2582,7 @@
       <c r="CH5" s="22"/>
       <c r="CI5" s="22"/>
     </row>
-    <row r="6" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="43" t="s">
         <v>85</v>
       </c>
@@ -2661,7 +2652,7 @@
       <c r="CH7" s="22"/>
       <c r="CI7" s="22"/>
     </row>
-    <row r="8" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>47</v>
       </c>
@@ -3047,7 +3038,7 @@
       <c r="CH18" s="22"/>
       <c r="CI18" s="22"/>
     </row>
-    <row r="19" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>228</v>
       </c>
@@ -3064,7 +3055,9 @@
       <c r="E19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="20"/>
+      <c r="F19" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="G19" s="34" t="s">
         <v>67</v>
       </c>
@@ -3115,7 +3108,7 @@
       <c r="CH20" s="22"/>
       <c r="CI20" s="22"/>
     </row>
-    <row r="21" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:87" s="21" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>164</v>
       </c>
@@ -3150,7 +3143,7 @@
       <c r="CH21" s="22"/>
       <c r="CI21" s="22"/>
     </row>
-    <row r="22" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>39</v>
       </c>
@@ -3185,7 +3178,7 @@
       <c r="CH22" s="22"/>
       <c r="CI22" s="22"/>
     </row>
-    <row r="23" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
         <v>46</v>
       </c>
@@ -3220,7 +3213,7 @@
       <c r="CH23" s="22"/>
       <c r="CI23" s="22"/>
     </row>
-    <row r="24" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
         <v>0</v>
       </c>
@@ -3255,7 +3248,7 @@
       <c r="CH24" s="22"/>
       <c r="CI24" s="22"/>
     </row>
-    <row r="25" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
         <v>0</v>
       </c>
@@ -3290,7 +3283,7 @@
       <c r="CH25" s="22"/>
       <c r="CI25" s="22"/>
     </row>
-    <row r="26" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="46" t="s">
         <v>216</v>
       </c>
@@ -3299,7 +3292,7 @@
       </c>
       <c r="C26" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ULg-MAR36</v>
+        <v>Ulg-MAR36</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>213</v>
@@ -3325,7 +3318,7 @@
       <c r="CH26" s="22"/>
       <c r="CI26" s="22"/>
     </row>
-    <row r="27" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>31</v>
       </c>
@@ -3360,7 +3353,7 @@
       <c r="CH27" s="22"/>
       <c r="CI27" s="22"/>
     </row>
-    <row r="28" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="32" t="s">
         <v>38</v>
       </c>
@@ -3395,7 +3388,7 @@
       <c r="CH28" s="22"/>
       <c r="CI28" s="22"/>
     </row>
-    <row r="29" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
         <v>58</v>
       </c>
@@ -3430,7 +3423,7 @@
       <c r="CH29" s="22"/>
       <c r="CI29" s="22"/>
     </row>
-    <row r="30" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="s">
         <v>33</v>
       </c>
@@ -3465,7 +3458,7 @@
       <c r="CH30" s="22"/>
       <c r="CI30" s="22"/>
     </row>
-    <row r="31" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>3</v>
       </c>
@@ -3500,7 +3493,7 @@
       <c r="CH31" s="22"/>
       <c r="CI31" s="22"/>
     </row>
-    <row r="32" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
         <v>41</v>
       </c>
@@ -3535,7 +3528,7 @@
       <c r="CH32" s="22"/>
       <c r="CI32" s="22"/>
     </row>
-    <row r="33" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
         <v>37</v>
       </c>
@@ -3570,7 +3563,7 @@
       <c r="CH33" s="22"/>
       <c r="CI33" s="22"/>
     </row>
-    <row r="34" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
         <v>198</v>
       </c>
@@ -3605,7 +3598,7 @@
       <c r="CH34" s="22"/>
       <c r="CI34" s="22"/>
     </row>
-    <row r="35" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
         <v>40</v>
       </c>
@@ -3640,7 +3633,7 @@
       <c r="CH35" s="22"/>
       <c r="CI35" s="22"/>
     </row>
-    <row r="36" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>223</v>
       </c>
@@ -3675,7 +3668,7 @@
       <c r="CH36" s="22"/>
       <c r="CI36" s="22"/>
     </row>
-    <row r="37" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>81</v>
       </c>
@@ -3710,7 +3703,7 @@
       <c r="CH37" s="22"/>
       <c r="CI37" s="22"/>
     </row>
-    <row r="38" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
         <v>49</v>
       </c>
@@ -3745,7 +3738,7 @@
       <c r="CH38" s="22"/>
       <c r="CI38" s="22"/>
     </row>
-    <row r="39" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>49</v>
       </c>
@@ -3780,7 +3773,7 @@
       <c r="CH39" s="22"/>
       <c r="CI39" s="22"/>
     </row>
-    <row r="40" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
         <v>32</v>
       </c>
@@ -3815,7 +3808,7 @@
       <c r="CH40" s="22"/>
       <c r="CI40" s="22"/>
     </row>
-    <row r="41" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>32</v>
       </c>
@@ -3850,7 +3843,7 @@
       <c r="CH41" s="22"/>
       <c r="CI41" s="22"/>
     </row>
-    <row r="42" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:87" s="21" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>32</v>
       </c>
@@ -3885,7 +3878,7 @@
       <c r="CH42" s="22"/>
       <c r="CI42" s="22"/>
     </row>
-    <row r="43" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
         <v>45</v>
       </c>
@@ -3920,7 +3913,7 @@
       <c r="CH43" s="22"/>
       <c r="CI43" s="22"/>
     </row>
-    <row r="44" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
         <v>45</v>
       </c>
@@ -3955,7 +3948,7 @@
       <c r="CH44" s="22"/>
       <c r="CI44" s="22"/>
     </row>
-    <row r="45" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>45</v>
       </c>
@@ -3990,7 +3983,7 @@
       <c r="CH45" s="22"/>
       <c r="CI45" s="22"/>
     </row>
-    <row r="46" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A46" s="31" t="s">
         <v>45</v>
       </c>
@@ -4025,7 +4018,7 @@
       <c r="CH46" s="22"/>
       <c r="CI46" s="22"/>
     </row>
-    <row r="47" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:87" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
         <v>45</v>
       </c>
@@ -4042,7 +4035,9 @@
       <c r="E47" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="F47" s="20"/>
+      <c r="F47" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="G47" s="34" t="s">
         <v>67</v>
       </c>
@@ -4058,7 +4053,7 @@
       <c r="CH47" s="22"/>
       <c r="CI47" s="22"/>
     </row>
-    <row r="48" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:87" s="21" customFormat="1" ht="51" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
         <v>230</v>
       </c>
@@ -4075,7 +4070,9 @@
       <c r="E48" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="F48" s="20"/>
+      <c r="F48" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="G48" s="34" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4088,7 @@
       <c r="CH48" s="22"/>
       <c r="CI48" s="22"/>
     </row>
-    <row r="49" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="30" t="s">
         <v>134</v>
       </c>
@@ -4126,7 +4123,7 @@
       <c r="CH49" s="22"/>
       <c r="CI49" s="22"/>
     </row>
-    <row r="50" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:87" s="21" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
         <v>56</v>
       </c>
@@ -4161,7 +4158,7 @@
       <c r="CH50" s="22"/>
       <c r="CI50" s="22"/>
     </row>
-    <row r="51" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="32" t="s">
         <v>195</v>
       </c>
@@ -4196,7 +4193,7 @@
       <c r="CH51" s="22"/>
       <c r="CI51" s="22"/>
     </row>
-    <row r="52" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="32" t="s">
         <v>196</v>
       </c>
@@ -4231,7 +4228,7 @@
       <c r="CH52" s="22"/>
       <c r="CI52" s="22"/>
     </row>
-    <row r="53" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
         <v>2</v>
       </c>
@@ -4266,7 +4263,7 @@
       <c r="CH53" s="22"/>
       <c r="CI53" s="22"/>
     </row>
-    <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A54" s="33" t="s">
         <v>2</v>
       </c>
@@ -4301,7 +4298,7 @@
       <c r="CH54" s="22"/>
       <c r="CI54" s="22"/>
     </row>
-    <row r="55" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A55" s="33" t="s">
         <v>51</v>
       </c>
@@ -4336,7 +4333,7 @@
       <c r="CH55" s="22"/>
       <c r="CI55" s="22"/>
     </row>
-    <row r="56" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="32" t="s">
         <v>51</v>
       </c>
@@ -4371,7 +4368,7 @@
       <c r="CH56" s="22"/>
       <c r="CI56" s="22"/>
     </row>
-    <row r="57" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="33" t="s">
         <v>50</v>
       </c>
@@ -4406,7 +4403,7 @@
       <c r="CH57" s="22"/>
       <c r="CI57" s="22"/>
     </row>
-    <row r="58" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="32" t="s">
         <v>209</v>
       </c>
@@ -4441,7 +4438,7 @@
       <c r="CH58" s="22"/>
       <c r="CI58" s="22"/>
     </row>
-    <row r="59" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="32" t="s">
         <v>53</v>
       </c>
@@ -4476,7 +4473,7 @@
       <c r="CH59" s="22"/>
       <c r="CI59" s="22"/>
     </row>
-    <row r="60" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="31" t="s">
         <v>66</v>
       </c>
@@ -4511,7 +4508,7 @@
       <c r="CH60" s="22"/>
       <c r="CI60" s="22"/>
     </row>
-    <row r="61" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A61" s="32" t="s">
         <v>174</v>
       </c>
@@ -4546,7 +4543,7 @@
       <c r="CH61" s="22"/>
       <c r="CI61" s="22"/>
     </row>
-    <row r="62" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A62" s="31" t="s">
         <v>57</v>
       </c>
@@ -4686,7 +4683,7 @@
       <c r="CH65" s="22"/>
       <c r="CI65" s="22"/>
     </row>
-    <row r="66" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="31" t="s">
         <v>129</v>
       </c>
@@ -4721,7 +4718,7 @@
       <c r="CH66" s="22"/>
       <c r="CI66" s="22"/>
     </row>
-    <row r="67" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A67" s="33" t="s">
         <v>121</v>
       </c>
@@ -4756,7 +4753,7 @@
       <c r="CH67" s="22"/>
       <c r="CI67" s="22"/>
     </row>
-    <row r="68" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="32" t="s">
         <v>210</v>
       </c>
@@ -4791,7 +4788,7 @@
       <c r="CH68" s="22"/>
       <c r="CI68" s="22"/>
     </row>
-    <row r="69" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:87" s="21" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="53" t="s">
         <v>87</v>
       </c>
@@ -4826,7 +4823,7 @@
       <c r="CH69" s="22"/>
       <c r="CI69" s="22"/>
     </row>
-    <row r="70" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:87" s="21" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A70" s="47" t="s">
         <v>220</v>
       </c>
@@ -4863,212 +4860,212 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E39:E40 F56:G56 B66:C66 E66:G66 B3:C6 A50:C50 F55 F62 C18:C19 F61:G61 E59:E62 G40:G42 F53 A53:C53 E57:G57 E42 A59:C62 E59:G60 E44:E46 A69:C69 E69:G69 A55:C57 A18:A24 B8:C16 B49:C49 F49:F50 A27:A46 A7:C7 G44:G46 F7:G7 E21 F18:G21 C21 E22:G24 F47:G48 B22:C46">
-    <cfRule type="containsText" dxfId="42" priority="52" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="41" priority="52" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A6 G38 F16 E25:G35 E3:G6 E12:F15 E37:G37 F36:G36 E8:G11 A8:A16">
-    <cfRule type="containsText" dxfId="41" priority="55" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="40" priority="55" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="containsText" dxfId="40" priority="54" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="39" priority="54" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38:F46">
-    <cfRule type="containsText" dxfId="39" priority="53" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="38" priority="53" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:G65 B65:C65">
-    <cfRule type="containsText" dxfId="38" priority="51" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="37" priority="51" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64:G64 B64:C64">
-    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="36" priority="50" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63:G63 A63:C63">
-    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="48" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:C67 E67:G67">
-    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="33" priority="46" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="46" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="containsText" dxfId="32" priority="45" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="31" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="44" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" dxfId="30" priority="43" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="32" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:G17 A17">
-    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B21">
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:E20">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:C51 E51:G51">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:C52 E52:G52">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:C68 E68:G68">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:C58 E58:G58">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70 A70:C70">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G55">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G16">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B48">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:E48">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E47)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5087,4 +5084,16 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Model name change for AUTH
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -721,9 +721,6 @@
     <t>Helmholtz-Zentrum Geesthacht, Climate Service Center Germany</t>
   </si>
   <si>
-    <t>WRF371</t>
-  </si>
-  <si>
     <t>"EUR-44 SAM-44 AFR-44"</t>
   </si>
   <si>
@@ -761,6 +758,9 @@
   </si>
   <si>
     <t>ULg</t>
+  </si>
+  <si>
+    <t>WRF371M</t>
   </si>
 </sst>
 </file>
@@ -1296,6 +1296,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1305,31 +1326,10 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1341,17 +1341,7 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2088,20 +2078,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2127,20 +2117,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2163,127 +2153,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="59"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="59"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="59"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="59"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="66"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="61"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2298,32 +2288,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2342,8 +2332,8 @@
   </sheetPr>
   <dimension ref="A1:CI70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A52" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,7 +3039,7 @@
     </row>
     <row r="19" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>7</v>
@@ -3295,7 +3285,7 @@
         <v>216</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C26" s="18" t="str">
         <f t="shared" si="0"/>
@@ -3642,23 +3632,23 @@
     </row>
     <row r="36" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>223</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>224</v>
       </c>
       <c r="C36" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CMCC-REMHI</v>
       </c>
       <c r="D36" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="F36" s="20" t="s">
         <v>226</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>227</v>
       </c>
       <c r="G36" s="34" t="s">
         <v>139</v>
@@ -4030,17 +4020,17 @@
         <v>45</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C47" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-AWI-REMO2009</v>
       </c>
       <c r="D47" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="E47" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="34" t="s">
@@ -4060,20 +4050,20 @@
     </row>
     <row r="48" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C48" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-AWI-ROM1.1</v>
       </c>
       <c r="D48" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="E48" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="34" t="s">
@@ -4564,7 +4554,7 @@
         <v>181</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G62" s="34" t="s">
         <v>139</v>
@@ -4828,14 +4818,14 @@
     </row>
     <row r="70" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A70" s="47" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C70" s="49" t="str">
         <f>CONCATENATE(B70,"-",A70)</f>
-        <v>AUTH-MC-WRF371</v>
+        <v>AUTH-MC-WRF371M</v>
       </c>
       <c r="D70" s="50" t="s">
         <v>189</v>
@@ -4863,212 +4853,212 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E39:E40 F56:G56 B66:C66 E66:G66 B3:C6 A50:C50 F55 F62 C18:C19 F61:G61 E59:E62 G40:G42 F53 A53:C53 E57:G57 E42 A59:C62 E59:G60 E44:E46 A69:C69 E69:G69 A55:C57 A18:A24 B8:C16 B49:C49 F49:F50 A27:A46 A7:C7 G44:G46 F7:G7 E21 F18:G21 C21 E22:G24 F47:G48 B22:C46">
-    <cfRule type="containsText" dxfId="42" priority="52" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="41" priority="52" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A6 G38 F16 E25:G35 E3:G6 E12:F15 E37:G37 F36:G36 E8:G11 A8:A16">
-    <cfRule type="containsText" dxfId="41" priority="55" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="40" priority="55" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="containsText" dxfId="40" priority="54" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="39" priority="54" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38:F46">
-    <cfRule type="containsText" dxfId="39" priority="53" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="38" priority="53" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:G65 B65:C65">
-    <cfRule type="containsText" dxfId="38" priority="51" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="37" priority="51" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64:G64 B64:C64">
-    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="36" priority="50" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63:G63 A63:C63">
-    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="48" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:C67 E67:G67">
-    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="47" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="33" priority="46" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="46" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="containsText" dxfId="32" priority="45" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="31" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="44" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" dxfId="30" priority="43" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="42" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="32" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:G17 A17">
-    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B21">
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:E20">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:C51 E51:G51">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:C52 E52:G52">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:C68 E68:G68">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:C58 E58:G58">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70 A70:C70">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G55">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G16">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B48">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C48">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:E48">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E47)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adding new CLM version CCLM4-8-17-CLM3-5
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -33,7 +33,7 @@
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AU$1</definedName>
     <definedName name="Print_Area" localSheetId="0">ReadMe!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$70</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$71</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="235">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -761,6 +761,9 @@
   </si>
   <si>
     <t>WRF371M</t>
+  </si>
+  <si>
+    <t>CCLM4-8-17-CLM3-5</t>
   </si>
 </sst>
 </file>
@@ -1296,6 +1299,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1303,33 +1327,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1341,7 +1344,97 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2078,20 +2171,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2117,20 +2210,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2153,127 +2246,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="61"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2288,32 +2381,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2330,10 +2423,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI70"/>
+  <dimension ref="A1:CI71"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A52" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,7 +2577,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f t="shared" ref="C3:C62" si="0">CONCATENATE(B3,"-",A3)</f>
+        <f t="shared" ref="C3:C63" si="0">CONCATENATE(B3,"-",A3)</f>
         <v>CHMI-ALADIN53</v>
       </c>
       <c r="D3" s="23" t="s">
@@ -2940,7 +3033,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C16" si="1">CONCATENATE(B16,"-",A16)</f>
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D16" s="23" t="s">
@@ -2969,20 +3062,20 @@
     </row>
     <row r="17" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>30</v>
+        <v>234</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="C17" s="18" t="str">
-        <f t="shared" ref="C17" si="1">CONCATENATE(B17,"-",A17)</f>
-        <v>OURANOS-CRCM5</v>
+        <f t="shared" si="0"/>
+        <v>CLMcom-CCLM4-8-17-CLM3-5</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>109</v>
@@ -3007,17 +3100,17 @@
         <v>30</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>7</v>
+        <v>170</v>
       </c>
       <c r="C18" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UQAM-CRCM5</v>
+        <f t="shared" ref="C18" si="2">CONCATENATE(B18,"-",A18)</f>
+        <v>OURANOS-CRCM5</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="F18" s="20" t="s">
         <v>109</v>
@@ -3039,14 +3132,14 @@
     </row>
     <row r="19" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>227</v>
+        <v>30</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UQAM-CRCM5-SN</v>
+        <v>UQAM-CRCM5</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>151</v>
@@ -3054,7 +3147,9 @@
       <c r="E19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="20"/>
+      <c r="F19" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="G19" s="34" t="s">
         <v>67</v>
       </c>
@@ -3070,28 +3165,26 @@
       <c r="CH19" s="22"/>
       <c r="CI19" s="22"/>
     </row>
-    <row r="20" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="C20" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UNIBELGRADE-EBU1</v>
+        <v>UQAM-CRCM5-SN</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>169</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F20" s="20"/>
       <c r="G20" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY20" s="22"/>
       <c r="BZ20" s="22"/>
@@ -3107,14 +3200,14 @@
     </row>
     <row r="21" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>165</v>
       </c>
       <c r="C21" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UNIBELGRADE-EBUPOM2c1</v>
+        <v>UNIBELGRADE-EBU1</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>167</v>
@@ -3140,28 +3233,28 @@
       <c r="CH21" s="22"/>
       <c r="CI21" s="22"/>
     </row>
-    <row r="22" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
-        <v>39</v>
+    <row r="22" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>164</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="C22" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MOHC-HadGEM3-RA</v>
+        <v>UNIBELGRADE-EBUPOM2c1</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>72</v>
+        <v>168</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY22" s="22"/>
       <c r="BZ22" s="22"/>
@@ -3177,23 +3270,23 @@
     </row>
     <row r="23" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MOHC-HadRM3P</v>
+        <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>108</v>
+      <c r="F23" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>67</v>
@@ -3212,23 +3305,23 @@
     </row>
     <row r="24" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="C24" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DMI-HIRHAM5</v>
+        <v>MOHC-HadRM3P</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>171</v>
+        <v>34</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>177</v>
+        <v>72</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="G24" s="34" t="s">
         <v>67</v>
@@ -3245,25 +3338,25 @@
       <c r="CH24" s="22"/>
       <c r="CI24" s="22"/>
     </row>
-    <row r="25" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C25" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AWI-HIRHAM5</v>
+        <v>DMI-HIRHAM5</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>35</v>
+        <v>171</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="G25" s="34" t="s">
         <v>67</v>
@@ -3280,25 +3373,25 @@
       <c r="CH25" s="22"/>
       <c r="CI25" s="22"/>
     </row>
-    <row r="26" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
-        <v>216</v>
+    <row r="26" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>0</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>232</v>
+        <v>36</v>
       </c>
       <c r="C26" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ULg-MAR36</v>
+        <v>AWI-HIRHAM5</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>213</v>
+        <v>35</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>214</v>
+        <v>74</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>215</v>
+        <v>109</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>67</v>
@@ -3316,24 +3409,24 @@
       <c r="CI26" s="22"/>
     </row>
     <row r="27" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>10</v>
+      <c r="A27" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>232</v>
       </c>
       <c r="C27" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCLM-PROMES</v>
+        <v>ULg-MAR36</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>109</v>
+        <v>215</v>
       </c>
       <c r="G27" s="34" t="s">
         <v>67</v>
@@ -3350,25 +3443,25 @@
       <c r="CH27" s="22"/>
       <c r="CI27" s="22"/>
     </row>
-    <row r="28" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>22</v>
+    <row r="28" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C28" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO21P</v>
+        <v>UCLM-PROMES</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>61</v>
+        <v>163</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G28" s="34" t="s">
         <v>67</v>
@@ -3387,14 +3480,14 @@
     </row>
     <row r="29" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO22E</v>
+        <v>KNMI-RACMO21P</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>42</v>
@@ -3403,7 +3496,7 @@
         <v>61</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G29" s="34" t="s">
         <v>67</v>
@@ -3422,14 +3515,14 @@
     </row>
     <row r="30" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO22T</v>
+        <v>KNMI-RACMO22E</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>42</v>
@@ -3438,7 +3531,7 @@
         <v>61</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G30" s="34" t="s">
         <v>67</v>
@@ -3456,24 +3549,24 @@
       <c r="CI30" s="22"/>
     </row>
     <row r="31" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>15</v>
+      <c r="A31" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="C31" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCA4</v>
+        <v>KNMI-RACMO22T</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>62</v>
+        <v>42</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>61</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G31" s="34" t="s">
         <v>67</v>
@@ -3492,23 +3585,23 @@
     </row>
     <row r="32" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C32" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCA4-SN</v>
+        <v>SMHI-RCA4</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>162</v>
+        <v>26</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="28" t="s">
-        <v>103</v>
+      <c r="F32" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="G32" s="34" t="s">
         <v>67</v>
@@ -3527,14 +3620,14 @@
     </row>
     <row r="33" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO</v>
+        <v>SMHI-RCA4-SN</v>
       </c>
       <c r="D33" s="23" t="s">
         <v>162</v>
@@ -3542,8 +3635,8 @@
       <c r="E33" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="20" t="s">
-        <v>109</v>
+      <c r="F33" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="G33" s="34" t="s">
         <v>67</v>
@@ -3562,26 +3655,26 @@
     </row>
     <row r="34" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>198</v>
+        <v>37</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C34" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CNRM-RCSM4</v>
+        <v>SMHI-RCAO</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>199</v>
+        <v>62</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY34" s="22"/>
       <c r="BZ34" s="22"/>
@@ -3597,26 +3690,26 @@
     </row>
     <row r="35" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO-SN</v>
+        <v>CNRM-RCSM4</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>62</v>
+        <v>199</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY35" s="22"/>
       <c r="BZ35" s="22"/>
@@ -3630,28 +3723,28 @@
       <c r="CH35" s="22"/>
       <c r="CI35" s="22"/>
     </row>
-    <row r="36" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>222</v>
+        <v>40</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>223</v>
+        <v>15</v>
       </c>
       <c r="C36" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CMCC-REMHI</v>
+        <v>SMHI-RCAO-SN</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>225</v>
+        <v>62</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>226</v>
+        <v>109</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY36" s="22"/>
       <c r="BZ36" s="22"/>
@@ -3667,23 +3760,23 @@
     </row>
     <row r="37" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>81</v>
+        <v>222</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>80</v>
+        <v>223</v>
       </c>
       <c r="C37" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>IITM-RegCM4-1</v>
+        <v>CMCC-REMHI</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>161</v>
+        <v>224</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>79</v>
+        <v>225</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>109</v>
+        <v>226</v>
       </c>
       <c r="G37" s="34" t="s">
         <v>139</v>
@@ -3702,26 +3795,26 @@
     </row>
     <row r="38" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C38" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CUNI-RegCM4-2</v>
+        <v>IITM-RegCM4-1</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="BY38" s="22"/>
       <c r="BZ38" s="22"/>
@@ -3740,23 +3833,23 @@
         <v>49</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C39" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DHMZ-RegCM4-2</v>
+        <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="F39" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BY39" s="22"/>
       <c r="BZ39" s="22"/>
@@ -3772,26 +3865,26 @@
     </row>
     <row r="40" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C40" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ICTP-RegCM4-3</v>
+        <v>DHMZ-RegCM4-2</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F40" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY40" s="22"/>
       <c r="BZ40" s="22"/>
@@ -3810,20 +3903,20 @@
         <v>32</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C41" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UM-RegCM4-3</v>
+        <v>ICTP-RegCM4-3</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>206</v>
+        <v>76</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>207</v>
+        <v>75</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>208</v>
+        <v>109</v>
       </c>
       <c r="G41" s="34" t="s">
         <v>67</v>
@@ -3840,28 +3933,28 @@
       <c r="CH41" s="22"/>
       <c r="CI41" s="22"/>
     </row>
-    <row r="42" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C42" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ENEA-RegCM4-3</v>
+        <v>UM-RegCM4-3</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>154</v>
+        <v>206</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>77</v>
+        <v>207</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY42" s="22"/>
       <c r="BZ42" s="22"/>
@@ -3875,28 +3968,28 @@
       <c r="CH42" s="22"/>
       <c r="CI42" s="22"/>
     </row>
-    <row r="43" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>217</v>
+        <v>65</v>
       </c>
       <c r="C43" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>GERICS-REMO2009</v>
+        <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>218</v>
+        <v>154</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>219</v>
+        <v>77</v>
       </c>
       <c r="F43" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY43" s="22"/>
       <c r="BZ43" s="22"/>
@@ -3910,22 +4003,22 @@
       <c r="CH43" s="22"/>
       <c r="CI43" s="22"/>
     </row>
-    <row r="44" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>44</v>
+        <v>217</v>
       </c>
       <c r="C44" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MPI-CSC-REMO2009</v>
+        <v>GERICS-REMO2009</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>153</v>
+        <v>218</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>64</v>
+        <v>219</v>
       </c>
       <c r="F44" s="20" t="s">
         <v>109</v>
@@ -3957,13 +4050,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="28" t="s">
-        <v>102</v>
+      <c r="F45" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G45" s="34" t="s">
         <v>67</v>
@@ -3992,13 +4085,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="20" t="s">
-        <v>109</v>
+      <c r="F46" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="G46" s="34" t="s">
         <v>67</v>
@@ -4015,24 +4108,26 @@
       <c r="CH46" s="22"/>
       <c r="CI46" s="22"/>
     </row>
-    <row r="47" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="31" t="s">
-        <v>228</v>
+      <c r="B47" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="C47" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>GERICS-AWI-REMO2009</v>
+        <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>230</v>
+        <v>157</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="F47" s="20"/>
+        <v>64</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="G47" s="34" t="s">
         <v>67</v>
       </c>
@@ -4050,14 +4145,14 @@
     </row>
     <row r="48" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>229</v>
+        <v>45</v>
       </c>
       <c r="B48" s="31" t="s">
         <v>228</v>
       </c>
       <c r="C48" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>GERICS-AWI-ROM1.1</v>
+        <v>GERICS-AWI-REMO2009</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>230</v>
@@ -4081,26 +4176,24 @@
       <c r="CH48" s="22"/>
       <c r="CI48" s="22"/>
     </row>
-    <row r="49" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B49" s="27" t="s">
-        <v>136</v>
+    <row r="49" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>228</v>
       </c>
       <c r="C49" s="18" t="str">
-        <f>CONCATENATE(B49,"-",A49)</f>
-        <v>MGO-RRCM</v>
+        <f t="shared" si="0"/>
+        <v>GERICS-AWI-ROM1.1</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>133</v>
+        <v>230</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F49" s="20" t="s">
-        <v>109</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="F49" s="20"/>
       <c r="G49" s="34" t="s">
         <v>67</v>
       </c>
@@ -4116,28 +4209,28 @@
       <c r="CH49" s="22"/>
       <c r="CI49" s="22"/>
     </row>
-    <row r="50" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>55</v>
+    <row r="50" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="C50" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>AUTH-LHTEE-WRF321B</v>
+        <f>CONCATENATE(B50,"-",A50)</f>
+        <v>MGO-RRCM</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>190</v>
+        <v>133</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="F50" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="BY50" s="22"/>
       <c r="BZ50" s="22"/>
@@ -4151,28 +4244,28 @@
       <c r="CH50" s="22"/>
       <c r="CI50" s="22"/>
     </row>
-    <row r="51" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>203</v>
+    <row r="51" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C51" s="18" t="str">
-        <f>CONCATENATE(B51,"-",A51)</f>
-        <v>IPSL-WRF311</v>
+        <f t="shared" si="0"/>
+        <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>205</v>
+        <v>191</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G51" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BY51" s="22"/>
       <c r="BZ51" s="22"/>
@@ -4188,14 +4281,14 @@
     </row>
     <row r="52" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B52" s="25" t="s">
         <v>203</v>
       </c>
       <c r="C52" s="18" t="str">
-        <f t="shared" ref="C52" si="2">CONCATENATE(B52,"-",A52)</f>
-        <v>IPSL-WRF311NEMO</v>
+        <f>CONCATENATE(B52,"-",A52)</f>
+        <v>IPSL-WRF311</v>
       </c>
       <c r="D52" s="23" t="s">
         <v>202</v>
@@ -4204,7 +4297,7 @@
         <v>182</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G52" s="34" t="s">
         <v>139</v>
@@ -4221,28 +4314,28 @@
       <c r="CH52" s="22"/>
       <c r="CI52" s="22"/>
     </row>
-    <row r="53" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>8</v>
+    <row r="53" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>203</v>
       </c>
       <c r="C53" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UM-WRF331</v>
+        <f t="shared" ref="C53" si="3">CONCATENATE(B53,"-",A53)</f>
+        <v>IPSL-WRF311NEMO</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E53" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="F53" s="20" t="s">
-        <v>105</v>
+        <v>202</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="BZ53" s="22"/>
@@ -4257,24 +4350,24 @@
       <c r="CI53" s="22"/>
     </row>
     <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="29" t="s">
-        <v>16</v>
+      <c r="B54" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="C54" s="18" t="str">
-        <f t="shared" ref="C54" si="3">CONCATENATE(B54,"-",A54)</f>
-        <v>BCCR-WRF331</v>
+        <f t="shared" si="0"/>
+        <v>UM-WRF331</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>118</v>
+        <v>193</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>192</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="G54" s="34" t="s">
         <v>67</v>
@@ -4293,23 +4386,23 @@
     </row>
     <row r="55" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A55" s="33" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C55" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>MIUB-WRF331A</v>
+        <f t="shared" ref="C55" si="4">CONCATENATE(B55,"-",A55)</f>
+        <v>BCCR-WRF331</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>186</v>
+        <v>118</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="G55" s="34" t="s">
         <v>67</v>
@@ -4327,24 +4420,24 @@
       <c r="CI55" s="22"/>
     </row>
     <row r="56" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="25" t="s">
-        <v>11</v>
+      <c r="B56" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="C56" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CRP-GL-WRF331A</v>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="D56" s="23" t="s">
         <v>185</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G56" s="34" t="s">
         <v>67</v>
@@ -4362,24 +4455,24 @@
       <c r="CI56" s="22"/>
     </row>
     <row r="57" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B57" s="29" t="s">
-        <v>16</v>
+      <c r="A57" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="C57" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>BCCR-WRF331C</v>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="G57" s="34" t="s">
         <v>67</v>
@@ -4396,25 +4489,25 @@
       <c r="CH57" s="22"/>
       <c r="CI57" s="22"/>
     </row>
-    <row r="58" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="32" t="s">
-        <v>209</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>59</v>
+    <row r="58" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C58" s="18" t="str">
-        <f>CONCATENATE(B58,"-",A58)</f>
-        <v>IPSL-INERIS-WRF331F</v>
+        <f t="shared" si="0"/>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>106</v>
+        <v>119</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="G58" s="34" t="s">
         <v>67</v>
@@ -4431,28 +4524,28 @@
       <c r="CH58" s="22"/>
       <c r="CI58" s="22"/>
     </row>
-    <row r="59" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>52</v>
+        <v>209</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="C59" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF331G</v>
+        <f>CONCATENATE(B59,"-",A59)</f>
+        <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY59" s="22"/>
       <c r="BZ59" s="22"/>
@@ -4467,24 +4560,24 @@
       <c r="CI59" s="22"/>
     </row>
     <row r="60" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="31" t="s">
-        <v>66</v>
+      <c r="A60" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C60" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>NUIM-WRF341E</v>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>109</v>
+        <v>181</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="G60" s="34" t="s">
         <v>139</v>
@@ -4502,21 +4595,21 @@
       <c r="CI60" s="22"/>
     </row>
     <row r="61" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="B61" s="25" t="s">
-        <v>17</v>
+      <c r="A61" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C61" s="18" t="str">
-        <f>CONCATENATE(B61,"-",A61)</f>
-        <v>IDL-WRF350D</v>
+        <f t="shared" si="0"/>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>176</v>
+        <v>78</v>
       </c>
       <c r="F61" s="20" t="s">
         <v>109</v>
@@ -4537,24 +4630,24 @@
       <c r="CI61" s="22"/>
     </row>
     <row r="62" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>52</v>
+      <c r="A62" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C62" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UCAN-WRF350I</v>
+        <f>CONCATENATE(B62,"-",A62)</f>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>220</v>
+        <v>109</v>
       </c>
       <c r="G62" s="34" t="s">
         <v>139</v>
@@ -4571,28 +4664,28 @@
       <c r="CH62" s="22"/>
       <c r="CI62" s="22"/>
     </row>
-    <row r="63" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
       <c r="C63" s="18" t="str">
-        <f t="shared" ref="C63" si="4">CONCATENATE(B63,"-",A63)</f>
-        <v>UNSW-WRF360J</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF350I</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E63" s="40" t="s">
-        <v>116</v>
+        <v>183</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="BY63" s="22"/>
       <c r="BZ63" s="22"/>
@@ -4608,14 +4701,14 @@
     </row>
     <row r="64" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B64" s="17" t="s">
         <v>140</v>
       </c>
       <c r="C64" s="18" t="str">
-        <f>CONCATENATE(B64,"-",A64)</f>
-        <v>UNSW-WRF360K</v>
+        <f t="shared" ref="C64" si="5">CONCATENATE(B64,"-",A64)</f>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D64" s="23" t="s">
         <v>115</v>
@@ -4643,14 +4736,14 @@
     </row>
     <row r="65" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>140</v>
       </c>
       <c r="C65" s="18" t="str">
-        <f t="shared" ref="C65" si="5">CONCATENATE(B65,"-",A65)</f>
-        <v>UNSW-WRF360L</v>
+        <f>CONCATENATE(B65,"-",A65)</f>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D65" s="23" t="s">
         <v>115</v>
@@ -4676,28 +4769,28 @@
       <c r="CH65" s="22"/>
       <c r="CI65" s="22"/>
     </row>
-    <row r="66" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C66" s="18" t="str">
-        <f>CONCATENATE(B66,"-",A66)</f>
-        <v>MU-WRF360M</v>
+        <f t="shared" ref="C66" si="6">CONCATENATE(B66,"-",A66)</f>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>130</v>
+        <v>115</v>
+      </c>
+      <c r="E66" s="40" t="s">
+        <v>116</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="BY66" s="22"/>
       <c r="BZ66" s="22"/>
@@ -4711,28 +4804,28 @@
       <c r="CH66" s="22"/>
       <c r="CI66" s="22"/>
     </row>
-    <row r="67" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="B67" s="29" t="s">
-        <v>16</v>
+    <row r="67" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>132</v>
       </c>
       <c r="C67" s="18" t="str">
-        <f t="shared" ref="C67" si="6">CONCATENATE(B67,"-",A67)</f>
-        <v>BCCR-WRF361</v>
+        <f>CONCATENATE(B67,"-",A67)</f>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E67" s="24" t="s">
-        <v>118</v>
+        <v>131</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY67" s="22"/>
       <c r="BZ67" s="22"/>
@@ -4746,25 +4839,25 @@
       <c r="CH67" s="22"/>
       <c r="CI67" s="22"/>
     </row>
-    <row r="68" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="B68" s="25" t="s">
-        <v>59</v>
+    <row r="68" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C68" s="18" t="str">
-        <f>CONCATENATE(B68,"-",A68)</f>
-        <v>IPSL-INERIS-WRF361F</v>
+        <f t="shared" ref="C68" si="7">CONCATENATE(B68,"-",A68)</f>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D68" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="E68" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F68" s="19" t="s">
-        <v>106</v>
+        <v>119</v>
+      </c>
+      <c r="E68" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="G68" s="34" t="s">
         <v>67</v>
@@ -4781,28 +4874,28 @@
       <c r="CH68" s="22"/>
       <c r="CI68" s="22"/>
     </row>
-    <row r="69" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>9</v>
+    <row r="69" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="C69" s="18" t="str">
         <f>CONCATENATE(B69,"-",A69)</f>
-        <v>UHOH-WRF361H</v>
+        <v>IPSL-INERIS-WRF361F</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F69" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G69" s="19" t="s">
-        <v>138</v>
+        <v>182</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G69" s="34" t="s">
+        <v>67</v>
       </c>
       <c r="BY69" s="22"/>
       <c r="BZ69" s="22"/>
@@ -4816,28 +4909,28 @@
       <c r="CH69" s="22"/>
       <c r="CI69" s="22"/>
     </row>
-    <row r="70" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="47" t="s">
-        <v>233</v>
-      </c>
-      <c r="B70" s="48" t="s">
-        <v>221</v>
-      </c>
-      <c r="C70" s="49" t="str">
+    <row r="70" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" s="18" t="str">
         <f>CONCATENATE(B70,"-",A70)</f>
-        <v>AUTH-MC-WRF371M</v>
-      </c>
-      <c r="D70" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="E70" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="F70" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="G70" s="52" t="s">
-        <v>67</v>
+        <v>UHOH-WRF361H</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="BY70" s="22"/>
       <c r="BZ70" s="22"/>
@@ -4851,223 +4944,278 @@
       <c r="CH70" s="22"/>
       <c r="CI70" s="22"/>
     </row>
+    <row r="71" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="B71" s="48" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="49" t="str">
+        <f>CONCATENATE(B71,"-",A71)</f>
+        <v>AUTH-MC-WRF371M</v>
+      </c>
+      <c r="D71" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F71" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="G71" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="BY71" s="22"/>
+      <c r="BZ71" s="22"/>
+      <c r="CA71" s="22"/>
+      <c r="CB71" s="22"/>
+      <c r="CC71" s="22"/>
+      <c r="CD71" s="22"/>
+      <c r="CE71" s="22"/>
+      <c r="CF71" s="22"/>
+      <c r="CG71" s="22"/>
+      <c r="CH71" s="22"/>
+      <c r="CI71" s="22"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E39:E40 F56:G56 B66:C66 E66:G66 B3:C6 A50:C50 F55 F62 C18:C19 F61:G61 E59:E62 G40:G42 F53 A53:C53 E57:G57 E42 A59:C62 E59:G60 E44:E46 A69:C69 E69:G69 A55:C57 A18:A24 B8:C16 B49:C49 F49:F50 A27:A46 A7:C7 G44:G46 F7:G7 E21 F18:G21 C21 E22:G24 F47:G48 B22:C46">
-    <cfRule type="containsText" dxfId="41" priority="52" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E40:E41 F57:G57 B67:C67 E67:G67 B3:C6 A51:C51 F56 F63 C19:C20 F62:G62 E60:E63 G41:G43 F54 A54:C54 E58:G58 E43 A60:C63 E60:G61 E45:E47 A70:C70 E70:G70 A56:C58 A19:A25 B50:C50 F50:F51 A28:A47 A7:C7 G45:G47 F7:G7 E22 F19:G22 C22 E23:G25 F48:G49 B23:C47 B8:C15 B17:C17 B16">
+    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6 G38 F16 E25:G35 E3:G6 E12:F15 E37:G37 F36:G36 E8:G11 A8:A16">
-    <cfRule type="containsText" dxfId="40" priority="55" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A3:A6 G39 F17 E26:G36 E3:G6 E12:F15 E38:G38 F37:G37 E8:G11 A8:A17">
+    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G39">
-    <cfRule type="containsText" dxfId="39" priority="54" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G39)))</formula>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="containsText" dxfId="47" priority="58" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G40)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:F46">
-    <cfRule type="containsText" dxfId="38" priority="53" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",F38)))</formula>
+  <conditionalFormatting sqref="F39:F47">
+    <cfRule type="containsText" dxfId="46" priority="57" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",F39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F66:G66 B66:C66">
+    <cfRule type="containsText" dxfId="45" priority="55" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65:G65 B65:C65">
-    <cfRule type="containsText" dxfId="37" priority="51" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="44" priority="54" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B65)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F64:G64 B64:C64">
-    <cfRule type="containsText" dxfId="36" priority="50" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F63:G63 A63:C63">
-    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="34" priority="48" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:C67 E67:G67">
-    <cfRule type="containsText" dxfId="33" priority="47" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="32" priority="46" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="F64:G64 A64:C64">
+    <cfRule type="containsText" dxfId="43" priority="53" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A55:C55 E55:G55">
+    <cfRule type="containsText" dxfId="42" priority="52" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:C68 E68:G68">
+    <cfRule type="containsText" dxfId="41" priority="51" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="containsText" dxfId="31" priority="45" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="30" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="39" priority="49" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G51">
+    <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63">
+    <cfRule type="containsText" dxfId="34" priority="37" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="28" priority="42" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="27" priority="37" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62">
-    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="25" priority="32" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:C17">
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17:G17 A17">
-    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",C20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:B21">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="B18:C18">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16:E20">
-    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="F18:G18 A18">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",C21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:B22">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:E21">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:C52 E52:G52">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53:C53 E53:G53">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69:C69 E69:G69">
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:C59 E59:G59">
+    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G44">
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F71 A71:C71">
+    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A71)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G71">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G71)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G63">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G15 G17">
+    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G54">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B49">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C49">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48:E49">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",F16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
-    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51:C51 E51:G51">
-    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52:C52 E52:G52">
-    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="14" priority="17" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:C68 E68:G68">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A68)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58:C58 E58:G58">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F70 A70:C70">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A70)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G70">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G70)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G62)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G55">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G55)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G16">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47:B48">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47:C48">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:E48">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E47)))</formula>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D51" r:id="rId1"/>
-    <hyperlink ref="D52" r:id="rId2"/>
-    <hyperlink ref="D41" r:id="rId3" display="javascript:_e(%7B%7D,'cvml','ambrya@umich.edu');"/>
+    <hyperlink ref="D52" r:id="rId1"/>
+    <hyperlink ref="D53" r:id="rId2"/>
+    <hyperlink ref="D42" r:id="rId3" display="javascript:_e(%7B%7D,'cvml','ambrya@umich.edu');"/>
     <hyperlink ref="D10" r:id="rId4"/>
-    <hyperlink ref="D36" r:id="rId5" display="mailto:e.bucchignani@cira.it"/>
+    <hyperlink ref="D37" r:id="rId5" display="mailto:e.bucchignani@cira.it"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Added GERICS-REMO2015 and CLMcom-CCLM5-0-2
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -33,10 +33,11 @@
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
     <definedName name="Print_Area" localSheetId="1">AllEntries!$A$1:$AU$1</definedName>
     <definedName name="Print_Area" localSheetId="0">ReadMe!$A$1:$O$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$73</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="240">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -764,6 +765,21 @@
   </si>
   <si>
     <t>CCLM4-8-17-CLM3-5</t>
+  </si>
+  <si>
+    <t>CCLM5-0-2</t>
+  </si>
+  <si>
+    <t>Beate.Geyer, beate.geyer@hzg.de</t>
+  </si>
+  <si>
+    <t>"AUS-44"</t>
+  </si>
+  <si>
+    <t>REMO2015</t>
+  </si>
+  <si>
+    <t>Climate Service Center Germany</t>
   </si>
 </sst>
 </file>
@@ -1299,6 +1315,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1308,31 +1345,10 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1344,7 +1360,27 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="53">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2171,20 +2207,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2210,20 +2246,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2246,127 +2282,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="59"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="59"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="59"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="59"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="66"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="61"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2381,32 +2417,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2423,10 +2459,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI71"/>
+  <dimension ref="A1:CI73"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,7 +2613,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f t="shared" ref="C3:C63" si="0">CONCATENATE(B3,"-",A3)</f>
+        <f t="shared" ref="C3:C65" si="0">CONCATENATE(B3,"-",A3)</f>
         <v>CHMI-ALADIN53</v>
       </c>
       <c r="D3" s="23" t="s">
@@ -3097,23 +3133,23 @@
     </row>
     <row r="18" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>30</v>
+        <v>235</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="C18" s="18" t="str">
-        <f t="shared" ref="C18" si="2">CONCATENATE(B18,"-",A18)</f>
-        <v>OURANOS-CRCM5</v>
+        <f t="shared" si="0"/>
+        <v>CLMcom-CCLM5-0-2</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>172</v>
+        <v>236</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>109</v>
+        <v>237</v>
       </c>
       <c r="G18" s="34" t="s">
         <v>67</v>
@@ -3135,17 +3171,17 @@
         <v>30</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>7</v>
+        <v>170</v>
       </c>
       <c r="C19" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UQAM-CRCM5</v>
+        <f t="shared" ref="C19" si="2">CONCATENATE(B19,"-",A19)</f>
+        <v>OURANOS-CRCM5</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>109</v>
@@ -3167,14 +3203,14 @@
     </row>
     <row r="20" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>227</v>
+        <v>30</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UQAM-CRCM5-SN</v>
+        <v>UQAM-CRCM5</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>151</v>
@@ -3182,7 +3218,9 @@
       <c r="E20" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="20"/>
+      <c r="F20" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="G20" s="34" t="s">
         <v>67</v>
       </c>
@@ -3198,28 +3236,26 @@
       <c r="CH20" s="22"/>
       <c r="CI20" s="22"/>
     </row>
-    <row r="21" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="C21" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UNIBELGRADE-EBU1</v>
+        <v>UQAM-CRCM5-SN</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>169</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F21" s="20"/>
       <c r="G21" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY21" s="22"/>
       <c r="BZ21" s="22"/>
@@ -3235,14 +3271,14 @@
     </row>
     <row r="22" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>165</v>
       </c>
       <c r="C22" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UNIBELGRADE-EBUPOM2c1</v>
+        <v>UNIBELGRADE-EBU1</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>167</v>
@@ -3268,28 +3304,28 @@
       <c r="CH22" s="22"/>
       <c r="CI22" s="22"/>
     </row>
-    <row r="23" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>39</v>
+    <row r="23" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>164</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="C23" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MOHC-HadGEM3-RA</v>
+        <v>UNIBELGRADE-EBUPOM2c1</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>72</v>
+        <v>168</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY23" s="22"/>
       <c r="BZ23" s="22"/>
@@ -3305,23 +3341,23 @@
     </row>
     <row r="24" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MOHC-HadRM3P</v>
+        <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>108</v>
+      <c r="F24" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G24" s="34" t="s">
         <v>67</v>
@@ -3340,23 +3376,23 @@
     </row>
     <row r="25" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="C25" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DMI-HIRHAM5</v>
+        <v>MOHC-HadRM3P</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>171</v>
+        <v>34</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>177</v>
+        <v>72</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="G25" s="34" t="s">
         <v>67</v>
@@ -3373,25 +3409,25 @@
       <c r="CH25" s="22"/>
       <c r="CI25" s="22"/>
     </row>
-    <row r="26" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C26" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AWI-HIRHAM5</v>
+        <v>DMI-HIRHAM5</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>35</v>
+        <v>171</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>67</v>
@@ -3408,25 +3444,25 @@
       <c r="CH26" s="22"/>
       <c r="CI26" s="22"/>
     </row>
-    <row r="27" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
-        <v>216</v>
+    <row r="27" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>0</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>232</v>
+        <v>36</v>
       </c>
       <c r="C27" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ULg-MAR36</v>
+        <v>AWI-HIRHAM5</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>213</v>
+        <v>35</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>214</v>
+        <v>74</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>215</v>
+        <v>109</v>
       </c>
       <c r="G27" s="34" t="s">
         <v>67</v>
@@ -3444,24 +3480,24 @@
       <c r="CI27" s="22"/>
     </row>
     <row r="28" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>10</v>
+      <c r="A28" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>232</v>
       </c>
       <c r="C28" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCLM-PROMES</v>
+        <v>ULg-MAR36</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>109</v>
+        <v>215</v>
       </c>
       <c r="G28" s="34" t="s">
         <v>67</v>
@@ -3478,25 +3514,25 @@
       <c r="CH28" s="22"/>
       <c r="CI28" s="22"/>
     </row>
-    <row r="29" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>22</v>
+    <row r="29" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C29" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO21P</v>
+        <v>UCLM-PROMES</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>61</v>
+        <v>163</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G29" s="34" t="s">
         <v>67</v>
@@ -3515,14 +3551,14 @@
     </row>
     <row r="30" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO22E</v>
+        <v>KNMI-RACMO21P</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>42</v>
@@ -3531,7 +3567,7 @@
         <v>61</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G30" s="34" t="s">
         <v>67</v>
@@ -3550,14 +3586,14 @@
     </row>
     <row r="31" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>KNMI-RACMO22T</v>
+        <v>KNMI-RACMO22E</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>42</v>
@@ -3566,7 +3602,7 @@
         <v>61</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G31" s="34" t="s">
         <v>67</v>
@@ -3584,24 +3620,24 @@
       <c r="CI31" s="22"/>
     </row>
     <row r="32" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>15</v>
+      <c r="A32" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="C32" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCA4</v>
+        <v>KNMI-RACMO22T</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>62</v>
+        <v>42</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>61</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G32" s="34" t="s">
         <v>67</v>
@@ -3620,23 +3656,23 @@
     </row>
     <row r="33" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCA4-SN</v>
+        <v>SMHI-RCA4</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>162</v>
+        <v>26</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="28" t="s">
-        <v>103</v>
+      <c r="F33" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="G33" s="34" t="s">
         <v>67</v>
@@ -3655,14 +3691,14 @@
     </row>
     <row r="34" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO</v>
+        <v>SMHI-RCA4-SN</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>162</v>
@@ -3670,8 +3706,8 @@
       <c r="E34" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="20" t="s">
-        <v>109</v>
+      <c r="F34" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="G34" s="34" t="s">
         <v>67</v>
@@ -3690,26 +3726,26 @@
     </row>
     <row r="35" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>198</v>
+        <v>37</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C35" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CNRM-RCSM4</v>
+        <v>SMHI-RCAO</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>199</v>
+        <v>62</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY35" s="22"/>
       <c r="BZ35" s="22"/>
@@ -3725,26 +3761,26 @@
     </row>
     <row r="36" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C36" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>SMHI-RCAO-SN</v>
+        <v>CNRM-RCSM4</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>62</v>
+        <v>199</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY36" s="22"/>
       <c r="BZ36" s="22"/>
@@ -3758,28 +3794,28 @@
       <c r="CH36" s="22"/>
       <c r="CI36" s="22"/>
     </row>
-    <row r="37" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>222</v>
+        <v>40</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>223</v>
+        <v>15</v>
       </c>
       <c r="C37" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CMCC-REMHI</v>
+        <v>SMHI-RCAO-SN</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>225</v>
+        <v>62</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>226</v>
+        <v>109</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY37" s="22"/>
       <c r="BZ37" s="22"/>
@@ -3795,23 +3831,23 @@
     </row>
     <row r="38" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>81</v>
+        <v>222</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>80</v>
+        <v>223</v>
       </c>
       <c r="C38" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>IITM-RegCM4-1</v>
+        <v>CMCC-REMHI</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>161</v>
+        <v>224</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>79</v>
+        <v>225</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>109</v>
+        <v>226</v>
       </c>
       <c r="G38" s="34" t="s">
         <v>139</v>
@@ -3830,26 +3866,26 @@
     </row>
     <row r="39" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C39" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>CUNI-RegCM4-2</v>
+        <v>IITM-RegCM4-1</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="F39" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="BY39" s="22"/>
       <c r="BZ39" s="22"/>
@@ -3868,23 +3904,23 @@
         <v>49</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C40" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>DHMZ-RegCM4-2</v>
+        <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="F40" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BY40" s="22"/>
       <c r="BZ40" s="22"/>
@@ -3900,26 +3936,26 @@
     </row>
     <row r="41" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C41" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ICTP-RegCM4-3</v>
+        <v>DHMZ-RegCM4-2</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F41" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY41" s="22"/>
       <c r="BZ41" s="22"/>
@@ -3938,20 +3974,20 @@
         <v>32</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C42" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UM-RegCM4-3</v>
+        <v>ICTP-RegCM4-3</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>206</v>
+        <v>76</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>207</v>
+        <v>75</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>208</v>
+        <v>109</v>
       </c>
       <c r="G42" s="34" t="s">
         <v>67</v>
@@ -3968,28 +4004,28 @@
       <c r="CH42" s="22"/>
       <c r="CI42" s="22"/>
     </row>
-    <row r="43" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C43" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>ENEA-RegCM4-3</v>
+        <v>UM-RegCM4-3</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>154</v>
+        <v>206</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>77</v>
+        <v>207</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY43" s="22"/>
       <c r="BZ43" s="22"/>
@@ -4003,28 +4039,28 @@
       <c r="CH43" s="22"/>
       <c r="CI43" s="22"/>
     </row>
-    <row r="44" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>217</v>
+        <v>65</v>
       </c>
       <c r="C44" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>GERICS-REMO2009</v>
+        <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>218</v>
+        <v>154</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>219</v>
+        <v>77</v>
       </c>
       <c r="F44" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY44" s="22"/>
       <c r="BZ44" s="22"/>
@@ -4038,22 +4074,22 @@
       <c r="CH44" s="22"/>
       <c r="CI44" s="22"/>
     </row>
-    <row r="45" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>44</v>
+        <v>217</v>
       </c>
       <c r="C45" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MPI-CSC-REMO2009</v>
+        <v>GERICS-REMO2009</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>153</v>
+        <v>218</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>64</v>
+        <v>219</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>109</v>
@@ -4085,13 +4121,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="28" t="s">
-        <v>102</v>
+      <c r="F46" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G46" s="34" t="s">
         <v>67</v>
@@ -4120,13 +4156,13 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F47" s="20" t="s">
-        <v>109</v>
+      <c r="F47" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="G47" s="34" t="s">
         <v>67</v>
@@ -4143,24 +4179,26 @@
       <c r="CH47" s="22"/>
       <c r="CI47" s="22"/>
     </row>
-    <row r="48" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>228</v>
+      <c r="B48" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="C48" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>GERICS-AWI-REMO2009</v>
+        <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>230</v>
+        <v>157</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="F48" s="20"/>
+        <v>64</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="G48" s="34" t="s">
         <v>67</v>
       </c>
@@ -4178,14 +4216,14 @@
     </row>
     <row r="49" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
-        <v>229</v>
+        <v>45</v>
       </c>
       <c r="B49" s="31" t="s">
         <v>228</v>
       </c>
       <c r="C49" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>GERICS-AWI-ROM1.1</v>
+        <v>GERICS-AWI-REMO2009</v>
       </c>
       <c r="D49" s="23" t="s">
         <v>230</v>
@@ -4210,24 +4248,24 @@
       <c r="CI49" s="22"/>
     </row>
     <row r="50" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B50" s="27" t="s">
-        <v>136</v>
+      <c r="A50" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>217</v>
       </c>
       <c r="C50" s="18" t="str">
-        <f>CONCATENATE(B50,"-",A50)</f>
-        <v>MGO-RRCM</v>
+        <f t="shared" si="0"/>
+        <v>GERICS-REMO2015</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F50" s="20" t="s">
-        <v>109</v>
+        <v>239</v>
+      </c>
+      <c r="F50" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="G50" s="34" t="s">
         <v>67</v>
@@ -4244,28 +4282,26 @@
       <c r="CH50" s="22"/>
       <c r="CI50" s="22"/>
     </row>
-    <row r="51" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>55</v>
+        <v>229</v>
+      </c>
+      <c r="B51" s="31" t="s">
+        <v>228</v>
       </c>
       <c r="C51" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AUTH-LHTEE-WRF321B</v>
+        <v>GERICS-AWI-ROM1.1</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>109</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="F51" s="20"/>
       <c r="G51" s="34" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="BY51" s="22"/>
       <c r="BZ51" s="22"/>
@@ -4279,28 +4315,28 @@
       <c r="CH51" s="22"/>
       <c r="CI51" s="22"/>
     </row>
-    <row r="52" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>203</v>
+    <row r="52" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="C52" s="18" t="str">
         <f>CONCATENATE(B52,"-",A52)</f>
-        <v>IPSL-WRF311</v>
+        <v>MGO-RRCM</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>202</v>
+        <v>133</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>205</v>
+        <v>135</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G52" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY52" s="22"/>
       <c r="BZ52" s="22"/>
@@ -4314,28 +4350,28 @@
       <c r="CH52" s="22"/>
       <c r="CI52" s="22"/>
     </row>
-    <row r="53" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>203</v>
+    <row r="53" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="C53" s="18" t="str">
-        <f t="shared" ref="C53" si="3">CONCATENATE(B53,"-",A53)</f>
-        <v>IPSL-WRF311NEMO</v>
+        <f t="shared" si="0"/>
+        <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>204</v>
+        <v>191</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="BZ53" s="22"/>
@@ -4349,28 +4385,28 @@
       <c r="CH53" s="22"/>
       <c r="CI53" s="22"/>
     </row>
-    <row r="54" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>8</v>
+    <row r="54" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>203</v>
       </c>
       <c r="C54" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>UM-WRF331</v>
+        <f>CONCATENATE(B54,"-",A54)</f>
+        <v>IPSL-WRF311</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E54" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>105</v>
+        <v>202</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>205</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY54" s="22"/>
       <c r="BZ54" s="22"/>
@@ -4384,28 +4420,28 @@
       <c r="CH54" s="22"/>
       <c r="CI54" s="22"/>
     </row>
-    <row r="55" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>16</v>
+    <row r="55" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>203</v>
       </c>
       <c r="C55" s="18" t="str">
-        <f t="shared" ref="C55" si="4">CONCATENATE(B55,"-",A55)</f>
-        <v>BCCR-WRF331</v>
+        <f t="shared" ref="C55" si="3">CONCATENATE(B55,"-",A55)</f>
+        <v>IPSL-WRF311NEMO</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>120</v>
+        <v>202</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY55" s="22"/>
       <c r="BZ55" s="22"/>
@@ -4420,24 +4456,24 @@
       <c r="CI55" s="22"/>
     </row>
     <row r="56" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>54</v>
+      <c r="A56" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="C56" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>MIUB-WRF331A</v>
+        <v>UM-WRF331</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>186</v>
+        <v>193</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>192</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G56" s="34" t="s">
         <v>67</v>
@@ -4455,24 +4491,24 @@
       <c r="CI56" s="22"/>
     </row>
     <row r="57" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>11</v>
+      <c r="A57" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C57" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>CRP-GL-WRF331A</v>
+        <f t="shared" ref="C57" si="4">CONCATENATE(B57,"-",A57)</f>
+        <v>BCCR-WRF331</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>185</v>
+        <v>119</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>187</v>
+        <v>118</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="G57" s="34" t="s">
         <v>67</v>
@@ -4491,23 +4527,23 @@
     </row>
     <row r="58" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A58" s="33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C58" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>BCCR-WRF331C</v>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>118</v>
+        <v>186</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="G58" s="34" t="s">
         <v>67</v>
@@ -4524,25 +4560,25 @@
       <c r="CH58" s="22"/>
       <c r="CI58" s="22"/>
     </row>
-    <row r="59" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>209</v>
+        <v>51</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="C59" s="18" t="str">
-        <f>CONCATENATE(B59,"-",A59)</f>
-        <v>IPSL-INERIS-WRF331F</v>
+        <f t="shared" si="0"/>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F59" s="19" t="s">
-        <v>106</v>
+        <v>185</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G59" s="34" t="s">
         <v>67</v>
@@ -4560,27 +4596,27 @@
       <c r="CI59" s="22"/>
     </row>
     <row r="60" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>52</v>
+      <c r="A60" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C60" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCAN-WRF331G</v>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="F60" s="19" t="s">
-        <v>105</v>
+        <v>119</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="G60" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY60" s="22"/>
       <c r="BZ60" s="22"/>
@@ -4594,28 +4630,28 @@
       <c r="CH60" s="22"/>
       <c r="CI60" s="22"/>
     </row>
-    <row r="61" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>24</v>
+    <row r="61" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="C61" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>NUIM-WRF341E</v>
+        <f>CONCATENATE(B61,"-",A61)</f>
+        <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F61" s="20" t="s">
-        <v>109</v>
+        <v>182</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="G61" s="34" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="BY61" s="22"/>
       <c r="BZ61" s="22"/>
@@ -4631,23 +4667,23 @@
     </row>
     <row r="62" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>17</v>
+        <v>53</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="C62" s="18" t="str">
-        <f>CONCATENATE(B62,"-",A62)</f>
-        <v>IDL-WRF350D</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="F62" s="20" t="s">
-        <v>109</v>
+        <v>181</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="G62" s="34" t="s">
         <v>139</v>
@@ -4666,23 +4702,23 @@
     </row>
     <row r="63" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C63" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>UCAN-WRF350I</v>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>181</v>
+        <v>78</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>220</v>
+        <v>109</v>
       </c>
       <c r="G63" s="34" t="s">
         <v>139</v>
@@ -4699,28 +4735,28 @@
       <c r="CH63" s="22"/>
       <c r="CI63" s="22"/>
     </row>
-    <row r="64" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>140</v>
+    <row r="64" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="C64" s="18" t="str">
-        <f t="shared" ref="C64" si="5">CONCATENATE(B64,"-",A64)</f>
-        <v>UNSW-WRF360J</v>
+        <f>CONCATENATE(B64,"-",A64)</f>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E64" s="40" t="s">
-        <v>116</v>
+        <v>175</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>176</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="BY64" s="22"/>
       <c r="BZ64" s="22"/>
@@ -4734,28 +4770,28 @@
       <c r="CH64" s="22"/>
       <c r="CI64" s="22"/>
     </row>
-    <row r="65" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
       <c r="C65" s="18" t="str">
-        <f>CONCATENATE(B65,"-",A65)</f>
-        <v>UNSW-WRF360K</v>
+        <f t="shared" si="0"/>
+        <v>UCAN-WRF350I</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="E65" s="40" t="s">
-        <v>116</v>
+        <v>183</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="BY65" s="22"/>
       <c r="BZ65" s="22"/>
@@ -4771,14 +4807,14 @@
     </row>
     <row r="66" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B66" s="17" t="s">
         <v>140</v>
       </c>
       <c r="C66" s="18" t="str">
-        <f t="shared" ref="C66" si="6">CONCATENATE(B66,"-",A66)</f>
-        <v>UNSW-WRF360L</v>
+        <f t="shared" ref="C66" si="5">CONCATENATE(B66,"-",A66)</f>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D66" s="23" t="s">
         <v>115</v>
@@ -4804,28 +4840,28 @@
       <c r="CH66" s="22"/>
       <c r="CI66" s="22"/>
     </row>
-    <row r="67" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C67" s="18" t="str">
         <f>CONCATENATE(B67,"-",A67)</f>
-        <v>MU-WRF360M</v>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>130</v>
+        <v>115</v>
+      </c>
+      <c r="E67" s="40" t="s">
+        <v>116</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="BY67" s="22"/>
       <c r="BZ67" s="22"/>
@@ -4839,28 +4875,28 @@
       <c r="CH67" s="22"/>
       <c r="CI67" s="22"/>
     </row>
-    <row r="68" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="B68" s="29" t="s">
-        <v>16</v>
+    <row r="68" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="C68" s="18" t="str">
-        <f t="shared" ref="C68" si="7">CONCATENATE(B68,"-",A68)</f>
-        <v>BCCR-WRF361</v>
+        <f t="shared" ref="C68" si="6">CONCATENATE(B68,"-",A68)</f>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D68" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E68" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="E68" s="40" t="s">
+        <v>116</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G68" s="34" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="BY68" s="22"/>
       <c r="BZ68" s="22"/>
@@ -4875,27 +4911,27 @@
       <c r="CI68" s="22"/>
     </row>
     <row r="69" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="B69" s="25" t="s">
-        <v>59</v>
+      <c r="A69" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>132</v>
       </c>
       <c r="C69" s="18" t="str">
         <f>CONCATENATE(B69,"-",A69)</f>
-        <v>IPSL-INERIS-WRF361F</v>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F69" s="19" t="s">
-        <v>106</v>
+        <v>130</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G69" s="34" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="BY69" s="22"/>
       <c r="BZ69" s="22"/>
@@ -4910,27 +4946,27 @@
       <c r="CI69" s="22"/>
     </row>
     <row r="70" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>9</v>
+      <c r="A70" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="C70" s="18" t="str">
-        <f>CONCATENATE(B70,"-",A70)</f>
-        <v>UHOH-WRF361H</v>
+        <f t="shared" ref="C70" si="7">CONCATENATE(B70,"-",A70)</f>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D70" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>88</v>
+        <v>119</v>
+      </c>
+      <c r="E70" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G70" s="19" t="s">
-        <v>138</v>
+        <v>122</v>
+      </c>
+      <c r="G70" s="34" t="s">
+        <v>67</v>
       </c>
       <c r="BY70" s="22"/>
       <c r="BZ70" s="22"/>
@@ -4944,27 +4980,27 @@
       <c r="CH70" s="22"/>
       <c r="CI70" s="22"/>
     </row>
-    <row r="71" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="47" t="s">
-        <v>233</v>
-      </c>
-      <c r="B71" s="48" t="s">
-        <v>221</v>
-      </c>
-      <c r="C71" s="49" t="str">
+    <row r="71" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="18" t="str">
         <f>CONCATENATE(B71,"-",A71)</f>
-        <v>AUTH-MC-WRF371M</v>
-      </c>
-      <c r="D71" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="E71" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="F71" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="G71" s="52" t="s">
+        <v>IPSL-INERIS-WRF361F</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G71" s="34" t="s">
         <v>67</v>
       </c>
       <c r="BY71" s="22"/>
@@ -4979,246 +5015,327 @@
       <c r="CH71" s="22"/>
       <c r="CI71" s="22"/>
     </row>
+    <row r="72" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="18" t="str">
+        <f>CONCATENATE(B72,"-",A72)</f>
+        <v>UHOH-WRF361H</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G72" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="BY72" s="22"/>
+      <c r="BZ72" s="22"/>
+      <c r="CA72" s="22"/>
+      <c r="CB72" s="22"/>
+      <c r="CC72" s="22"/>
+      <c r="CD72" s="22"/>
+      <c r="CE72" s="22"/>
+      <c r="CF72" s="22"/>
+      <c r="CG72" s="22"/>
+      <c r="CH72" s="22"/>
+      <c r="CI72" s="22"/>
+    </row>
+    <row r="73" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="B73" s="48" t="s">
+        <v>221</v>
+      </c>
+      <c r="C73" s="49" t="str">
+        <f>CONCATENATE(B73,"-",A73)</f>
+        <v>AUTH-MC-WRF371M</v>
+      </c>
+      <c r="D73" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="E73" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F73" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="G73" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="BY73" s="22"/>
+      <c r="BZ73" s="22"/>
+      <c r="CA73" s="22"/>
+      <c r="CB73" s="22"/>
+      <c r="CC73" s="22"/>
+      <c r="CD73" s="22"/>
+      <c r="CE73" s="22"/>
+      <c r="CF73" s="22"/>
+      <c r="CG73" s="22"/>
+      <c r="CH73" s="22"/>
+      <c r="CI73" s="22"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E40:E41 F57:G57 B67:C67 E67:G67 B3:C6 A51:C51 F56 F63 C19:C20 F62:G62 E60:E63 G41:G43 F54 A54:C54 E58:G58 E43 A60:C63 E60:G61 E45:E47 A70:C70 E70:G70 A56:C58 A19:A25 B50:C50 F50:F51 A28:A47 A7:C7 G45:G47 F7:G7 E22 F19:G22 C22 E23:G25 F48:G49 B23:C47 B8:C15 B17:C17 B16">
-    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="E41:E42 F59:G59 B69:C69 E69:G69 B3:C6 A53:C53 F58 F65 C20:C21 F64:G64 E62:E65 G42:G44 F56 A56:C56 E60:G60 E44 A62:C65 E62:G63 E46:E48 A72:C72 E72:G72 A58:C60 A20:A26 B52:C52 F52:F53 A29:A48 A7:C7 G46:G48 F7:G7 E23 F20:G23 C23 E24:G26 F49:G49 B24:C48 B8:C15 B17:C18 B16 F51:G51 G50">
+    <cfRule type="containsText" dxfId="50" priority="58" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A6 G39 F17 E26:G36 E3:G6 E12:F15 E38:G38 F37:G37 E8:G11 A8:A17">
-    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A3:A6 G40 F17:F18 E27:G37 E3:G6 E12:F15 E39:G39 F38:G38 E8:G11 A8:A18">
+    <cfRule type="containsText" dxfId="49" priority="61" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="containsText" dxfId="47" priority="58" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G40)))</formula>
+  <conditionalFormatting sqref="G41">
+    <cfRule type="containsText" dxfId="48" priority="60" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39:F47">
-    <cfRule type="containsText" dxfId="46" priority="57" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",F39)))</formula>
+  <conditionalFormatting sqref="F40:F48">
+    <cfRule type="containsText" dxfId="47" priority="59" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",F40)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F66:G66 B66:C66">
-    <cfRule type="containsText" dxfId="45" priority="55" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B66)))</formula>
+  <conditionalFormatting sqref="F68:G68 B68:C68">
+    <cfRule type="containsText" dxfId="46" priority="57" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F65:G65 B65:C65">
-    <cfRule type="containsText" dxfId="44" priority="54" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B65)))</formula>
+  <conditionalFormatting sqref="F67:G67 B67:C67">
+    <cfRule type="containsText" dxfId="45" priority="56" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B67)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F64:G64 A64:C64">
-    <cfRule type="containsText" dxfId="43" priority="53" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A64)))</formula>
+  <conditionalFormatting sqref="F66:G66 A66:C66">
+    <cfRule type="containsText" dxfId="44" priority="55" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55:C55 E55:G55">
-    <cfRule type="containsText" dxfId="42" priority="52" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
+  <conditionalFormatting sqref="A57:C57 E57:G57">
+    <cfRule type="containsText" dxfId="43" priority="54" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A68:C68 E68:G68">
-    <cfRule type="containsText" dxfId="41" priority="51" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A70:C70 E70:G70">
+    <cfRule type="containsText" dxfId="42" priority="53" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A70)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="containsText" dxfId="41" priority="52" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="containsText" dxfId="40" priority="51" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A65)))</formula>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="containsText" dxfId="39" priority="50" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A69)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="containsText" dxfId="39" priority="49" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="containsText" dxfId="38" priority="49" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E52)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
+  <conditionalFormatting sqref="G53">
+    <cfRule type="containsText" dxfId="37" priority="48" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E50)))</formula>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G51)))</formula>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E65)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E39)))</formula>
+  <conditionalFormatting sqref="G52">
+    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
-    <cfRule type="containsText" dxfId="34" priority="37" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
+  <conditionalFormatting sqref="B19:C19">
     <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:C18">
-    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",B18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18:G18 A18">
-    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",C21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:B22">
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E21">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="F19:G19 A19">
+    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:B23">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",B20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:E22">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E56)))</formula>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E57)))</formula>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E59)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52:C52 E52:G52">
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A52)))</formula>
+  <conditionalFormatting sqref="A54:C54 E54:G54">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:C53 E53:G53">
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A53)))</formula>
+  <conditionalFormatting sqref="A55:C55 E55:G55">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E42)))</formula>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69:C69 E69:G69">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A69)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:C59 E59:G59">
-    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
-    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F71 A71:C71">
-    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="unrestricted">
+  <conditionalFormatting sqref="A71:C71 E71:G71">
+    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A71)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G71">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G71)))</formula>
+  <conditionalFormatting sqref="A61:C61 E61:G61">
+    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G63">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G63)))</formula>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G45">
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F73 A73:C73">
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G73">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G65">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G15 G17:G18">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G15 G17">
-    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G12)))</formula>
+  <conditionalFormatting sqref="E38">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G54">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G54)))</formula>
+  <conditionalFormatting sqref="A49:B51">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E37)))</formula>
+  <conditionalFormatting sqref="C49:C51">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48:B49">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",A48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C49">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48:E49">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",E48)))</formula>
+  <conditionalFormatting sqref="E49 E51">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G16)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",E50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",F50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D52" r:id="rId1"/>
-    <hyperlink ref="D53" r:id="rId2"/>
-    <hyperlink ref="D42" r:id="rId3" display="javascript:_e(%7B%7D,'cvml','ambrya@umich.edu');"/>
+    <hyperlink ref="D54" r:id="rId1"/>
+    <hyperlink ref="D55" r:id="rId2"/>
+    <hyperlink ref="D43" r:id="rId3" display="javascript:_e(%7B%7D,'cvml','ambrya@umich.edu');"/>
     <hyperlink ref="D10" r:id="rId4"/>
-    <hyperlink ref="D37" r:id="rId5" display="mailto:e.bucchignani@cira.it"/>
+    <hyperlink ref="D38" r:id="rId5" display="mailto:e.bucchignani@cira.it"/>
+    <hyperlink ref="D18" r:id="rId6" display="mailto:burkhardt.rockel@hzg.de"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId7"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
New data for AUTH
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="239">
   <si>
     <t>HIRHAM5</t>
   </si>
@@ -470,9 +470,6 @@
     <t>MGO</t>
   </si>
   <si>
-    <t>unknown</t>
-  </si>
-  <si>
     <t xml:space="preserve">non-commercial </t>
   </si>
   <si>
@@ -631,9 +628,6 @@
     <t>Aristotle University of Thessaloniki, Laboratory of Heat Transfer and Environmental Engeneering</t>
   </si>
   <si>
-    <t>Liana Kalognomou liana@aix.meng.auth.gr</t>
-  </si>
-  <si>
     <t>Universidad de Murcia</t>
   </si>
   <si>
@@ -779,6 +773,9 @@
   </si>
   <si>
     <t>RMIB-UGent</t>
+  </si>
+  <si>
+    <t>George Tsegas  gtseg@aix.meng.auth.gr</t>
   </si>
 </sst>
 </file>
@@ -1314,6 +1311,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1321,33 +1339,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1359,7 +1356,27 @@
     <cellStyle name="Normal 2" xfId="5"/>
     <cellStyle name="Standard 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2166,20 +2183,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
       <c r="M1" s="2"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -2205,20 +2222,20 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
       <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2241,127 +2258,127 @@
       <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="61"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
@@ -2376,32 +2393,32 @@
       <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
@@ -2420,8 +2437,8 @@
   </sheetPr>
   <dimension ref="A1:CI73"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,13 +2596,13 @@
         <v>29</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY3" s="22"/>
       <c r="BZ3" s="22"/>
@@ -2620,7 +2637,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY4" s="22"/>
       <c r="BZ4" s="22"/>
@@ -2646,16 +2663,16 @@
         <v>CNRM-ALADIN52</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY5" s="22"/>
       <c r="BZ5" s="22"/>
@@ -2681,16 +2698,16 @@
         <v>CNRM-ALADIN53</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E6" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>200</v>
-      </c>
       <c r="G6" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY6" s="22"/>
       <c r="BZ6" s="22"/>
@@ -2706,26 +2723,26 @@
     </row>
     <row r="7" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C7" s="18" t="str">
         <f>CONCATENATE(B7,"-",A7)</f>
         <v>RMIB-UGent-ALARO-0</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>179</v>
-      </c>
       <c r="F7" s="20" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY7" s="22"/>
       <c r="BZ7" s="22"/>
@@ -2751,10 +2768,10 @@
         <v>CNRM-ARPEGE52</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>109</v>
@@ -2787,7 +2804,7 @@
         <v>CCCma-CanRCM4</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>68</v>
@@ -2857,7 +2874,7 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>60</v>
@@ -2892,7 +2909,7 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>60</v>
@@ -2927,7 +2944,7 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>60</v>
@@ -2962,7 +2979,7 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>60</v>
@@ -2997,7 +3014,7 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>60</v>
@@ -3032,7 +3049,7 @@
         <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>60</v>
@@ -3057,7 +3074,7 @@
     </row>
     <row r="17" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>20</v>
@@ -3067,7 +3084,7 @@
         <v>CLMcom-CCLM4-8-17-CLM3-5</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>60</v>
@@ -3092,7 +3109,7 @@
     </row>
     <row r="18" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>20</v>
@@ -3102,13 +3119,13 @@
         <v>CLMcom-CCLM5-0-2</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>60</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G18" s="34" t="s">
         <v>67</v>
@@ -3130,17 +3147,17 @@
         <v>30</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" s="18" t="str">
         <f t="shared" ref="C19" si="2">CONCATENATE(B19,"-",A19)</f>
         <v>OURANOS-CRCM5</v>
       </c>
       <c r="D19" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>172</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>173</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>109</v>
@@ -3172,7 +3189,7 @@
         <v>UQAM-CRCM5</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>69</v>
@@ -3197,7 +3214,7 @@
     </row>
     <row r="21" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>7</v>
@@ -3207,7 +3224,7 @@
         <v>UQAM-CRCM5-SN</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>69</v>
@@ -3230,26 +3247,26 @@
     </row>
     <row r="22" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C22" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UNIBELGRADE-EBU1</v>
       </c>
       <c r="D22" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="F22" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="F22" s="20" t="s">
-        <v>169</v>
-      </c>
       <c r="G22" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY22" s="22"/>
       <c r="BZ22" s="22"/>
@@ -3265,26 +3282,26 @@
     </row>
     <row r="23" spans="1:87" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="C23" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UNIBELGRADE-EBUPOM2c1</v>
       </c>
       <c r="D23" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="F23" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="F23" s="20" t="s">
-        <v>169</v>
-      </c>
       <c r="G23" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY23" s="22"/>
       <c r="BZ23" s="22"/>
@@ -3310,7 +3327,7 @@
         <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>72</v>
@@ -3380,13 +3397,13 @@
         <v>DMI-HIRHAM5</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>67</v>
@@ -3440,23 +3457,23 @@
     </row>
     <row r="28" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C28" s="18" t="str">
         <f t="shared" si="0"/>
         <v>ULg-MAR36</v>
       </c>
       <c r="D28" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>212</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>214</v>
       </c>
       <c r="G28" s="34" t="s">
         <v>67</v>
@@ -3485,7 +3502,7 @@
         <v>UCLM-PROMES</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>63</v>
@@ -3660,7 +3677,7 @@
         <v>SMHI-RCA4-SN</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>62</v>
@@ -3695,7 +3712,7 @@
         <v>SMHI-RCAO</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>62</v>
@@ -3720,7 +3737,7 @@
     </row>
     <row r="36" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>13</v>
@@ -3730,16 +3747,16 @@
         <v>CNRM-RCSM4</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY36" s="22"/>
       <c r="BZ36" s="22"/>
@@ -3765,7 +3782,7 @@
         <v>SMHI-RCAO-SN</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>62</v>
@@ -3790,26 +3807,26 @@
     </row>
     <row r="38" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C38" s="18" t="str">
         <f t="shared" si="0"/>
         <v>CMCC-REMHI</v>
       </c>
       <c r="D38" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="E38" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>225</v>
-      </c>
       <c r="G38" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY38" s="22"/>
       <c r="BZ38" s="22"/>
@@ -3835,7 +3852,7 @@
         <v>IITM-RegCM4-1</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>79</v>
@@ -3844,7 +3861,7 @@
         <v>109</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY39" s="22"/>
       <c r="BZ39" s="22"/>
@@ -3870,10 +3887,10 @@
         <v>CUNI-RegCM4-2</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F40" s="20" t="s">
         <v>109</v>
@@ -3905,7 +3922,7 @@
         <v>DHMZ-RegCM4-2</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>71</v>
@@ -3914,7 +3931,7 @@
         <v>109</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY41" s="22"/>
       <c r="BZ41" s="22"/>
@@ -3975,13 +3992,13 @@
         <v>UM-RegCM4-3</v>
       </c>
       <c r="D43" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="F43" s="20" t="s">
         <v>205</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>207</v>
       </c>
       <c r="G43" s="34" t="s">
         <v>67</v>
@@ -4010,7 +4027,7 @@
         <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>77</v>
@@ -4019,7 +4036,7 @@
         <v>109</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY44" s="22"/>
       <c r="BZ44" s="22"/>
@@ -4038,17 +4055,17 @@
         <v>45</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C45" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-REMO2009</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>109</v>
@@ -4080,7 +4097,7 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>64</v>
@@ -4115,7 +4132,7 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>64</v>
@@ -4150,7 +4167,7 @@
         <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>64</v>
@@ -4178,17 +4195,17 @@
         <v>45</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C49" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-AWI-REMO2009</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="34" t="s">
@@ -4208,20 +4225,20 @@
     </row>
     <row r="50" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C50" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-REMO2015</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F50" s="28" t="s">
         <v>102</v>
@@ -4243,20 +4260,20 @@
     </row>
     <row r="51" spans="1:87" s="21" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C51" s="18" t="str">
         <f t="shared" si="0"/>
         <v>GERICS-AWI-ROM1.1</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="34" t="s">
@@ -4321,16 +4338,16 @@
         <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F53" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="BZ53" s="22"/>
@@ -4346,26 +4363,26 @@
     </row>
     <row r="54" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C54" s="18" t="str">
         <f>CONCATENATE(B54,"-",A54)</f>
         <v>IPSL-WRF311</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY54" s="22"/>
       <c r="BZ54" s="22"/>
@@ -4381,26 +4398,26 @@
     </row>
     <row r="55" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C55" s="18" t="str">
         <f t="shared" ref="C55" si="3">CONCATENATE(B55,"-",A55)</f>
         <v>IPSL-WRF311NEMO</v>
       </c>
       <c r="D55" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F55" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E55" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>203</v>
-      </c>
       <c r="G55" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY55" s="22"/>
       <c r="BZ55" s="22"/>
@@ -4426,10 +4443,10 @@
         <v>UM-WRF331</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F56" s="20" t="s">
         <v>105</v>
@@ -4496,10 +4513,10 @@
         <v>MIUB-WRF331A</v>
       </c>
       <c r="D58" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="E58" s="24" t="s">
         <v>184</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>185</v>
       </c>
       <c r="F58" s="20" t="s">
         <v>106</v>
@@ -4531,10 +4548,10 @@
         <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F59" s="20" t="s">
         <v>109</v>
@@ -4591,7 +4608,7 @@
     </row>
     <row r="61" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B61" s="25" t="s">
         <v>59</v>
@@ -4601,10 +4618,10 @@
         <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F61" s="19" t="s">
         <v>106</v>
@@ -4636,16 +4653,16 @@
         <v>UCAN-WRF331G</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F62" s="19" t="s">
         <v>105</v>
       </c>
       <c r="G62" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY62" s="22"/>
       <c r="BZ62" s="22"/>
@@ -4671,7 +4688,7 @@
         <v>NUIM-WRF341E</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E63" s="19" t="s">
         <v>78</v>
@@ -4680,7 +4697,7 @@
         <v>109</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY63" s="22"/>
       <c r="BZ63" s="22"/>
@@ -4696,7 +4713,7 @@
     </row>
     <row r="64" spans="1:87" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A64" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B64" s="25" t="s">
         <v>17</v>
@@ -4706,16 +4723,16 @@
         <v>IDL-WRF350D</v>
       </c>
       <c r="D64" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" s="19" t="s">
         <v>175</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>176</v>
       </c>
       <c r="F64" s="20" t="s">
         <v>109</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY64" s="22"/>
       <c r="BZ64" s="22"/>
@@ -4741,16 +4758,16 @@
         <v>UCAN-WRF350I</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY65" s="22"/>
       <c r="BZ65" s="22"/>
@@ -4769,7 +4786,7 @@
         <v>127</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C66" s="18" t="str">
         <f t="shared" ref="C66" si="5">CONCATENATE(B66,"-",A66)</f>
@@ -4804,7 +4821,7 @@
         <v>126</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C67" s="18" t="str">
         <f>CONCATENATE(B67,"-",A67)</f>
@@ -4839,7 +4856,7 @@
         <v>128</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C68" s="18" t="str">
         <f t="shared" ref="C68" si="6">CONCATENATE(B68,"-",A68)</f>
@@ -4890,7 +4907,7 @@
         <v>109</v>
       </c>
       <c r="G69" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BY69" s="22"/>
       <c r="BZ69" s="22"/>
@@ -4941,7 +4958,7 @@
     </row>
     <row r="71" spans="1:87" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B71" s="25" t="s">
         <v>59</v>
@@ -4951,10 +4968,10 @@
         <v>IPSL-INERIS-WRF361F</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F71" s="19" t="s">
         <v>106</v>
@@ -4995,7 +5012,7 @@
         <v>109</v>
       </c>
       <c r="G72" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BY72" s="22"/>
       <c r="BZ72" s="22"/>
@@ -5011,20 +5028,20 @@
     </row>
     <row r="73" spans="1:87" s="21" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A73" s="47" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B73" s="48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C73" s="49" t="str">
         <f>CONCATENATE(B73,"-",A73)</f>
         <v>AUTH-MC-WRF371M</v>
       </c>
       <c r="D73" s="50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E73" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F73" s="51" t="s">
         <v>105</v>
@@ -5046,248 +5063,248 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E41:E42 F59:G59 B69:C69 E69:G69 B3:C6 A53:C53 F58 F65 C20:C21 F64:G64 E62:E65 G42:G44 F56 A56:C56 E60:G60 E44 A62:C65 E62:G63 E46:E48 A72:C72 E72:G72 A58:C60 A20:A26 B52:C52 F52:F53 A29:A48 A7:C7 G46:G48 F7:G7 E23 F20:G23 C23 E24:G26 F49:G49 B24:C48 B8:C15 B17:C18 B16 F51:G51 G50">
-    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="50" priority="60" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A6 F17:F18 E27:G37 E3:G6 E12:F15 E39:G39 F38:G38 E8:G11 A8:A18">
-    <cfRule type="containsText" dxfId="47" priority="62" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="49" priority="63" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41">
-    <cfRule type="containsText" dxfId="46" priority="61" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="48" priority="62" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40:F48">
-    <cfRule type="containsText" dxfId="45" priority="60" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="47" priority="61" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F68:G68 B68:C68">
-    <cfRule type="containsText" dxfId="44" priority="58" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="46" priority="59" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F67:G67 B67:C67">
-    <cfRule type="containsText" dxfId="43" priority="57" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="45" priority="58" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66:G66 A66:C66">
-    <cfRule type="containsText" dxfId="42" priority="56" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="44" priority="57" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:C57 E57:G57">
-    <cfRule type="containsText" dxfId="41" priority="55" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="43" priority="56" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:C70 E70:G70">
-    <cfRule type="containsText" dxfId="40" priority="54" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="42" priority="55" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="containsText" dxfId="39" priority="53" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="41" priority="54" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="containsText" dxfId="38" priority="52" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="40" priority="53" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="containsText" dxfId="37" priority="51" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="39" priority="52" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" dxfId="36" priority="50" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="38" priority="51" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E52)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="35" priority="49" operator="containsText" text="unrestricted">
-      <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="36" priority="45" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="containsText" dxfId="33" priority="40" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="34" priority="40" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C19">
-    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:G19 A19">
-    <cfRule type="containsText" dxfId="30" priority="38" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:B23">
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:E22">
-    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:C54 E54:G54">
-    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:C55 E55:G55">
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:C71 E71:G71">
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:C61 E61:G61">
-    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F73 A73:C73">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G73">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G65">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G15 G17:G18">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B51">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C51">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49 E51">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",E50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",F50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="unrestricted">
       <formula>NOT(ISERROR(SEARCH("unrestricted",G40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G53">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unrestricted">
+      <formula>NOT(ISERROR(SEARCH("unrestricted",G53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
CSIRO and REMO updates
Added new CSIRO-CCAM model version; belatedly updated contact addresses for GERICS-REMO
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -33,7 +33,7 @@
     <definedName name="MED_44">AllEntries!#REF!</definedName>
     <definedName name="MED44tier1" localSheetId="0">ReadMe!#REF!</definedName>
     <definedName name="MED44tier1">AllEntries!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$98</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">AllEntries!$A$1:$G$99</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ReadMe!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="327">
   <si>
     <t>Register of CORDEX RCMs including target domains</t>
   </si>
@@ -484,9 +484,6 @@
     <t>GERICS</t>
   </si>
   <si>
-    <t>claas.teichmann@zmaw.de</t>
-  </si>
-  <si>
     <t>Helmholtz-Zentrum Geesthacht, Climate Service Center Germany</t>
   </si>
   <si>
@@ -494,10 +491,6 @@
   </si>
   <si>
     <t>Helmholtz-Zentrum Geesthacht, Climate Service Center, Max Planck Institute for Meteorology</t>
-  </si>
-  <si>
-    <t>claas.teichmann@zmaw.de
-lennart.marien@hzg.de</t>
   </si>
   <si>
     <t>"EUR-11"</t>
@@ -1046,6 +1039,12 @@
   </si>
   <si>
     <t>CCLM5-0-9-NEMOMED12-3-6-NEMONORDIC3-3</t>
+  </si>
+  <si>
+    <t>CCAM-1704</t>
+  </si>
+  <si>
+    <t>gerics_cordex@hzg.de</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1054,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\-yy"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1212,6 +1211,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1419,7 +1425,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1566,19 +1572,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1590,6 +1587,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -2457,20 +2467,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -2496,20 +2506,20 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2532,127 +2542,127 @@
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
@@ -2667,32 +2677,32 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B7:J7"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B7:J7"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -2704,10 +2714,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI99"/>
+  <dimension ref="A1:CI100"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A72" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A63" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,7 +2859,7 @@
         <v>88</v>
       </c>
       <c r="C2" s="27" t="str">
-        <f t="shared" ref="C2:C35" si="0">CONCATENATE(B2,"-",A2)</f>
+        <f t="shared" ref="C2:C36" si="0">CONCATENATE(B2,"-",A2)</f>
         <v>ULg-MAR36</v>
       </c>
       <c r="D2" s="28" t="s">
@@ -2894,7 +2904,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G3" s="31" t="s">
         <v>41</v>
@@ -2993,7 +3003,7 @@
         <v>CNRM-ALADIN53</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>34</v>
@@ -3018,7 +3028,7 @@
     </row>
     <row r="7" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>32</v>
@@ -3028,7 +3038,7 @@
         <v>CNRM-ALADIN63</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>34</v>
@@ -3053,7 +3063,7 @@
     </row>
     <row r="8" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>32</v>
@@ -3063,13 +3073,13 @@
         <v>CNRM-ALADIN64</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>41</v>
@@ -3112,7 +3122,7 @@
     </row>
     <row r="10" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>32</v>
@@ -3122,7 +3132,7 @@
         <v>CNRM-AROME-41t1</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>34</v>
@@ -3157,7 +3167,7 @@
         <v>CNRM-ARPEGE52</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>34</v>
@@ -3223,10 +3233,10 @@
         <v>47</v>
       </c>
       <c r="C13" s="27" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(B13,"-",A13)</f>
         <v>CSIRO-CCAM</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="29" t="s">
@@ -3238,7 +3248,6 @@
       <c r="G13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M13"/>
       <c r="BY13" s="33"/>
       <c r="BZ13" s="33"/>
       <c r="CA13" s="33"/>
@@ -3252,26 +3261,26 @@
       <c r="CI13" s="33"/>
     </row>
     <row r="14" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>CLMcom-CCLM4-8-17</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>54</v>
+      <c r="A14" s="64" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="64" t="str">
+        <f>CONCATENATE(B14,"-",A14)</f>
+        <v>CSIRO-CCAM-1704</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="29" t="s">
         <v>41</v>
       </c>
       <c r="M14"/>
@@ -3288,18 +3297,18 @@
       <c r="CI14" s="33"/>
     </row>
     <row r="15" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-CCLM4-8-17-CLM3-5</v>
+        <v>CLMcom-CCLM4-8-17</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>52</v>
@@ -3325,23 +3334,23 @@
     </row>
     <row r="16" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>225</v>
+        <v>56</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-CCLM5-0-0</v>
+        <v>CLMcom-CCLM4-8-17-CLM3-5</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>226</v>
+        <v>55</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>52</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>275</v>
+        <v>25</v>
       </c>
       <c r="G16" s="31" t="s">
         <v>41</v>
@@ -3359,25 +3368,25 @@
       <c r="CH16" s="33"/>
       <c r="CI16" s="33"/>
     </row>
-    <row r="17" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>283</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>289</v>
+    <row r="17" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>51</v>
       </c>
       <c r="C17" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-KIT-CCLM5-0-10</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>304</v>
-      </c>
-      <c r="E17" s="52" t="s">
-        <v>302</v>
-      </c>
-      <c r="F17" s="53" t="s">
-        <v>300</v>
+        <v>CLMcom-CCLM5-0-0</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>273</v>
       </c>
       <c r="G17" s="31" t="s">
         <v>41</v>
@@ -3396,29 +3405,29 @@
       <c r="CI17" s="33"/>
     </row>
     <row r="18" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>289</v>
+      <c r="A18" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>287</v>
       </c>
       <c r="C18" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-KIT-CCLM5-0-14</v>
+        <v>CLMcom-KIT-CCLM5-0-10</v>
       </c>
       <c r="D18" s="52" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G18" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M18" s="10"/>
+      <c r="M18"/>
       <c r="BY18" s="33"/>
       <c r="BZ18" s="33"/>
       <c r="CA18" s="33"/>
@@ -3432,29 +3441,29 @@
       <c r="CI18" s="33"/>
     </row>
     <row r="19" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>284</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>290</v>
+      <c r="A19" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>287</v>
       </c>
       <c r="C19" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-ZAMG-CCLM5-0-14</v>
+        <v>CLMcom-KIT-CCLM5-0-14</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G19" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M19"/>
+      <c r="M19" s="10"/>
       <c r="BY19" s="33"/>
       <c r="BZ19" s="33"/>
       <c r="CA19" s="33"/>
@@ -3469,28 +3478,28 @@
     </row>
     <row r="20" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C20" s="27" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">CLMcom-BTU-CCLM5-0-14 </v>
+        <v>CLMcom-ZAMG-CCLM5-0-14</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F20" s="53" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G20" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M20" s="10"/>
+      <c r="M20"/>
       <c r="BY20" s="33"/>
       <c r="BZ20" s="33"/>
       <c r="CA20" s="33"/>
@@ -3505,23 +3514,23 @@
     </row>
     <row r="21" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C21" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-DWD-CCLM5-0-15</v>
+        <v xml:space="preserve">CLMcom-BTU-CCLM5-0-14 </v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="F21" s="53" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G21" s="31" t="s">
         <v>41</v>
@@ -3541,23 +3550,23 @@
     </row>
     <row r="22" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>292</v>
       </c>
       <c r="C22" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-HZG-CCLM5-0-15</v>
+        <v>CLMcom-DWD-CCLM5-0-15</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F22" s="53" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="G22" s="31" t="s">
         <v>41</v>
@@ -3577,23 +3586,23 @@
     </row>
     <row r="23" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C23" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-JLU-CCLM5-0-15</v>
+        <v>CLMcom-HZG-CCLM5-0-15</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F23" s="53" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="G23" s="31" t="s">
         <v>41</v>
@@ -3611,25 +3620,25 @@
       <c r="CH23" s="33"/>
       <c r="CI23" s="33"/>
     </row>
-    <row r="24" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C24" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-KIT-CCLM5-0-15</v>
+        <v>CLMcom-JLU-CCLM5-0-15</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="F24" s="53" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="G24" s="31" t="s">
         <v>41</v>
@@ -3647,25 +3656,25 @@
       <c r="CH24" s="33"/>
       <c r="CI24" s="33"/>
     </row>
-    <row r="25" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
-        <v>57</v>
+        <v>284</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>51</v>
+        <v>287</v>
       </c>
       <c r="C25" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-CCLM5-0-2</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>224</v>
+        <v>CLMcom-KIT-CCLM5-0-15</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>307</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>300</v>
+      </c>
+      <c r="F25" s="53" t="s">
+        <v>308</v>
       </c>
       <c r="G25" s="31" t="s">
         <v>41</v>
@@ -3685,23 +3694,23 @@
     </row>
     <row r="26" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
-        <v>227</v>
+        <v>57</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-CCLM5-0-6</v>
+        <v>CLMcom-CCLM5-0-2</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>228</v>
+        <v>58</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>52</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>25</v>
+        <v>222</v>
       </c>
       <c r="G26" s="31" t="s">
         <v>41</v>
@@ -3719,25 +3728,25 @@
       <c r="CH26" s="33"/>
       <c r="CI26" s="33"/>
     </row>
-    <row r="27" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>288</v>
+        <v>51</v>
       </c>
       <c r="C27" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-CMCC-CCLM5-0-9</v>
-      </c>
-      <c r="D27" s="52" t="s">
-        <v>298</v>
-      </c>
-      <c r="E27" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="F27" s="53" t="s">
-        <v>300</v>
+        <v>CLMcom-CCLM5-0-6</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>25</v>
       </c>
       <c r="G27" s="31" t="s">
         <v>41</v>
@@ -3757,23 +3766,23 @@
     </row>
     <row r="28" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="C28" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-GUF-CCLM5-0-9</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>270</v>
+        <v>CLMcom-CMCC-CCLM5-0-9</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>296</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>297</v>
+      </c>
+      <c r="F28" s="53" t="s">
+        <v>298</v>
       </c>
       <c r="G28" s="31" t="s">
         <v>41</v>
@@ -3791,25 +3800,25 @@
       <c r="CH28" s="33"/>
       <c r="CI28" s="33"/>
     </row>
-    <row r="29" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="C29" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-KIT-CCLM5-0-9</v>
-      </c>
-      <c r="D29" s="52" t="s">
-        <v>301</v>
-      </c>
-      <c r="E29" s="52" t="s">
-        <v>302</v>
-      </c>
-      <c r="F29" s="53" t="s">
-        <v>303</v>
+        <v>CLMcom-GUF-CCLM5-0-9</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>268</v>
       </c>
       <c r="G29" s="31" t="s">
         <v>41</v>
@@ -3827,25 +3836,25 @@
       <c r="CH29" s="33"/>
       <c r="CI29" s="33"/>
     </row>
-    <row r="30" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>287</v>
       </c>
       <c r="C30" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>CLMcom-WEGC-CCLM5-0-9</v>
+        <v>CLMcom-KIT-CCLM5-0-9</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F30" s="53" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="G30" s="31" t="s">
         <v>41</v>
@@ -3863,25 +3872,25 @@
       <c r="CH30" s="33"/>
       <c r="CI30" s="33"/>
     </row>
-    <row r="31" spans="1:87" s="32" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="C31" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>POSTECH-CCLM5-0-9</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>263</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>250</v>
+        <v>CLMcom-WEGC-CCLM5-0-9</v>
+      </c>
+      <c r="D31" s="52" t="s">
+        <v>293</v>
+      </c>
+      <c r="E31" s="52" t="s">
+        <v>294</v>
+      </c>
+      <c r="F31" s="53" t="s">
+        <v>295</v>
       </c>
       <c r="G31" s="31" t="s">
         <v>41</v>
@@ -3899,25 +3908,25 @@
       <c r="CH31" s="33"/>
       <c r="CI31" s="33"/>
     </row>
-    <row r="32" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:87" s="32" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>325</v>
+        <v>260</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="C32" s="27" t="str">
-        <f t="shared" ref="C32:C33" si="1">CONCATENATE(B32,"-",A32)</f>
-        <v>CLMcom-GUF-CCLM5-0-9-NEMOMED12-3-6</v>
+        <f t="shared" si="0"/>
+        <v>POSTECH-CCLM5-0-9</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="G32" s="31" t="s">
         <v>41</v>
@@ -3937,23 +3946,23 @@
     </row>
     <row r="33" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C33" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>CLMcom-GUF-CCLM5-0-9-NEMOMED12-3-6-NEMONORDIC3-3</v>
+        <f t="shared" ref="C33:C34" si="1">CONCATENATE(B33,"-",A33)</f>
+        <v>CLMcom-GUF-CCLM5-0-9-NEMOMED12-3-6</v>
       </c>
       <c r="D33" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="F33" s="30" t="s">
         <v>268</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>270</v>
       </c>
       <c r="G33" s="31" t="s">
         <v>41</v>
@@ -3973,23 +3982,23 @@
     </row>
     <row r="34" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
-        <v>281</v>
+        <v>324</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C34" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>CLMcom-ETH-COSMO-crCLIM-v1-1</v>
+        <f t="shared" si="1"/>
+        <v>CLMcom-GUF-CCLM5-0-9-NEMOMED12-3-6-NEMONORDIC3-3</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>228</v>
+        <v>266</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>147</v>
+        <v>268</v>
       </c>
       <c r="G34" s="31" t="s">
         <v>41</v>
@@ -4007,25 +4016,25 @@
       <c r="CH34" s="33"/>
       <c r="CI34" s="33"/>
     </row>
-    <row r="35" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>59</v>
+        <v>279</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>60</v>
+        <v>277</v>
       </c>
       <c r="C35" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>OURANOS-CRCM5</v>
+        <v>CLMcom-ETH-COSMO-crCLIM-v1-1</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>62</v>
+        <v>278</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="G35" s="31" t="s">
         <v>41</v>
@@ -4043,22 +4052,22 @@
       <c r="CH35" s="33"/>
       <c r="CI35" s="33"/>
     </row>
-    <row r="36" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C36" s="27" t="str">
-        <f t="shared" ref="C36:C67" si="2">CONCATENATE(B36,"-",A36)</f>
-        <v>UQAM-CRCM5</v>
+        <f t="shared" si="0"/>
+        <v>OURANOS-CRCM5</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F36" s="30" t="s">
         <v>25</v>
@@ -4081,14 +4090,14 @@
     </row>
     <row r="37" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B37" s="27" t="s">
         <v>63</v>
       </c>
       <c r="C37" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v>UQAM-CRCM5-SN</v>
+        <f t="shared" ref="C37:C68" si="2">CONCATENATE(B37,"-",A37)</f>
+        <v>UQAM-CRCM5</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>64</v>
@@ -4097,12 +4106,12 @@
         <v>65</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="G37" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M37"/>
+      <c r="M37" s="10"/>
       <c r="BY37" s="33"/>
       <c r="BZ37" s="33"/>
       <c r="CA37" s="33"/>
@@ -4115,28 +4124,28 @@
       <c r="CH37" s="33"/>
       <c r="CI37" s="33"/>
     </row>
-    <row r="38" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C38" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>UNIBELGRADE-EBU1</v>
+        <v>UQAM-CRCM5-SN</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G38" s="31" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="M38"/>
       <c r="BY38" s="33"/>
@@ -4152,15 +4161,15 @@
       <c r="CI38" s="33"/>
     </row>
     <row r="39" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="26" t="s">
+      <c r="A39" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>UNIBELGRADE-EBUPOM2c1</v>
+        <v>UNIBELGRADE-EBU1</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>70</v>
@@ -4187,28 +4196,28 @@
       <c r="CH39" s="33"/>
       <c r="CI39" s="33"/>
     </row>
-    <row r="40" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
-        <v>230</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>231</v>
+    <row r="40" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="C40" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>INPE-ETA</v>
+        <v>UNIBELGRADE-EBUPOM2c1</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>232</v>
+        <v>70</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>233</v>
+        <v>72</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="M40"/>
       <c r="BY40" s="33"/>
@@ -4224,29 +4233,29 @@
       <c r="CI40" s="33"/>
     </row>
     <row r="41" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
-        <v>74</v>
+      <c r="A41" s="35" t="s">
+        <v>228</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>75</v>
+        <v>229</v>
       </c>
       <c r="C41" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>MOHC-HadGEM3-RA</v>
+        <v>INPE-ETA</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>76</v>
+        <v>232</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>25</v>
+        <v>231</v>
       </c>
       <c r="G41" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M41" s="10"/>
+      <c r="M41"/>
       <c r="BY41" s="33"/>
       <c r="BZ41" s="33"/>
       <c r="CA41" s="33"/>
@@ -4259,25 +4268,25 @@
       <c r="CH41" s="33"/>
       <c r="CI41" s="33"/>
     </row>
-    <row r="42" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="s">
         <v>74</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>266</v>
+        <v>75</v>
       </c>
       <c r="C42" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>NIMS-KMA-HadGEM3-RA</v>
+        <v>MOHC-HadGEM3-RA</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>265</v>
+        <v>76</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="G42" s="31" t="s">
         <v>41</v>
@@ -4295,25 +4304,25 @@
       <c r="CH42" s="33"/>
       <c r="CI42" s="33"/>
     </row>
-    <row r="43" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="s">
-        <v>282</v>
+        <v>74</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>75</v>
+        <v>264</v>
       </c>
       <c r="C43" s="27" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">MOHC-HadREM3-GA7-05 </v>
+        <v>NIMS-KMA-HadGEM3-RA</v>
       </c>
       <c r="D43" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="F43" s="30" t="s">
         <v>248</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="F43" s="30" t="s">
-        <v>147</v>
       </c>
       <c r="G43" s="31" t="s">
         <v>41</v>
@@ -4333,28 +4342,28 @@
     </row>
     <row r="44" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="B44" s="27" t="s">
         <v>75</v>
       </c>
       <c r="C44" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>MOHC-HadRM3P</v>
+        <v xml:space="preserve">MOHC-HadREM3-GA7-05 </v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E44" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="F44" s="29" t="s">
-        <v>78</v>
+      <c r="F44" s="30" t="s">
+        <v>145</v>
       </c>
       <c r="G44" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M44"/>
+      <c r="M44" s="10"/>
       <c r="BY44" s="33"/>
       <c r="BZ44" s="33"/>
       <c r="CA44" s="33"/>
@@ -4367,25 +4376,25 @@
       <c r="CH44" s="33"/>
       <c r="CI44" s="33"/>
     </row>
-    <row r="45" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" s="38" t="s">
-        <v>84</v>
+        <v>77</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>75</v>
       </c>
       <c r="C45" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>AWI-HIRHAM5</v>
-      </c>
-      <c r="D45" s="28" t="s">
-        <v>85</v>
+        <v>MOHC-HadRM3P</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>246</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="F45" s="30" t="s">
-        <v>25</v>
+        <v>76</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>78</v>
       </c>
       <c r="G45" s="31" t="s">
         <v>41</v>
@@ -4403,25 +4412,25 @@
       <c r="CH45" s="33"/>
       <c r="CI45" s="33"/>
     </row>
-    <row r="46" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
         <v>79</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C46" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>DMI-HIRHAM5</v>
+        <v>AWI-HIRHAM5</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F46" s="30" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="G46" s="31" t="s">
         <v>41</v>
@@ -4440,24 +4449,24 @@
       <c r="CI46" s="33"/>
     </row>
     <row r="47" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="27" t="s">
-        <v>93</v>
+      <c r="A47" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>80</v>
       </c>
       <c r="C47" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>UCLM-PROMES</v>
+        <v>DMI-HIRHAM5</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="G47" s="31" t="s">
         <v>41</v>
@@ -4476,24 +4485,24 @@
       <c r="CI47" s="33"/>
     </row>
     <row r="48" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="37" t="s">
-        <v>97</v>
+      <c r="A48" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="C48" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>KNMI-RACMO21P</v>
+        <v>UCLM-PROMES</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="40" t="s">
-        <v>99</v>
+        <v>94</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>95</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G48" s="31" t="s">
         <v>41</v>
@@ -4513,14 +4522,14 @@
     </row>
     <row r="49" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B49" s="37" t="s">
         <v>97</v>
       </c>
       <c r="C49" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>KNMI-RACMO22E</v>
+        <v>KNMI-RACMO21P</v>
       </c>
       <c r="D49" s="28" t="s">
         <v>98</v>
@@ -4529,7 +4538,7 @@
         <v>99</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G49" s="31" t="s">
         <v>41</v>
@@ -4549,14 +4558,14 @@
     </row>
     <row r="50" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B50" s="37" t="s">
         <v>97</v>
       </c>
       <c r="C50" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>KNMI-RACMO22T</v>
+        <v>KNMI-RACMO22E</v>
       </c>
       <c r="D50" s="28" t="s">
         <v>98</v>
@@ -4565,7 +4574,7 @@
         <v>99</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="G50" s="31" t="s">
         <v>41</v>
@@ -4583,25 +4592,25 @@
       <c r="CH50" s="33"/>
       <c r="CI50" s="33"/>
     </row>
-    <row r="51" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="B51" s="27" t="s">
-        <v>105</v>
+    <row r="51" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>97</v>
       </c>
       <c r="C51" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>SMHI-RCA4</v>
+        <v>KNMI-RACMO22T</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="E51" s="40" t="s">
+        <v>99</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="G51" s="31" t="s">
         <v>41</v>
@@ -4620,24 +4629,24 @@
       <c r="CI51" s="33"/>
     </row>
     <row r="52" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="B52" s="26" t="s">
+      <c r="A52" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="27" t="s">
         <v>105</v>
       </c>
       <c r="C52" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>SMHI-RCA4-SN</v>
-      </c>
-      <c r="D52" s="29" t="s">
-        <v>109</v>
+        <v>SMHI-RCA4</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>247</v>
       </c>
       <c r="E52" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="F52" s="41" t="s">
-        <v>110</v>
+      <c r="F52" s="30" t="s">
+        <v>107</v>
       </c>
       <c r="G52" s="31" t="s">
         <v>41</v>
@@ -4657,23 +4666,23 @@
     </row>
     <row r="53" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B53" s="26" t="s">
         <v>105</v>
       </c>
       <c r="C53" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>SMHI-RCAO</v>
-      </c>
-      <c r="D53" s="28" t="s">
+        <v>SMHI-RCA4-SN</v>
+      </c>
+      <c r="D53" s="29" t="s">
         <v>109</v>
       </c>
       <c r="E53" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="F53" s="30" t="s">
-        <v>25</v>
+      <c r="F53" s="41" t="s">
+        <v>110</v>
       </c>
       <c r="G53" s="31" t="s">
         <v>41</v>
@@ -4693,14 +4702,14 @@
     </row>
     <row r="54" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B54" s="26" t="s">
         <v>105</v>
       </c>
       <c r="C54" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>SMHI-RCAO-SN</v>
+        <v>SMHI-RCAO</v>
       </c>
       <c r="D54" s="28" t="s">
         <v>109</v>
@@ -4727,25 +4736,25 @@
       <c r="CH54" s="33"/>
       <c r="CI54" s="33"/>
     </row>
-    <row r="55" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="B55" s="27" t="s">
-        <v>32</v>
+    <row r="55" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>105</v>
       </c>
       <c r="C55" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>CNRM-RCSM4</v>
+        <v>SMHI-RCAO-SN</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>321</v>
+        <v>109</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="F55" s="30" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="G55" s="31" t="s">
         <v>41</v>
@@ -4765,28 +4774,28 @@
     </row>
     <row r="56" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
-        <v>319</v>
+        <v>112</v>
       </c>
       <c r="B56" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C56" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>CNRM-RCSM6</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>321</v>
+        <v>CNRM-RCSM4</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>319</v>
       </c>
       <c r="E56" s="29" t="s">
         <v>34</v>
       </c>
       <c r="F56" s="30" t="s">
-        <v>322</v>
+        <v>72</v>
       </c>
       <c r="G56" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M56" s="10"/>
+      <c r="M56"/>
       <c r="BY56" s="33"/>
       <c r="BZ56" s="33"/>
       <c r="CA56" s="33"/>
@@ -4800,29 +4809,29 @@
       <c r="CI56" s="33"/>
     </row>
     <row r="57" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
-        <v>253</v>
-      </c>
-      <c r="B57" s="26" t="s">
-        <v>254</v>
+      <c r="A57" s="35" t="s">
+        <v>317</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="C57" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>KNU-RegCM4-0</v>
-      </c>
-      <c r="D57" s="28" t="s">
-        <v>255</v>
+        <v>CNRM-RCSM6</v>
+      </c>
+      <c r="D57" s="29" t="s">
+        <v>319</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>256</v>
+        <v>34</v>
       </c>
       <c r="F57" s="30" t="s">
-        <v>250</v>
+        <v>320</v>
       </c>
       <c r="G57" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M57"/>
+      <c r="M57" s="10"/>
       <c r="BY57" s="33"/>
       <c r="BZ57" s="33"/>
       <c r="CA57" s="33"/>
@@ -4836,27 +4845,27 @@
       <c r="CI57" s="33"/>
     </row>
     <row r="58" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="B58" s="27" t="s">
-        <v>119</v>
+      <c r="A58" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>252</v>
       </c>
       <c r="C58" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>IITM-RegCM4-1</v>
+        <v>KNU-RegCM4-0</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>120</v>
+        <v>253</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>121</v>
+        <v>254</v>
       </c>
       <c r="F58" s="30" t="s">
-        <v>25</v>
+        <v>248</v>
       </c>
       <c r="G58" s="31" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="M58"/>
       <c r="BY58" s="33"/>
@@ -4873,26 +4882,26 @@
     </row>
     <row r="59" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C59" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>CUNI-RegCM4-2</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>124</v>
+        <v>IITM-RegCM4-1</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>120</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F59" s="30" t="s">
         <v>25</v>
       </c>
       <c r="G59" s="31" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="M59"/>
       <c r="BY59" s="33"/>
@@ -4912,25 +4921,25 @@
         <v>122</v>
       </c>
       <c r="B60" s="27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C60" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>DHMZ-RegCM4-2</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>127</v>
+        <v>CUNI-RegCM4-2</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>124</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F60" s="30" t="s">
         <v>25</v>
       </c>
       <c r="G60" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="M60" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="M60"/>
       <c r="BY60" s="33"/>
       <c r="BZ60" s="33"/>
       <c r="CA60" s="33"/>
@@ -4945,28 +4954,28 @@
     </row>
     <row r="61" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A61" s="35" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>243</v>
+        <v>126</v>
       </c>
       <c r="C61" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>BOUN-RegCM4-3</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>244</v>
+        <v>DHMZ-RegCM4-2</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>245</v>
+        <v>128</v>
       </c>
       <c r="F61" s="30" t="s">
-        <v>276</v>
+        <v>25</v>
       </c>
       <c r="G61" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="M61"/>
+      <c r="M61" s="10"/>
       <c r="BY61" s="33"/>
       <c r="BZ61" s="33"/>
       <c r="CA61" s="33"/>
@@ -4979,25 +4988,25 @@
       <c r="CH61" s="33"/>
       <c r="CI61" s="33"/>
     </row>
-    <row r="62" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A62" s="35" t="s">
         <v>129</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>137</v>
+        <v>241</v>
       </c>
       <c r="C62" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>ENEA-RegCM4-3</v>
-      </c>
-      <c r="D62" s="28" t="s">
-        <v>138</v>
+        <v>BOUN-RegCM4-3</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>242</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>139</v>
+        <v>243</v>
       </c>
       <c r="F62" s="30" t="s">
-        <v>25</v>
+        <v>274</v>
       </c>
       <c r="G62" s="31" t="s">
         <v>26</v>
@@ -5015,28 +5024,28 @@
       <c r="CH62" s="33"/>
       <c r="CI62" s="33"/>
     </row>
-    <row r="63" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="35" t="s">
         <v>129</v>
       </c>
       <c r="B63" s="27" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C63" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>ICTP-RegCM4-3</v>
+        <v>ENEA-RegCM4-3</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F63" s="30" t="s">
         <v>25</v>
       </c>
       <c r="G63" s="31" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="M63"/>
       <c r="BY63" s="33"/>
@@ -5056,20 +5065,20 @@
         <v>129</v>
       </c>
       <c r="B64" s="27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C64" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>UM-RegCM4-3</v>
+        <v>ICTP-RegCM4-3</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F64" s="30" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="G64" s="31" t="s">
         <v>41</v>
@@ -5087,25 +5096,25 @@
       <c r="CH64" s="33"/>
       <c r="CI64" s="33"/>
     </row>
-    <row r="65" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A65" s="35" t="s">
-        <v>264</v>
+        <v>129</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C65" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>ICTP-RegCM4-6</v>
-      </c>
-      <c r="D65" s="29" t="s">
-        <v>131</v>
+        <v>UM-RegCM4-3</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>134</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F65" s="30" t="s">
-        <v>247</v>
+        <v>136</v>
       </c>
       <c r="G65" s="31" t="s">
         <v>41</v>
@@ -5125,14 +5134,14 @@
     </row>
     <row r="66" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="B66" s="27" t="s">
         <v>130</v>
       </c>
       <c r="C66" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>ICTP-RegCM4-7</v>
+        <v>ICTP-RegCM4-6</v>
       </c>
       <c r="D66" s="29" t="s">
         <v>131</v>
@@ -5141,12 +5150,12 @@
         <v>132</v>
       </c>
       <c r="F66" s="30" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G66" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M66" s="10"/>
+      <c r="M66"/>
       <c r="BY66" s="33"/>
       <c r="BZ66" s="33"/>
       <c r="CA66" s="33"/>
@@ -5159,28 +5168,28 @@
       <c r="CH66" s="33"/>
       <c r="CI66" s="33"/>
     </row>
-    <row r="67" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A67" s="35" t="s">
-        <v>114</v>
+        <v>244</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C67" s="27" t="str">
         <f t="shared" si="2"/>
-        <v>CMCC-REMHI</v>
+        <v>ICTP-RegCM4-7</v>
       </c>
       <c r="D67" s="29" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="E67" s="29" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="F67" s="30" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="G67" s="31" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="M67" s="10"/>
       <c r="BY67" s="33"/>
@@ -5195,28 +5204,28 @@
       <c r="CH67" s="33"/>
       <c r="CI67" s="33"/>
     </row>
-    <row r="68" spans="1:87" s="32" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A68" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="B68" s="45" t="s">
-        <v>148</v>
+        <v>114</v>
+      </c>
+      <c r="B68" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="C68" s="27" t="str">
-        <f t="shared" ref="C68:C98" si="3">CONCATENATE(B68,"-",A68)</f>
-        <v>GERICS-AWI-REMO2009</v>
+        <f t="shared" si="2"/>
+        <v>CMCC-REMHI</v>
       </c>
       <c r="D68" s="29" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="F68" s="30" t="s">
-        <v>67</v>
+        <v>273</v>
       </c>
       <c r="G68" s="31" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="M68" s="10"/>
       <c r="BY68" s="33"/>
@@ -5231,30 +5240,30 @@
       <c r="CH68" s="33"/>
       <c r="CI68" s="33"/>
     </row>
-    <row r="69" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:87" s="32" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A69" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="26" t="s">
-        <v>141</v>
+      <c r="B69" s="45" t="s">
+        <v>146</v>
       </c>
       <c r="C69" s="27" t="str">
-        <f t="shared" si="3"/>
-        <v>GERICS-REMO2009</v>
-      </c>
-      <c r="D69" s="28" t="s">
-        <v>142</v>
+        <f t="shared" ref="C69:C99" si="3">CONCATENATE(B69,"-",A69)</f>
+        <v>GERICS-AWI-REMO2009</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>147</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F69" s="30" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="G69" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M69"/>
+      <c r="M69" s="10"/>
       <c r="BY69" s="33"/>
       <c r="BZ69" s="33"/>
       <c r="CA69" s="33"/>
@@ -5267,25 +5276,25 @@
       <c r="CH69" s="33"/>
       <c r="CI69" s="33"/>
     </row>
-    <row r="70" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A70" s="35" t="s">
         <v>140</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C70" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>MPI-CSC-REMO2009</v>
-      </c>
-      <c r="D70" s="28" t="s">
-        <v>146</v>
+        <v>GERICS-REMO2009</v>
+      </c>
+      <c r="D70" s="65" t="s">
+        <v>326</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="F70" s="41" t="s">
-        <v>147</v>
+        <v>142</v>
+      </c>
+      <c r="F70" s="30" t="s">
+        <v>25</v>
       </c>
       <c r="G70" s="31" t="s">
         <v>41</v>
@@ -5303,25 +5312,25 @@
       <c r="CH70" s="33"/>
       <c r="CI70" s="33"/>
     </row>
-    <row r="71" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B71" s="45" t="s">
-        <v>141</v>
+    <row r="71" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>143</v>
       </c>
       <c r="C71" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>GERICS-REMO2015</v>
+        <v>MPI-CSC-REMO2009</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>142</v>
+        <v>326</v>
       </c>
       <c r="E71" s="29" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G71" s="31" t="s">
         <v>41</v>
@@ -5339,25 +5348,25 @@
       <c r="CH71" s="33"/>
       <c r="CI71" s="33"/>
     </row>
-    <row r="72" spans="1:87" s="32" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="B72" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="B72" s="45" t="s">
+        <v>141</v>
       </c>
       <c r="C72" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>GERICS-AWI-ROM1.1</v>
+        <v>GERICS-REMO2015</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>149</v>
+        <v>326</v>
       </c>
       <c r="E72" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="F72" s="30" t="s">
-        <v>67</v>
+      <c r="F72" s="41" t="s">
+        <v>145</v>
       </c>
       <c r="G72" s="31" t="s">
         <v>41</v>
@@ -5375,25 +5384,25 @@
       <c r="CH72" s="33"/>
       <c r="CI72" s="33"/>
     </row>
-    <row r="73" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="B73" s="54" t="s">
-        <v>155</v>
+    <row r="73" spans="1:87" s="32" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="35" t="s">
+        <v>146</v>
       </c>
       <c r="C73" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>MGO-RRCM</v>
+        <v>GERICS-AWI-ROM1.1</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E73" s="29" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F73" s="30" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="G73" s="31" t="s">
         <v>41</v>
@@ -5413,23 +5422,23 @@
     </row>
     <row r="74" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A74" s="34" t="s">
-        <v>278</v>
-      </c>
-      <c r="B74" s="38" t="s">
-        <v>277</v>
+        <v>152</v>
+      </c>
+      <c r="B74" s="54" t="s">
+        <v>153</v>
       </c>
       <c r="C74" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>UNIST-SNURCM</v>
+        <v>MGO-RRCM</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>251</v>
+        <v>154</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>252</v>
+        <v>155</v>
       </c>
       <c r="F74" s="30" t="s">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="G74" s="31" t="s">
         <v>41</v>
@@ -5447,28 +5456,28 @@
       <c r="CH74" s="33"/>
       <c r="CI74" s="33"/>
     </row>
-    <row r="75" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="B75" s="37" t="s">
-        <v>163</v>
+    <row r="75" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>275</v>
       </c>
       <c r="C75" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>IPSL-WRF311</v>
-      </c>
-      <c r="D75" s="29" t="s">
-        <v>164</v>
+        <v>UNIST-SNURCM</v>
+      </c>
+      <c r="D75" s="28" t="s">
+        <v>249</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="F75" s="29" t="s">
-        <v>166</v>
+        <v>250</v>
+      </c>
+      <c r="F75" s="30" t="s">
+        <v>248</v>
       </c>
       <c r="G75" s="31" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="M75"/>
       <c r="BY75" s="33"/>
@@ -5485,28 +5494,28 @@
     </row>
     <row r="76" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="36" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C76" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>IPSL-WRF311NEMO</v>
-      </c>
-      <c r="D76" s="28" t="s">
+        <v>IPSL-WRF311</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F76" s="29" t="s">
         <v>164</v>
-      </c>
-      <c r="E76" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="F76" s="29" t="s">
-        <v>168</v>
       </c>
       <c r="G76" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="M76" s="10"/>
+      <c r="M76"/>
       <c r="BY76" s="33"/>
       <c r="BZ76" s="33"/>
       <c r="CA76" s="33"/>
@@ -5519,30 +5528,30 @@
       <c r="CH76" s="33"/>
       <c r="CI76" s="33"/>
     </row>
-    <row r="77" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="35" t="s">
-        <v>158</v>
-      </c>
-      <c r="B77" s="27" t="s">
-        <v>159</v>
+    <row r="77" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B77" s="37" t="s">
+        <v>161</v>
       </c>
       <c r="C77" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>AUTH-LHTEE-WRF321B</v>
+        <v>IPSL-WRF311NEMO</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="E77" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="F77" s="30" t="s">
-        <v>25</v>
+        <v>162</v>
+      </c>
+      <c r="E77" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="F77" s="29" t="s">
+        <v>166</v>
       </c>
       <c r="G77" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="M77"/>
+        <v>26</v>
+      </c>
+      <c r="M77" s="10"/>
       <c r="BY77" s="33"/>
       <c r="BZ77" s="33"/>
       <c r="CA77" s="33"/>
@@ -5555,25 +5564,25 @@
       <c r="CH77" s="33"/>
       <c r="CI77" s="33"/>
     </row>
-    <row r="78" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="42" t="s">
-        <v>169</v>
-      </c>
-      <c r="B78" s="43" t="s">
-        <v>172</v>
+    <row r="78" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>157</v>
       </c>
       <c r="C78" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>BCCR-WRF331</v>
+        <v>AUTH-LHTEE-WRF321B</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="E78" s="40" t="s">
-        <v>174</v>
+        <v>158</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>159</v>
       </c>
       <c r="F78" s="30" t="s">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="G78" s="31" t="s">
         <v>41</v>
@@ -5592,24 +5601,24 @@
       <c r="CI78" s="33"/>
     </row>
     <row r="79" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="B79" s="26" t="s">
-        <v>133</v>
+      <c r="A79" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B79" s="43" t="s">
+        <v>170</v>
       </c>
       <c r="C79" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>UM-WRF331</v>
+        <v>BCCR-WRF331</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="E79" s="28" t="s">
         <v>171</v>
       </c>
+      <c r="E79" s="40" t="s">
+        <v>172</v>
+      </c>
       <c r="F79" s="30" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="G79" s="31" t="s">
         <v>41</v>
@@ -5627,29 +5636,30 @@
       <c r="CH79" s="33"/>
       <c r="CI79" s="33"/>
     </row>
-    <row r="80" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="B80" s="37" t="s">
-        <v>180</v>
+    <row r="80" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>133</v>
       </c>
       <c r="C80" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>CRP-GL-WRF331A</v>
+        <v>UM-WRF331</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="E80" s="40" t="s">
-        <v>181</v>
+        <v>168</v>
+      </c>
+      <c r="E80" s="28" t="s">
+        <v>169</v>
       </c>
       <c r="F80" s="30" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G80" s="31" t="s">
         <v>41</v>
       </c>
+      <c r="M80"/>
       <c r="BY80" s="33"/>
       <c r="BZ80" s="33"/>
       <c r="CA80" s="33"/>
@@ -5663,24 +5673,24 @@
       <c r="CI80" s="33"/>
     </row>
     <row r="81" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="B81" s="43" t="s">
-        <v>177</v>
+      <c r="A81" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="B81" s="37" t="s">
+        <v>178</v>
       </c>
       <c r="C81" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>MIUB-WRF331A</v>
+        <v>CRP-GL-WRF331A</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E81" s="40" t="s">
         <v>179</v>
       </c>
       <c r="F81" s="30" t="s">
-        <v>102</v>
+        <v>25</v>
       </c>
       <c r="G81" s="31" t="s">
         <v>41</v>
@@ -5699,23 +5709,23 @@
     </row>
     <row r="82" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A82" s="42" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B82" s="43" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C82" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>BCCR-WRF331C</v>
+        <v>MIUB-WRF331A</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E82" s="40" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F82" s="30" t="s">
-        <v>183</v>
+        <v>102</v>
       </c>
       <c r="G82" s="31" t="s">
         <v>41</v>
@@ -5732,25 +5742,25 @@
       <c r="CH82" s="33"/>
       <c r="CI82" s="33"/>
     </row>
-    <row r="83" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A83" s="36" t="s">
-        <v>184</v>
-      </c>
-      <c r="B83" s="37" t="s">
-        <v>185</v>
+    <row r="83" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B83" s="43" t="s">
+        <v>170</v>
       </c>
       <c r="C83" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>IPSL-INERIS-WRF331F</v>
+        <v>BCCR-WRF331C</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="E83" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="F83" s="29" t="s">
-        <v>102</v>
+        <v>171</v>
+      </c>
+      <c r="E83" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F83" s="30" t="s">
+        <v>181</v>
       </c>
       <c r="G83" s="31" t="s">
         <v>41</v>
@@ -5767,25 +5777,25 @@
       <c r="CH83" s="33"/>
       <c r="CI83" s="33"/>
     </row>
-    <row r="84" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A84" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="B84" s="27" t="s">
-        <v>188</v>
+        <v>182</v>
+      </c>
+      <c r="B84" s="37" t="s">
+        <v>183</v>
       </c>
       <c r="C84" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>UCAN-WRF331G</v>
+        <v>IPSL-INERIS-WRF331F</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="F84" s="29" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="G84" s="31" t="s">
         <v>41</v>
@@ -5803,27 +5813,27 @@
       <c r="CI84" s="33"/>
     </row>
     <row r="85" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="B85" s="26" t="s">
-        <v>192</v>
+      <c r="A85" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="B85" s="27" t="s">
+        <v>186</v>
       </c>
       <c r="C85" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>NUIM-WRF341E</v>
+        <v>UCAN-WRF331G</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="F85" s="30" t="s">
-        <v>25</v>
+        <v>188</v>
+      </c>
+      <c r="F85" s="29" t="s">
+        <v>31</v>
       </c>
       <c r="G85" s="31" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="BY85" s="33"/>
       <c r="BZ85" s="33"/>
@@ -5839,26 +5849,26 @@
     </row>
     <row r="86" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A86" s="35" t="s">
-        <v>229</v>
+        <v>189</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C86" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>UCAN-WRF341I</v>
+        <v>NUIM-WRF341E</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E86" s="29" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F86" s="30" t="s">
-        <v>199</v>
+        <v>25</v>
       </c>
       <c r="G86" s="31" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="BY86" s="33"/>
       <c r="BZ86" s="33"/>
@@ -5873,27 +5883,27 @@
       <c r="CI86" s="33"/>
     </row>
     <row r="87" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="B87" s="37" t="s">
-        <v>196</v>
+      <c r="A87" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="B87" s="26" t="s">
+        <v>186</v>
       </c>
       <c r="C87" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>IDL-WRF350D</v>
+        <v>UCAN-WRF341I</v>
       </c>
       <c r="D87" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="F87" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="E87" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="F87" s="30" t="s">
-        <v>25</v>
-      </c>
       <c r="G87" s="31" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="BY87" s="33"/>
       <c r="BZ87" s="33"/>
@@ -5907,28 +5917,28 @@
       <c r="CH87" s="33"/>
       <c r="CI87" s="33"/>
     </row>
-    <row r="88" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A88" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="B88" s="26" t="s">
-        <v>201</v>
+    <row r="88" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B88" s="37" t="s">
+        <v>194</v>
       </c>
       <c r="C88" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>UNSW-WRF360J</v>
+        <v>IDL-WRF350D</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="E88" s="44" t="s">
-        <v>203</v>
+        <v>195</v>
+      </c>
+      <c r="E88" s="29" t="s">
+        <v>196</v>
       </c>
       <c r="F88" s="30" t="s">
-        <v>204</v>
+        <v>25</v>
       </c>
       <c r="G88" s="31" t="s">
-        <v>205</v>
+        <v>26</v>
       </c>
       <c r="BY88" s="33"/>
       <c r="BZ88" s="33"/>
@@ -5944,26 +5954,26 @@
     </row>
     <row r="89" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A89" s="25" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C89" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>UNSW-WRF360K</v>
+        <v>UNSW-WRF360J</v>
       </c>
       <c r="D89" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E89" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="F89" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="E89" s="44" t="s">
+      <c r="G89" s="31" t="s">
         <v>203</v>
-      </c>
-      <c r="F89" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="G89" s="31" t="s">
-        <v>205</v>
       </c>
       <c r="BY89" s="33"/>
       <c r="BZ89" s="33"/>
@@ -5978,27 +5988,27 @@
       <c r="CI89" s="33"/>
     </row>
     <row r="90" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A90" s="35" t="s">
-        <v>207</v>
+      <c r="A90" s="25" t="s">
+        <v>204</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C90" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>UNSW-WRF360L</v>
+        <v>UNSW-WRF360K</v>
       </c>
       <c r="D90" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E90" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="F90" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="E90" s="44" t="s">
+      <c r="G90" s="31" t="s">
         <v>203</v>
-      </c>
-      <c r="F90" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="G90" s="31" t="s">
-        <v>205</v>
       </c>
       <c r="BY90" s="33"/>
       <c r="BZ90" s="33"/>
@@ -6013,27 +6023,27 @@
       <c r="CI90" s="33"/>
     </row>
     <row r="91" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A91" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="B91" s="27" t="s">
-        <v>209</v>
+      <c r="A91" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="B91" s="26" t="s">
+        <v>199</v>
       </c>
       <c r="C91" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>MU-WRF360M</v>
+        <v>UNSW-WRF360L</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="E91" s="29" t="s">
-        <v>211</v>
+        <v>200</v>
+      </c>
+      <c r="E91" s="44" t="s">
+        <v>201</v>
       </c>
       <c r="F91" s="30" t="s">
-        <v>25</v>
+        <v>202</v>
       </c>
       <c r="G91" s="31" t="s">
-        <v>26</v>
+        <v>203</v>
       </c>
       <c r="BY91" s="33"/>
       <c r="BZ91" s="33"/>
@@ -6047,28 +6057,28 @@
       <c r="CH91" s="33"/>
       <c r="CI91" s="33"/>
     </row>
-    <row r="92" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="42" t="s">
-        <v>212</v>
-      </c>
-      <c r="B92" s="43" t="s">
-        <v>172</v>
+    <row r="92" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A92" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="B92" s="27" t="s">
+        <v>207</v>
       </c>
       <c r="C92" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>BCCR-WRF361</v>
+        <v>MU-WRF360M</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="E92" s="40" t="s">
-        <v>174</v>
+        <v>208</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>209</v>
       </c>
       <c r="F92" s="30" t="s">
-        <v>213</v>
+        <v>25</v>
       </c>
       <c r="G92" s="31" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="BY92" s="33"/>
       <c r="BZ92" s="33"/>
@@ -6082,25 +6092,25 @@
       <c r="CH92" s="33"/>
       <c r="CI92" s="33"/>
     </row>
-    <row r="93" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A93" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="B93" s="37" t="s">
-        <v>185</v>
+    <row r="93" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="B93" s="43" t="s">
+        <v>170</v>
       </c>
       <c r="C93" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>IPSL-INERIS-WRF361F</v>
+        <v>BCCR-WRF361</v>
       </c>
       <c r="D93" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="E93" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="F93" s="29" t="s">
-        <v>102</v>
+        <v>171</v>
+      </c>
+      <c r="E93" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F93" s="30" t="s">
+        <v>211</v>
       </c>
       <c r="G93" s="31" t="s">
         <v>41</v>
@@ -6117,28 +6127,28 @@
       <c r="CH93" s="33"/>
       <c r="CI93" s="33"/>
     </row>
-    <row r="94" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="B94" s="27" t="s">
-        <v>216</v>
+    <row r="94" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A94" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="B94" s="37" t="s">
+        <v>183</v>
       </c>
       <c r="C94" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>UHOH-WRF361H</v>
+        <v>IPSL-INERIS-WRF361F</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>217</v>
+        <v>184</v>
       </c>
       <c r="E94" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="F94" s="30" t="s">
-        <v>25</v>
+        <v>163</v>
+      </c>
+      <c r="F94" s="29" t="s">
+        <v>102</v>
       </c>
       <c r="G94" s="31" t="s">
-        <v>219</v>
+        <v>41</v>
       </c>
       <c r="BY94" s="33"/>
       <c r="BZ94" s="33"/>
@@ -6152,28 +6162,28 @@
       <c r="CH94" s="33"/>
       <c r="CI94" s="33"/>
     </row>
-    <row r="95" spans="1:87" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="45" t="s">
-        <v>257</v>
-      </c>
-      <c r="B95" s="26" t="s">
-        <v>258</v>
+    <row r="95" spans="1:87" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A95" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="B95" s="27" t="s">
+        <v>214</v>
       </c>
       <c r="C95" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>PNU-WRF370</v>
+        <v>UHOH-WRF361H</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
       <c r="E95" s="29" t="s">
-        <v>260</v>
+        <v>216</v>
       </c>
       <c r="F95" s="30" t="s">
-        <v>250</v>
-      </c>
-      <c r="G95" s="29" t="s">
-        <v>41</v>
+        <v>25</v>
+      </c>
+      <c r="G95" s="31" t="s">
+        <v>217</v>
       </c>
       <c r="BY95" s="33"/>
       <c r="BZ95" s="33"/>
@@ -6188,24 +6198,24 @@
       <c r="CI95" s="33"/>
     </row>
     <row r="96" spans="1:87" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="B96" s="47" t="s">
-        <v>221</v>
+      <c r="A96" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="B96" s="26" t="s">
+        <v>256</v>
       </c>
       <c r="C96" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>AUTH-MC-WRF371M</v>
-      </c>
-      <c r="D96" s="29" t="s">
-        <v>222</v>
+        <v>PNU-WRF370</v>
+      </c>
+      <c r="D96" s="28" t="s">
+        <v>257</v>
       </c>
       <c r="E96" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="F96" s="49" t="s">
-        <v>31</v>
+        <v>258</v>
+      </c>
+      <c r="F96" s="30" t="s">
+        <v>248</v>
       </c>
       <c r="G96" s="29" t="s">
         <v>41</v>
@@ -6222,25 +6232,25 @@
       <c r="CH96" s="33"/>
       <c r="CI96" s="33"/>
     </row>
-    <row r="97" spans="1:87" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:87" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A97" s="51" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="B97" s="47" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="C97" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>WEGC-WRF371O</v>
+        <v>AUTH-MC-WRF371M</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="E97" s="29" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="F97" s="49" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G97" s="29" t="s">
         <v>41</v>
@@ -6257,28 +6267,28 @@
       <c r="CH97" s="33"/>
       <c r="CI97" s="33"/>
     </row>
-    <row r="98" spans="1:87" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="46" t="s">
-        <v>235</v>
+    <row r="98" spans="1:87" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="51" t="s">
+        <v>237</v>
       </c>
       <c r="B98" s="47" t="s">
-        <v>237</v>
-      </c>
-      <c r="C98" s="47" t="str">
+        <v>238</v>
+      </c>
+      <c r="C98" s="27" t="str">
         <f t="shared" si="3"/>
-        <v>CRC-BGS-WRF381</v>
-      </c>
-      <c r="D98" s="48" t="s">
-        <v>236</v>
-      </c>
-      <c r="E98" s="55" t="s">
-        <v>238</v>
+        <v>WEGC-WRF371O</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>240</v>
       </c>
       <c r="F98" s="49" t="s">
-        <v>274</v>
-      </c>
-      <c r="G98" s="50" t="s">
-        <v>219</v>
+        <v>39</v>
+      </c>
+      <c r="G98" s="29" t="s">
+        <v>41</v>
       </c>
       <c r="BY98" s="33"/>
       <c r="BZ98" s="33"/>
@@ -6292,7 +6302,29 @@
       <c r="CH98" s="33"/>
       <c r="CI98" s="33"/>
     </row>
-    <row r="99" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:87" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="B99" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="C99" s="47" t="str">
+        <f t="shared" si="3"/>
+        <v>CRC-BGS-WRF381</v>
+      </c>
+      <c r="D99" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="E99" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="F99" s="49" t="s">
+        <v>272</v>
+      </c>
+      <c r="G99" s="50" t="s">
+        <v>217</v>
+      </c>
       <c r="BY99" s="33"/>
       <c r="BZ99" s="33"/>
       <c r="CA99" s="33"/>
@@ -6305,178 +6337,192 @@
       <c r="CH99" s="33"/>
       <c r="CI99" s="33"/>
     </row>
+    <row r="100" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="BY100" s="33"/>
+      <c r="BZ100" s="33"/>
+      <c r="CA100" s="33"/>
+      <c r="CB100" s="33"/>
+      <c r="CC100" s="33"/>
+      <c r="CD100" s="33"/>
+      <c r="CE100" s="33"/>
+      <c r="CF100" s="33"/>
+      <c r="CG100" s="33"/>
+      <c r="CH100" s="33"/>
+      <c r="CI100" s="33"/>
+    </row>
   </sheetData>
   <sortState ref="A2:G96">
     <sortCondition ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="G62 B37:B41 F68:F71 A72:C73">
+  <conditionalFormatting sqref="G63 B38:B42 F69:F72 A73:C74">
     <cfRule type="containsText" dxfId="47" priority="23" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F61:F65">
+  <conditionalFormatting sqref="F62:F66">
     <cfRule type="containsText" dxfId="46" priority="24" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A90">
+  <conditionalFormatting sqref="A91">
     <cfRule type="containsText" dxfId="45" priority="30" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
+  <conditionalFormatting sqref="A92">
     <cfRule type="containsText" dxfId="44" priority="31" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A92">
+  <conditionalFormatting sqref="A93">
     <cfRule type="containsText" dxfId="43" priority="32" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74:E75">
+  <conditionalFormatting sqref="E75:E76">
     <cfRule type="containsText" dxfId="42" priority="33" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61">
+  <conditionalFormatting sqref="E62">
     <cfRule type="containsText" dxfId="41" priority="34" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E88">
+  <conditionalFormatting sqref="E89">
     <cfRule type="containsText" dxfId="40" priority="35" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G74:G75">
+  <conditionalFormatting sqref="G75:G76">
     <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36:C36">
+  <conditionalFormatting sqref="B37:C37">
     <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
+  <conditionalFormatting sqref="C40">
     <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16:E21 E36:E39">
+  <conditionalFormatting sqref="E17:E22 E37:E40">
     <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
     <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E81">
+  <conditionalFormatting sqref="E82">
     <cfRule type="containsText" dxfId="34" priority="43" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
+  <conditionalFormatting sqref="E83">
     <cfRule type="containsText" dxfId="33" priority="44" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64:E65">
+  <conditionalFormatting sqref="E65:E66">
     <cfRule type="containsText" dxfId="32" priority="47" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="E70">
     <cfRule type="containsText" dxfId="31" priority="50" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G69">
+  <conditionalFormatting sqref="G70">
     <cfRule type="containsText" dxfId="30" priority="51" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G88">
+  <conditionalFormatting sqref="G89">
     <cfRule type="containsText" dxfId="29" priority="54" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G81">
+  <conditionalFormatting sqref="G82">
     <cfRule type="containsText" dxfId="28" priority="55" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G79">
+  <conditionalFormatting sqref="G80">
     <cfRule type="containsText" dxfId="27" priority="57" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58:E59">
+  <conditionalFormatting sqref="E59:E60">
     <cfRule type="containsText" dxfId="26" priority="58" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C16">
     <cfRule type="containsText" dxfId="25" priority="62" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15">
+  <conditionalFormatting sqref="F16">
     <cfRule type="containsText" dxfId="24" priority="63" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="E16">
     <cfRule type="containsText" dxfId="23" priority="64" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
+  <conditionalFormatting sqref="G16">
     <cfRule type="containsText" dxfId="22" priority="65" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E72">
+  <conditionalFormatting sqref="E73">
     <cfRule type="containsText" dxfId="21" priority="66" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F72">
+  <conditionalFormatting sqref="F73">
     <cfRule type="containsText" dxfId="20" priority="67" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G61">
+  <conditionalFormatting sqref="G62">
     <cfRule type="containsText" dxfId="19" priority="68" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G76">
+  <conditionalFormatting sqref="G77">
     <cfRule type="containsText" dxfId="18" priority="69" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
+  <conditionalFormatting sqref="G99">
     <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F66">
+  <conditionalFormatting sqref="F67">
     <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
+  <conditionalFormatting sqref="D22">
     <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67">
+  <conditionalFormatting sqref="F68">
     <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
+  <conditionalFormatting sqref="E36">
     <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E31 E34">
+  <conditionalFormatting sqref="E23:E32 E35">
     <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D31">
+  <conditionalFormatting sqref="D23:D32">
     <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D35">
     <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+  <conditionalFormatting sqref="D36">
     <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D37">
     <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D38">
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
+  <conditionalFormatting sqref="D39">
     <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
+  <conditionalFormatting sqref="D40">
     <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D43">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E33">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
+  <conditionalFormatting sqref="E34">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D34">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="unrestricted"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1"/>
-    <hyperlink ref="D25" r:id="rId2"/>
-    <hyperlink ref="D67" r:id="rId3"/>
-    <hyperlink ref="D64" r:id="rId4"/>
-    <hyperlink ref="D75" r:id="rId5"/>
-    <hyperlink ref="D76" r:id="rId6"/>
-    <hyperlink ref="D98" r:id="rId7" display="mailto:julien.pergaud@u-bourgogne.fr"/>
-    <hyperlink ref="D51" r:id="rId8" display="grigory.nikulin@smhi.se_x000a_Grigory"/>
-    <hyperlink ref="D44" r:id="rId9"/>
-    <hyperlink ref="D41" r:id="rId10"/>
-    <hyperlink ref="D43" r:id="rId11"/>
-    <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D30" r:id="rId13"/>
-    <hyperlink ref="D23" r:id="rId14" display="merja.toelle@geogr.uni-giessen.de"/>
+    <hyperlink ref="D26" r:id="rId2"/>
+    <hyperlink ref="D68" r:id="rId3"/>
+    <hyperlink ref="D65" r:id="rId4"/>
+    <hyperlink ref="D76" r:id="rId5"/>
+    <hyperlink ref="D77" r:id="rId6"/>
+    <hyperlink ref="D99" r:id="rId7" display="mailto:julien.pergaud@u-bourgogne.fr"/>
+    <hyperlink ref="D52" r:id="rId8" display="grigory.nikulin@smhi.se_x000a_Grigory"/>
+    <hyperlink ref="D45" r:id="rId9"/>
+    <hyperlink ref="D42" r:id="rId10"/>
+    <hyperlink ref="D44" r:id="rId11"/>
+    <hyperlink ref="D23" r:id="rId12"/>
+    <hyperlink ref="D31" r:id="rId13"/>
+    <hyperlink ref="D24" r:id="rId14" display="merja.toelle@geogr.uni-giessen.de"/>
     <hyperlink ref="D6" r:id="rId15" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
     <hyperlink ref="D7" r:id="rId16" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
     <hyperlink ref="D10" r:id="rId17" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
     <hyperlink ref="D11" r:id="rId18" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
-    <hyperlink ref="D55" r:id="rId19" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
-    <hyperlink ref="D56" r:id="rId20" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
+    <hyperlink ref="D56" r:id="rId19" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
+    <hyperlink ref="D57" r:id="rId20" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
     <hyperlink ref="D8" r:id="rId21" display="http://cadillac/sympa/info/contact.aladin-cordex"/>
+    <hyperlink ref="D14" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" scale="65" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" scale="65" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correction to recent CCAM entry
</commit_message>
<xml_diff>
--- a/CORDEX_register.xlsx
+++ b/CORDEX_register.xlsx
@@ -1050,13 +1050,13 @@
     <t>RegCM4-4</t>
   </si>
   <si>
-    <t>CCAM-795</t>
-  </si>
-  <si>
     <t>Marcus.Thatcher@csiro.au</t>
   </si>
   <si>
     <t>"AUS-44 ANT-44"</t>
+  </si>
+  <si>
+    <t>CCAM-2008</t>
   </si>
 </sst>
 </file>
@@ -1601,10 +1601,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1615,18 +1627,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2507,28 +2507,28 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.75"/>
-    <col min="2" max="15" width="13.75"/>
-    <col min="16" max="1025" width="8.875"/>
+    <col min="1" max="1" width="20.7109375"/>
+    <col min="2" max="15" width="13.7109375"/>
+    <col min="16" max="1025" width="8.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -2554,20 +2554,20 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2590,127 +2590,127 @@
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
     </row>
     <row r="13" spans="1:15" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
@@ -2725,32 +2725,32 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B7:J7"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="B11:J11"/>
     <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B7:J7"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -2764,54 +2764,54 @@
   </sheetPr>
   <dimension ref="A1:CI102"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A76" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="13.875"/>
-    <col min="3" max="3" width="31.75" customWidth="1"/>
-    <col min="4" max="5" width="22.875"/>
-    <col min="6" max="6" width="23.375"/>
-    <col min="7" max="7" width="15.375"/>
-    <col min="8" max="8" width="13.75"/>
+    <col min="1" max="1" width="22.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="5" width="22.85546875"/>
+    <col min="6" max="6" width="23.42578125"/>
+    <col min="7" max="7" width="15.42578125"/>
+    <col min="8" max="8" width="13.7109375"/>
     <col min="9" max="14" width="21"/>
-    <col min="15" max="15" width="14.625"/>
-    <col min="16" max="16" width="13.875"/>
-    <col min="17" max="17" width="20.625"/>
+    <col min="15" max="15" width="14.5703125"/>
+    <col min="16" max="16" width="13.85546875"/>
+    <col min="17" max="17" width="20.5703125"/>
     <col min="18" max="18" width="17"/>
-    <col min="19" max="19" width="14.375"/>
-    <col min="20" max="20" width="14.625"/>
+    <col min="19" max="19" width="14.42578125"/>
+    <col min="20" max="20" width="14.5703125"/>
     <col min="21" max="21" width="16"/>
-    <col min="22" max="22" width="17.375"/>
-    <col min="23" max="24" width="17.625"/>
-    <col min="25" max="25" width="12.125"/>
-    <col min="26" max="26" width="15.375"/>
-    <col min="27" max="27" width="12.625"/>
-    <col min="28" max="28" width="15.75"/>
-    <col min="29" max="29" width="15.375"/>
+    <col min="22" max="22" width="17.42578125"/>
+    <col min="23" max="24" width="17.5703125"/>
+    <col min="25" max="25" width="12.140625"/>
+    <col min="26" max="26" width="15.42578125"/>
+    <col min="27" max="27" width="12.5703125"/>
+    <col min="28" max="28" width="15.7109375"/>
+    <col min="29" max="29" width="15.42578125"/>
     <col min="30" max="30" width="16"/>
-    <col min="31" max="31" width="17.125"/>
+    <col min="31" max="31" width="17.140625"/>
     <col min="32" max="32" width="16"/>
     <col min="33" max="33" width="17"/>
-    <col min="34" max="36" width="20.625"/>
-    <col min="37" max="37" width="10.75"/>
-    <col min="38" max="38" width="23.625"/>
-    <col min="39" max="39" width="12.375"/>
-    <col min="40" max="40" width="15.625"/>
-    <col min="41" max="41" width="18.375"/>
-    <col min="42" max="42" width="20.25"/>
+    <col min="34" max="36" width="20.5703125"/>
+    <col min="37" max="37" width="10.7109375"/>
+    <col min="38" max="38" width="23.5703125"/>
+    <col min="39" max="39" width="12.42578125"/>
+    <col min="40" max="40" width="15.5703125"/>
+    <col min="41" max="41" width="18.42578125"/>
+    <col min="42" max="42" width="20.28515625"/>
     <col min="43" max="43" width="16"/>
-    <col min="44" max="44" width="13.75"/>
-    <col min="45" max="45" width="22.625"/>
-    <col min="46" max="46" width="16.125"/>
-    <col min="47" max="48" width="15.625"/>
-    <col min="49" max="49" width="16.125"/>
-    <col min="50" max="76" width="8.875"/>
-    <col min="77" max="87" width="8.875" style="17"/>
-    <col min="88" max="1025" width="8.875"/>
+    <col min="44" max="44" width="13.7109375"/>
+    <col min="45" max="45" width="22.5703125"/>
+    <col min="46" max="46" width="16.140625"/>
+    <col min="47" max="48" width="15.5703125"/>
+    <col min="49" max="49" width="16.140625"/>
+    <col min="50" max="76" width="8.85546875"/>
+    <col min="77" max="87" width="8.85546875" style="17"/>
+    <col min="88" max="1025" width="8.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:87" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
       <c r="CH2" s="24"/>
       <c r="CI2" s="24"/>
     </row>
-    <row r="3" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>27</v>
       </c>
@@ -3039,7 +3039,7 @@
       <c r="CH5" s="33"/>
       <c r="CI5" s="33"/>
     </row>
-    <row r="6" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>21</v>
       </c>
@@ -3074,7 +3074,7 @@
       <c r="CH6" s="33"/>
       <c r="CI6" s="33"/>
     </row>
-    <row r="7" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>316</v>
       </c>
@@ -3109,7 +3109,7 @@
       <c r="CH7" s="33"/>
       <c r="CI7" s="33"/>
     </row>
-    <row r="8" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>321</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="CH8" s="33"/>
       <c r="CI8" s="33"/>
     </row>
-    <row r="9" spans="1:87" s="17" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:87" s="17" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>35</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>318</v>
       </c>
@@ -3203,7 +3203,7 @@
       <c r="CH10" s="33"/>
       <c r="CI10" s="33"/>
     </row>
-    <row r="11" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>40</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="CH12" s="33"/>
       <c r="CI12" s="33"/>
     </row>
-    <row r="13" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>46</v>
       </c>
@@ -3308,7 +3308,7 @@
       <c r="CH13" s="33"/>
       <c r="CI13" s="33"/>
     </row>
-    <row r="14" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
         <v>325</v>
       </c>
@@ -3344,25 +3344,25 @@
       <c r="CH14" s="33"/>
       <c r="CI14" s="33"/>
     </row>
-    <row r="15" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="66" t="s">
-        <v>328</v>
+    <row r="15" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="58" t="s">
+        <v>330</v>
       </c>
       <c r="B15" s="56" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="56" t="str">
         <f>CONCATENATE(B15,"-",A15)</f>
-        <v>CSIRO-CCAM-795</v>
+        <v>CSIRO-CCAM-2008</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>49</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G15" s="29" t="s">
         <v>41</v>
@@ -3848,7 +3848,7 @@
       <c r="CH28" s="33"/>
       <c r="CI28" s="33"/>
     </row>
-    <row r="29" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>260</v>
       </c>
@@ -4172,7 +4172,7 @@
       <c r="CH37" s="33"/>
       <c r="CI37" s="33"/>
     </row>
-    <row r="38" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
         <v>59</v>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="CH38" s="33"/>
       <c r="CI38" s="33"/>
     </row>
-    <row r="39" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A39" s="35" t="s">
         <v>66</v>
       </c>
@@ -4244,7 +4244,7 @@
       <c r="CH39" s="33"/>
       <c r="CI39" s="33"/>
     </row>
-    <row r="40" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>68</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="CH40" s="33"/>
       <c r="CI40" s="33"/>
     </row>
-    <row r="41" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>73</v>
       </c>
@@ -4604,7 +4604,7 @@
       <c r="CH49" s="33"/>
       <c r="CI49" s="33"/>
     </row>
-    <row r="50" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
         <v>96</v>
       </c>
@@ -4640,7 +4640,7 @@
       <c r="CH50" s="33"/>
       <c r="CI50" s="33"/>
     </row>
-    <row r="51" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A51" s="36" t="s">
         <v>101</v>
       </c>
@@ -4676,7 +4676,7 @@
       <c r="CH51" s="33"/>
       <c r="CI51" s="33"/>
     </row>
-    <row r="52" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A52" s="36" t="s">
         <v>103</v>
       </c>
@@ -4856,7 +4856,7 @@
       <c r="CH56" s="33"/>
       <c r="CI56" s="33"/>
     </row>
-    <row r="57" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A57" s="35" t="s">
         <v>112</v>
       </c>
@@ -4892,7 +4892,7 @@
       <c r="CH57" s="33"/>
       <c r="CI57" s="33"/>
     </row>
-    <row r="58" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
         <v>317</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="CH70" s="33"/>
       <c r="CI70" s="33"/>
     </row>
-    <row r="71" spans="1:87" s="32" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:87" s="32" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
         <v>140</v>
       </c>
@@ -5396,7 +5396,7 @@
       <c r="CH71" s="33"/>
       <c r="CI71" s="33"/>
     </row>
-    <row r="72" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A72" s="35" t="s">
         <v>140</v>
       </c>
@@ -5432,7 +5432,7 @@
       <c r="CH72" s="33"/>
       <c r="CI72" s="33"/>
     </row>
-    <row r="73" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="35" t="s">
         <v>140</v>
       </c>
@@ -5468,7 +5468,7 @@
       <c r="CH73" s="33"/>
       <c r="CI73" s="33"/>
     </row>
-    <row r="74" spans="1:87" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>149</v>
       </c>
@@ -5504,7 +5504,7 @@
       <c r="CH74" s="33"/>
       <c r="CI74" s="33"/>
     </row>
-    <row r="75" spans="1:87" s="32" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:87" s="32" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>151</v>
       </c>
@@ -5576,7 +5576,7 @@
       <c r="CH76" s="33"/>
       <c r="CI76" s="33"/>
     </row>
-    <row r="77" spans="1:87" s="32" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A77" s="34" t="s">
         <v>276</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="CH79" s="33"/>
       <c r="CI79" s="33"/>
     </row>
-    <row r="80" spans="1:87" s="32" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:87" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="35" t="s">
         <v>156</v>
       </c>
@@ -6317,7 +6317,7 @@
       <c r="CH97" s="33"/>
       <c r="CI97" s="33"/>
     </row>
-    <row r="98" spans="1:87" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:87" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="45" t="s">
         <v>255</v>
       </c>
@@ -6387,7 +6387,7 @@
       <c r="CH99" s="33"/>
       <c r="CI99" s="33"/>
     </row>
-    <row r="100" spans="1:87" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:87" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A100" s="51" t="s">
         <v>237</v>
       </c>

</xml_diff>